<commit_message>
fix spp in #66 + add test to check
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="813">
   <si>
     <t xml:space="preserve">species_order</t>
   </si>
@@ -812,6 +812,9 @@
   </si>
   <si>
     <t xml:space="preserve">Not threatened; Marine; Not migratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1_2_3_5_6</t>
   </si>
   <si>
     <t xml:space="preserve">Stercorarius longicaudus</t>
@@ -2554,23 +2557,22 @@
   </sheetPr>
   <dimension ref="A1:K385"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A265" colorId="64" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A276" activeCellId="0" sqref="A276"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A357" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D379" activeCellId="0" sqref="D379"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.984693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5969387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6275510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.219387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7142857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="91.7397959183674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.6734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="14.9387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6647,7 +6649,7 @@
         <v>20</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H117" s="0" t="s">
         <v>16</v>
@@ -6667,16 +6669,16 @@
         <v>394</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F118" s="0" t="s">
         <v>20</v>
@@ -6688,7 +6690,7 @@
         <v>1700</v>
       </c>
       <c r="K118" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6696,10 +6698,10 @@
         <v>395</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>13</v>
@@ -6723,7 +6725,7 @@
         <v>2005</v>
       </c>
       <c r="K119" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6731,16 +6733,16 @@
         <v>396</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D120" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F120" s="0" t="s">
         <v>20</v>
@@ -6758,7 +6760,7 @@
         <v>2005</v>
       </c>
       <c r="K120" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6766,16 +6768,16 @@
         <v>400</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F121" s="0" t="s">
         <v>20</v>
@@ -6793,7 +6795,7 @@
         <v>2005</v>
       </c>
       <c r="K121" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6801,10 +6803,10 @@
         <v>404</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>13</v>
@@ -6828,7 +6830,7 @@
         <v>2005</v>
       </c>
       <c r="K122" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6836,10 +6838,10 @@
         <v>411</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D123" s="0" t="s">
         <v>13</v>
@@ -6871,10 +6873,10 @@
         <v>416</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C124" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D124" s="0" t="s">
         <v>13</v>
@@ -6906,10 +6908,10 @@
         <v>417</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D125" s="0" t="s">
         <v>13</v>
@@ -6941,10 +6943,10 @@
         <v>423</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D126" s="0" t="s">
         <v>13</v>
@@ -6976,10 +6978,10 @@
         <v>428</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D127" s="0" t="s">
         <v>13</v>
@@ -7003,7 +7005,7 @@
         <v>2005</v>
       </c>
       <c r="K127" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7011,16 +7013,16 @@
         <v>431</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D128" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E128" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F128" s="0" t="s">
         <v>20</v>
@@ -7038,7 +7040,7 @@
         <v>2005</v>
       </c>
       <c r="K128" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7046,10 +7048,10 @@
         <v>434</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D129" s="0" t="s">
         <v>13</v>
@@ -7081,16 +7083,16 @@
         <v>442</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D130" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E130" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F130" s="0" t="s">
         <v>20</v>
@@ -7116,16 +7118,16 @@
         <v>443</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D131" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E131" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F131" s="0" t="s">
         <v>20</v>
@@ -7151,10 +7153,10 @@
         <v>444</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D132" s="0" t="s">
         <v>13</v>
@@ -7186,10 +7188,10 @@
         <v>446</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D133" s="0" t="s">
         <v>13</v>
@@ -7221,10 +7223,10 @@
         <v>456</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D134" s="0" t="s">
         <v>13</v>
@@ -7256,10 +7258,10 @@
         <v>463</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D135" s="0" t="s">
         <v>13</v>
@@ -7291,16 +7293,16 @@
         <v>465</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D136" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E136" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F136" s="0" t="s">
         <v>20</v>
@@ -7318,7 +7320,7 @@
         <v>2005</v>
       </c>
       <c r="K136" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7326,16 +7328,16 @@
         <v>493</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E137" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F137" s="0" t="s">
         <v>20</v>
@@ -7347,7 +7349,7 @@
         <v>1700</v>
       </c>
       <c r="K137" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7355,10 +7357,10 @@
         <v>497</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D138" s="0" t="s">
         <v>13</v>
@@ -7376,7 +7378,7 @@
         <v>1700</v>
       </c>
       <c r="K138" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7384,10 +7386,10 @@
         <v>501</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D139" s="0" t="s">
         <v>13</v>
@@ -7405,7 +7407,7 @@
         <v>1700</v>
       </c>
       <c r="K139" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7413,22 +7415,22 @@
         <v>517</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D140" s="0" t="s">
         <v>179</v>
       </c>
       <c r="E140" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="F140" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G140" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H140" s="0" t="s">
         <v>16</v>
@@ -7440,7 +7442,7 @@
         <v>1700</v>
       </c>
       <c r="K140" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7448,16 +7450,16 @@
         <v>519</v>
       </c>
       <c r="B141" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E141" s="0" t="s">
         <v>315</v>
-      </c>
-      <c r="C141" s="0" t="s">
-        <v>316</v>
-      </c>
-      <c r="D141" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E141" s="0" t="s">
-        <v>314</v>
       </c>
       <c r="F141" s="0" t="s">
         <v>20</v>
@@ -7469,7 +7471,7 @@
         <v>1700</v>
       </c>
       <c r="K141" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7477,16 +7479,16 @@
         <v>534</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D142" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E142" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F142" s="0" t="s">
         <v>179</v>
@@ -7498,7 +7500,7 @@
         <v>1700</v>
       </c>
       <c r="K142" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7506,10 +7508,10 @@
         <v>535</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="D143" s="0" t="s">
         <v>13</v>
@@ -7527,7 +7529,7 @@
         <v>1700</v>
       </c>
       <c r="K143" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7535,10 +7537,10 @@
         <v>537</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D144" s="0" t="s">
         <v>13</v>
@@ -7556,7 +7558,7 @@
         <v>1700</v>
       </c>
       <c r="K144" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7564,10 +7566,10 @@
         <v>547</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D145" s="0" t="s">
         <v>13</v>
@@ -7585,7 +7587,7 @@
         <v>1700</v>
       </c>
       <c r="K145" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7593,10 +7595,10 @@
         <v>548</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D146" s="0" t="s">
         <v>13</v>
@@ -7614,7 +7616,7 @@
         <v>1700</v>
       </c>
       <c r="K146" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7622,16 +7624,16 @@
         <v>555</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D147" s="0" t="s">
         <v>114</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F147" s="0" t="s">
         <v>20</v>
@@ -7649,7 +7651,7 @@
         <v>2005</v>
       </c>
       <c r="K147" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7657,10 +7659,10 @@
         <v>563</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D148" s="0" t="s">
         <v>114</v>
@@ -7678,7 +7680,7 @@
         <v>1700</v>
       </c>
       <c r="K148" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7686,16 +7688,16 @@
         <v>564</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C149" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D149" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E149" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="F149" s="0" t="s">
         <v>20</v>
@@ -7707,7 +7709,7 @@
         <v>1700</v>
       </c>
       <c r="K149" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7715,16 +7717,16 @@
         <v>582</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C150" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D150" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E150" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F150" s="0" t="s">
         <v>114</v>
@@ -7742,7 +7744,7 @@
         <v>2005</v>
       </c>
       <c r="K150" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7750,10 +7752,10 @@
         <v>584</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C151" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="D151" s="0" t="s">
         <v>13</v>
@@ -7777,7 +7779,7 @@
         <v>2005</v>
       </c>
       <c r="K151" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7785,16 +7787,16 @@
         <v>587</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D152" s="0" t="s">
         <v>153</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F152" s="0" t="s">
         <v>20</v>
@@ -7806,7 +7808,7 @@
         <v>1700</v>
       </c>
       <c r="K152" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7814,10 +7816,10 @@
         <v>589</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D153" s="0" t="s">
         <v>153</v>
@@ -7835,7 +7837,7 @@
         <v>1700</v>
       </c>
       <c r="K153" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7843,10 +7845,10 @@
         <v>590</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D154" s="0" t="s">
         <v>13</v>
@@ -7858,7 +7860,7 @@
         <v>20</v>
       </c>
       <c r="G154" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H154" s="0" t="s">
         <v>16</v>
@@ -7870,7 +7872,7 @@
         <v>1700</v>
       </c>
       <c r="K154" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7878,10 +7880,10 @@
         <v>591</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D155" s="0" t="s">
         <v>179</v>
@@ -7905,7 +7907,7 @@
         <v>1700</v>
       </c>
       <c r="K155" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7913,10 +7915,10 @@
         <v>611</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D156" s="0" t="s">
         <v>153</v>
@@ -7948,10 +7950,10 @@
         <v>613</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D157" s="0" t="s">
         <v>13</v>
@@ -7983,10 +7985,10 @@
         <v>615</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D158" s="0" t="s">
         <v>13</v>
@@ -8018,10 +8020,10 @@
         <v>619</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D159" s="0" t="s">
         <v>13</v>
@@ -8053,10 +8055,10 @@
         <v>627</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D160" s="0" t="s">
         <v>13</v>
@@ -8088,10 +8090,10 @@
         <v>629</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D161" s="0" t="s">
         <v>13</v>
@@ -8123,10 +8125,10 @@
         <v>636</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D162" s="0" t="s">
         <v>13</v>
@@ -8158,10 +8160,10 @@
         <v>640</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D163" s="0" t="s">
         <v>13</v>
@@ -8193,10 +8195,10 @@
         <v>645</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D164" s="0" t="s">
         <v>13</v>
@@ -8228,10 +8230,10 @@
         <v>647</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C165" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D165" s="0" t="s">
         <v>13</v>
@@ -8263,10 +8265,10 @@
         <v>650</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C166" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="D166" s="0" t="s">
         <v>13</v>
@@ -8298,10 +8300,10 @@
         <v>651</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D167" s="0" t="s">
         <v>13</v>
@@ -8333,10 +8335,10 @@
         <v>656</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D168" s="0" t="s">
         <v>13</v>
@@ -8368,10 +8370,10 @@
         <v>658</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D169" s="0" t="s">
         <v>13</v>
@@ -8403,10 +8405,10 @@
         <v>659</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D170" s="0" t="s">
         <v>13</v>
@@ -8438,10 +8440,10 @@
         <v>660</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="D171" s="0" t="s">
         <v>13</v>
@@ -8473,10 +8475,10 @@
         <v>661</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D172" s="0" t="s">
         <v>13</v>
@@ -8508,10 +8510,10 @@
         <v>662</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D173" s="0" t="s">
         <v>13</v>
@@ -8543,10 +8545,10 @@
         <v>663</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="D174" s="0" t="s">
         <v>13</v>
@@ -8570,7 +8572,7 @@
         <v>2005</v>
       </c>
       <c r="K174" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8578,10 +8580,10 @@
         <v>669</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D175" s="0" t="s">
         <v>13</v>
@@ -8605,7 +8607,7 @@
         <v>2005</v>
       </c>
       <c r="K175" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8613,16 +8615,16 @@
         <v>670</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D176" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E176" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F176" s="0" t="s">
         <v>20</v>
@@ -8640,7 +8642,7 @@
         <v>2005</v>
       </c>
       <c r="K176" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8648,10 +8650,10 @@
         <v>672</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>13</v>
@@ -8663,7 +8665,7 @@
         <v>20</v>
       </c>
       <c r="G177" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H177" s="0" t="s">
         <v>16</v>
@@ -8675,7 +8677,7 @@
         <v>1700</v>
       </c>
       <c r="K177" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8683,16 +8685,16 @@
         <v>674</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="D178" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E178" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F178" s="0" t="s">
         <v>20</v>
@@ -8710,7 +8712,7 @@
         <v>2005</v>
       </c>
       <c r="K178" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8718,10 +8720,10 @@
         <v>677</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D179" s="0" t="s">
         <v>13</v>
@@ -8753,10 +8755,10 @@
         <v>682</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="D180" s="0" t="s">
         <v>13</v>
@@ -8788,10 +8790,10 @@
         <v>684</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D181" s="0" t="s">
         <v>13</v>
@@ -8823,10 +8825,10 @@
         <v>686</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D182" s="0" t="s">
         <v>13</v>
@@ -8858,10 +8860,10 @@
         <v>688</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D183" s="0" t="s">
         <v>13</v>
@@ -8893,10 +8895,10 @@
         <v>690</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D184" s="0" t="s">
         <v>13</v>
@@ -8928,10 +8930,10 @@
         <v>693</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="D185" s="0" t="s">
         <v>13</v>
@@ -8963,10 +8965,10 @@
         <v>697</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="D186" s="0" t="s">
         <v>13</v>
@@ -8998,10 +9000,10 @@
         <v>698</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D187" s="0" t="s">
         <v>13</v>
@@ -9033,10 +9035,10 @@
         <v>699</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="D188" s="0" t="s">
         <v>13</v>
@@ -9068,10 +9070,10 @@
         <v>702</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D189" s="0" t="s">
         <v>13</v>
@@ -9103,10 +9105,10 @@
         <v>705</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="D190" s="0" t="s">
         <v>13</v>
@@ -9138,10 +9140,10 @@
         <v>706</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="D191" s="0" t="s">
         <v>13</v>
@@ -9173,10 +9175,10 @@
         <v>707</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D192" s="0" t="s">
         <v>13</v>
@@ -9208,10 +9210,10 @@
         <v>708</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D193" s="0" t="s">
         <v>13</v>
@@ -9243,10 +9245,10 @@
         <v>710</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="D194" s="0" t="s">
         <v>13</v>
@@ -9278,10 +9280,10 @@
         <v>717</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C195" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D195" s="0" t="s">
         <v>13</v>
@@ -9313,10 +9315,10 @@
         <v>720</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C196" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="D196" s="0" t="s">
         <v>13</v>
@@ -9348,10 +9350,10 @@
         <v>721</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C197" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="D197" s="0" t="s">
         <v>13</v>
@@ -9383,10 +9385,10 @@
         <v>722</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C198" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D198" s="0" t="s">
         <v>13</v>
@@ -9418,10 +9420,10 @@
         <v>724</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C199" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D199" s="0" t="s">
         <v>13</v>
@@ -9453,10 +9455,10 @@
         <v>726</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C200" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D200" s="0" t="s">
         <v>13</v>
@@ -9488,10 +9490,10 @@
         <v>728</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C201" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D201" s="0" t="s">
         <v>13</v>
@@ -9523,10 +9525,10 @@
         <v>730</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C202" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D202" s="0" t="s">
         <v>13</v>
@@ -9558,10 +9560,10 @@
         <v>735</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C203" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D203" s="0" t="s">
         <v>13</v>
@@ -9593,10 +9595,10 @@
         <v>741</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C204" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D204" s="0" t="s">
         <v>13</v>
@@ -9628,10 +9630,10 @@
         <v>742</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C205" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D205" s="0" t="s">
         <v>13</v>
@@ -9663,10 +9665,10 @@
         <v>746</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C206" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D206" s="0" t="s">
         <v>13</v>
@@ -9698,10 +9700,10 @@
         <v>764</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C207" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D207" s="0" t="s">
         <v>13</v>
@@ -9733,10 +9735,10 @@
         <v>765</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C208" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D208" s="0" t="s">
         <v>13</v>
@@ -9768,10 +9770,10 @@
         <v>773</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C209" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D209" s="0" t="s">
         <v>13</v>
@@ -9803,10 +9805,10 @@
         <v>782</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C210" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="D210" s="0" t="s">
         <v>13</v>
@@ -9838,10 +9840,10 @@
         <v>785</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C211" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D211" s="0" t="s">
         <v>13</v>
@@ -9873,10 +9875,10 @@
         <v>789</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C212" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D212" s="0" t="s">
         <v>13</v>
@@ -9908,10 +9910,10 @@
         <v>793</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C213" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D213" s="0" t="s">
         <v>13</v>
@@ -9943,10 +9945,10 @@
         <v>797</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D214" s="0" t="s">
         <v>13</v>
@@ -9978,10 +9980,10 @@
         <v>800</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D215" s="0" t="s">
         <v>13</v>
@@ -9993,7 +9995,7 @@
         <v>20</v>
       </c>
       <c r="G215" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H215" s="0" t="s">
         <v>16</v>
@@ -10013,10 +10015,10 @@
         <v>803</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="D216" s="0" t="s">
         <v>13</v>
@@ -10048,10 +10050,10 @@
         <v>807</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D217" s="0" t="s">
         <v>13</v>
@@ -10083,10 +10085,10 @@
         <v>810</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D218" s="0" t="s">
         <v>13</v>
@@ -10118,10 +10120,10 @@
         <v>813</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D219" s="0" t="s">
         <v>13</v>
@@ -10153,10 +10155,10 @@
         <v>814</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="D220" s="0" t="s">
         <v>13</v>
@@ -10188,10 +10190,10 @@
         <v>818</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D221" s="0" t="s">
         <v>13</v>
@@ -10223,10 +10225,10 @@
         <v>819</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D222" s="0" t="s">
         <v>13</v>
@@ -10258,10 +10260,10 @@
         <v>825</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C223" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D223" s="0" t="s">
         <v>13</v>
@@ -10293,10 +10295,10 @@
         <v>829</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C224" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D224" s="0" t="s">
         <v>13</v>
@@ -10328,10 +10330,10 @@
         <v>838</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C225" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D225" s="0" t="s">
         <v>13</v>
@@ -10363,10 +10365,10 @@
         <v>842</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C226" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="D226" s="0" t="s">
         <v>13</v>
@@ -10398,10 +10400,10 @@
         <v>845</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="D227" s="0" t="s">
         <v>13</v>
@@ -10433,10 +10435,10 @@
         <v>849</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D228" s="0" t="s">
         <v>13</v>
@@ -10468,10 +10470,10 @@
         <v>853</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D229" s="0" t="s">
         <v>13</v>
@@ -10503,10 +10505,10 @@
         <v>861</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D230" s="0" t="s">
         <v>13</v>
@@ -10538,10 +10540,10 @@
         <v>864</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="D231" s="0" t="s">
         <v>13</v>
@@ -10573,10 +10575,10 @@
         <v>871</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D232" s="0" t="s">
         <v>13</v>
@@ -10608,10 +10610,10 @@
         <v>887</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C233" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D233" s="0" t="s">
         <v>13</v>
@@ -10643,10 +10645,10 @@
         <v>898</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="D234" s="0" t="s">
         <v>13</v>
@@ -10678,10 +10680,10 @@
         <v>901</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D235" s="0" t="s">
         <v>13</v>
@@ -10713,16 +10715,16 @@
         <v>914</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D236" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E236" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F236" s="0" t="s">
         <v>179</v>
@@ -10748,10 +10750,10 @@
         <v>933</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D237" s="0" t="s">
         <v>13</v>
@@ -10783,10 +10785,10 @@
         <v>935</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D238" s="0" t="s">
         <v>13</v>
@@ -10818,10 +10820,10 @@
         <v>938</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D239" s="0" t="s">
         <v>13</v>
@@ -10853,10 +10855,10 @@
         <v>943</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D240" s="0" t="s">
         <v>13</v>
@@ -10888,10 +10890,10 @@
         <v>948</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D241" s="0" t="s">
         <v>13</v>
@@ -10923,10 +10925,10 @@
         <v>961</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D242" s="0" t="s">
         <v>13</v>
@@ -10958,10 +10960,10 @@
         <v>980</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D243" s="0" t="s">
         <v>13</v>
@@ -10993,10 +10995,10 @@
         <v>983</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D244" s="0" t="s">
         <v>13</v>
@@ -11028,10 +11030,10 @@
         <v>984</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D245" s="0" t="s">
         <v>13</v>
@@ -11063,10 +11065,10 @@
         <v>995</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D246" s="0" t="s">
         <v>13</v>
@@ -11098,10 +11100,10 @@
         <v>1001</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D247" s="0" t="s">
         <v>13</v>
@@ -11133,10 +11135,10 @@
         <v>1006</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D248" s="0" t="s">
         <v>13</v>
@@ -11148,7 +11150,7 @@
         <v>20</v>
       </c>
       <c r="G248" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H248" s="0" t="s">
         <v>16</v>
@@ -11168,10 +11170,10 @@
         <v>1019</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D249" s="0" t="s">
         <v>13</v>
@@ -11203,10 +11205,10 @@
         <v>1025</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D250" s="0" t="s">
         <v>13</v>
@@ -11238,10 +11240,10 @@
         <v>1037</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="D251" s="0" t="s">
         <v>13</v>
@@ -11273,10 +11275,10 @@
         <v>1094</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D252" s="0" t="s">
         <v>13</v>
@@ -11308,10 +11310,10 @@
         <v>1101</v>
       </c>
       <c r="B253" s="0" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D253" s="0" t="s">
         <v>13</v>
@@ -11343,10 +11345,10 @@
         <v>1103</v>
       </c>
       <c r="B254" s="0" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D254" s="0" t="s">
         <v>114</v>
@@ -11378,10 +11380,10 @@
         <v>1104</v>
       </c>
       <c r="B255" s="0" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D255" s="0" t="s">
         <v>13</v>
@@ -11413,10 +11415,10 @@
         <v>1116</v>
       </c>
       <c r="B256" s="0" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C256" s="0" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="D256" s="0" t="s">
         <v>13</v>
@@ -11448,10 +11450,10 @@
         <v>1119</v>
       </c>
       <c r="B257" s="0" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="D257" s="0" t="s">
         <v>13</v>
@@ -11483,10 +11485,10 @@
         <v>1123</v>
       </c>
       <c r="B258" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C258" s="0" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D258" s="0" t="s">
         <v>13</v>
@@ -11518,10 +11520,10 @@
         <v>1131</v>
       </c>
       <c r="B259" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D259" s="0" t="s">
         <v>13</v>
@@ -11553,10 +11555,10 @@
         <v>1137</v>
       </c>
       <c r="B260" s="0" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="D260" s="0" t="s">
         <v>13</v>
@@ -11588,10 +11590,10 @@
         <v>1145</v>
       </c>
       <c r="B261" s="0" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D261" s="0" t="s">
         <v>13</v>
@@ -11623,10 +11625,10 @@
         <v>1149</v>
       </c>
       <c r="B262" s="0" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C262" s="0" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D262" s="0" t="s">
         <v>13</v>
@@ -11658,10 +11660,10 @@
         <v>1153</v>
       </c>
       <c r="B263" s="0" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C263" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="D263" s="0" t="s">
         <v>13</v>
@@ -11693,10 +11695,10 @@
         <v>1159</v>
       </c>
       <c r="B264" s="0" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C264" s="0" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D264" s="0" t="s">
         <v>13</v>
@@ -11728,10 +11730,10 @@
         <v>1162</v>
       </c>
       <c r="B265" s="0" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C265" s="0" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="D265" s="0" t="s">
         <v>13</v>
@@ -11763,10 +11765,10 @@
         <v>1171</v>
       </c>
       <c r="B266" s="0" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C266" s="0" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="D266" s="0" t="s">
         <v>13</v>
@@ -11798,10 +11800,10 @@
         <v>1195</v>
       </c>
       <c r="B267" s="0" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C267" s="0" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D267" s="0" t="s">
         <v>13</v>
@@ -11833,10 +11835,10 @@
         <v>1208</v>
       </c>
       <c r="B268" s="0" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C268" s="0" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D268" s="0" t="s">
         <v>13</v>
@@ -11868,10 +11870,10 @@
         <v>1210</v>
       </c>
       <c r="B269" s="0" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C269" s="0" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D269" s="0" t="s">
         <v>13</v>
@@ -11903,16 +11905,16 @@
         <v>1214</v>
       </c>
       <c r="B270" s="0" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C270" s="0" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D270" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E270" s="0" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F270" s="0" t="s">
         <v>179</v>
@@ -11938,10 +11940,10 @@
         <v>1215</v>
       </c>
       <c r="B271" s="0" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C271" s="0" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D271" s="0" t="s">
         <v>13</v>
@@ -11973,10 +11975,10 @@
         <v>1231</v>
       </c>
       <c r="B272" s="0" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C272" s="0" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="D272" s="0" t="s">
         <v>13</v>
@@ -12008,10 +12010,10 @@
         <v>1238</v>
       </c>
       <c r="B273" s="0" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C273" s="0" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D273" s="0" t="s">
         <v>13</v>
@@ -12043,10 +12045,10 @@
         <v>1249</v>
       </c>
       <c r="B274" s="0" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C274" s="0" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="D274" s="0" t="s">
         <v>13</v>
@@ -12078,10 +12080,10 @@
         <v>1250</v>
       </c>
       <c r="B275" s="0" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C275" s="0" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D275" s="0" t="s">
         <v>13</v>
@@ -12113,10 +12115,10 @@
         <v>1261</v>
       </c>
       <c r="B276" s="0" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C276" s="0" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="D276" s="0" t="s">
         <v>13</v>
@@ -12148,10 +12150,10 @@
         <v>1262</v>
       </c>
       <c r="B277" s="0" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C277" s="0" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D277" s="0" t="s">
         <v>13</v>
@@ -12183,10 +12185,10 @@
         <v>1274</v>
       </c>
       <c r="B278" s="0" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C278" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="D278" s="0" t="s">
         <v>13</v>
@@ -12218,10 +12220,10 @@
         <v>1282</v>
       </c>
       <c r="B279" s="0" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C279" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D279" s="0" t="s">
         <v>13</v>
@@ -12253,10 +12255,10 @@
         <v>1290</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C280" s="0" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="D280" s="0" t="s">
         <v>13</v>
@@ -12288,10 +12290,10 @@
         <v>1300</v>
       </c>
       <c r="B281" s="0" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C281" s="0" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D281" s="0" t="s">
         <v>13</v>
@@ -12323,10 +12325,10 @@
         <v>1313</v>
       </c>
       <c r="B282" s="0" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C282" s="0" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="D282" s="0" t="s">
         <v>13</v>
@@ -12358,10 +12360,10 @@
         <v>1321</v>
       </c>
       <c r="B283" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C283" s="0" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="D283" s="0" t="s">
         <v>13</v>
@@ -12393,10 +12395,10 @@
         <v>1330</v>
       </c>
       <c r="B284" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C284" s="0" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D284" s="0" t="s">
         <v>13</v>
@@ -12428,10 +12430,10 @@
         <v>1355</v>
       </c>
       <c r="B285" s="0" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C285" s="0" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="D285" s="0" t="s">
         <v>13</v>
@@ -12463,10 +12465,10 @@
         <v>1360</v>
       </c>
       <c r="B286" s="0" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C286" s="0" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D286" s="0" t="s">
         <v>13</v>
@@ -12498,10 +12500,10 @@
         <v>1374</v>
       </c>
       <c r="B287" s="0" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C287" s="0" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D287" s="0" t="s">
         <v>13</v>
@@ -12533,10 +12535,10 @@
         <v>1389</v>
       </c>
       <c r="B288" s="0" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C288" s="0" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="D288" s="0" t="s">
         <v>13</v>
@@ -12568,10 +12570,10 @@
         <v>1394</v>
       </c>
       <c r="B289" s="0" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C289" s="0" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D289" s="0" t="s">
         <v>13</v>
@@ -12603,10 +12605,10 @@
         <v>1398</v>
       </c>
       <c r="B290" s="0" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C290" s="0" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D290" s="0" t="s">
         <v>13</v>
@@ -12638,10 +12640,10 @@
         <v>1411</v>
       </c>
       <c r="B291" s="0" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C291" s="0" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="D291" s="0" t="s">
         <v>13</v>
@@ -12673,10 +12675,10 @@
         <v>1424</v>
       </c>
       <c r="B292" s="0" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C292" s="0" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D292" s="0" t="s">
         <v>13</v>
@@ -12708,10 +12710,10 @@
         <v>1430</v>
       </c>
       <c r="B293" s="0" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C293" s="0" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="D293" s="0" t="s">
         <v>13</v>
@@ -12743,10 +12745,10 @@
         <v>1434</v>
       </c>
       <c r="B294" s="0" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C294" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D294" s="0" t="s">
         <v>13</v>
@@ -12778,10 +12780,10 @@
         <v>1444</v>
       </c>
       <c r="B295" s="0" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C295" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="D295" s="0" t="s">
         <v>13</v>
@@ -12813,10 +12815,10 @@
         <v>1450</v>
       </c>
       <c r="B296" s="0" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C296" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="D296" s="0" t="s">
         <v>13</v>
@@ -12828,7 +12830,7 @@
         <v>20</v>
       </c>
       <c r="G296" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H296" s="0" t="s">
         <v>16</v>
@@ -12848,10 +12850,10 @@
         <v>1451</v>
       </c>
       <c r="B297" s="0" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C297" s="0" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="D297" s="0" t="s">
         <v>13</v>
@@ -12883,10 +12885,10 @@
         <v>1453</v>
       </c>
       <c r="B298" s="0" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C298" s="0" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="D298" s="0" t="s">
         <v>13</v>
@@ -12918,10 +12920,10 @@
         <v>1457</v>
       </c>
       <c r="B299" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C299" s="0" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D299" s="0" t="s">
         <v>13</v>
@@ -12953,10 +12955,10 @@
         <v>1463</v>
       </c>
       <c r="B300" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C300" s="0" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D300" s="0" t="s">
         <v>13</v>
@@ -12988,10 +12990,10 @@
         <v>1466</v>
       </c>
       <c r="B301" s="0" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C301" s="0" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D301" s="0" t="s">
         <v>13</v>
@@ -13023,10 +13025,10 @@
         <v>1469</v>
       </c>
       <c r="B302" s="0" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C302" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="D302" s="0" t="s">
         <v>13</v>
@@ -13058,10 +13060,10 @@
         <v>1474</v>
       </c>
       <c r="B303" s="0" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C303" s="0" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D303" s="0" t="s">
         <v>13</v>
@@ -13093,10 +13095,10 @@
         <v>1500</v>
       </c>
       <c r="B304" s="0" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C304" s="0" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D304" s="0" t="s">
         <v>13</v>
@@ -13128,10 +13130,10 @@
         <v>1509</v>
       </c>
       <c r="B305" s="0" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C305" s="0" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="D305" s="0" t="s">
         <v>13</v>
@@ -13163,10 +13165,10 @@
         <v>1520</v>
       </c>
       <c r="B306" s="0" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C306" s="0" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D306" s="0" t="s">
         <v>13</v>
@@ -13198,10 +13200,10 @@
         <v>1529</v>
       </c>
       <c r="B307" s="0" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C307" s="0" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D307" s="0" t="s">
         <v>13</v>
@@ -13233,10 +13235,10 @@
         <v>1536</v>
       </c>
       <c r="B308" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C308" s="0" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="D308" s="0" t="s">
         <v>13</v>
@@ -13268,10 +13270,10 @@
         <v>1543</v>
       </c>
       <c r="B309" s="0" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C309" s="0" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D309" s="0" t="s">
         <v>13</v>
@@ -13303,10 +13305,10 @@
         <v>1553</v>
       </c>
       <c r="B310" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C310" s="0" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D310" s="0" t="s">
         <v>13</v>
@@ -13338,10 +13340,10 @@
         <v>1557</v>
       </c>
       <c r="B311" s="0" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C311" s="0" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="D311" s="0" t="s">
         <v>13</v>
@@ -13373,10 +13375,10 @@
         <v>1573</v>
       </c>
       <c r="B312" s="0" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C312" s="0" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D312" s="0" t="s">
         <v>13</v>
@@ -13408,10 +13410,10 @@
         <v>1592</v>
       </c>
       <c r="B313" s="0" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C313" s="0" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D313" s="0" t="s">
         <v>13</v>
@@ -13443,10 +13445,10 @@
         <v>1601</v>
       </c>
       <c r="B314" s="0" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="C314" s="0" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D314" s="0" t="s">
         <v>13</v>
@@ -13478,10 +13480,10 @@
         <v>1604</v>
       </c>
       <c r="B315" s="0" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C315" s="0" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D315" s="0" t="s">
         <v>13</v>
@@ -13513,10 +13515,10 @@
         <v>1612</v>
       </c>
       <c r="B316" s="0" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="C316" s="0" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="D316" s="0" t="s">
         <v>13</v>
@@ -13548,10 +13550,10 @@
         <v>1613</v>
       </c>
       <c r="B317" s="0" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="C317" s="0" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D317" s="0" t="s">
         <v>13</v>
@@ -13583,10 +13585,10 @@
         <v>1614</v>
       </c>
       <c r="B318" s="0" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C318" s="0" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D318" s="0" t="s">
         <v>13</v>
@@ -13618,10 +13620,10 @@
         <v>1617</v>
       </c>
       <c r="B319" s="0" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C319" s="0" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D319" s="0" t="s">
         <v>13</v>
@@ -13653,10 +13655,10 @@
         <v>1622</v>
       </c>
       <c r="B320" s="0" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C320" s="0" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D320" s="0" t="s">
         <v>13</v>
@@ -13668,7 +13670,7 @@
         <v>20</v>
       </c>
       <c r="G320" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H320" s="0" t="s">
         <v>16</v>
@@ -13688,10 +13690,10 @@
         <v>1625</v>
       </c>
       <c r="B321" s="0" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C321" s="0" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D321" s="0" t="s">
         <v>13</v>
@@ -13723,10 +13725,10 @@
         <v>1627</v>
       </c>
       <c r="B322" s="0" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C322" s="0" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="D322" s="0" t="s">
         <v>13</v>
@@ -13758,10 +13760,10 @@
         <v>1635</v>
       </c>
       <c r="B323" s="0" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="C323" s="0" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="D323" s="0" t="s">
         <v>13</v>
@@ -13793,10 +13795,10 @@
         <v>1639</v>
       </c>
       <c r="B324" s="0" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C324" s="0" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="D324" s="0" t="s">
         <v>13</v>
@@ -13828,10 +13830,10 @@
         <v>1644</v>
       </c>
       <c r="B325" s="0" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="C325" s="0" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="D325" s="0" t="s">
         <v>13</v>
@@ -13863,10 +13865,10 @@
         <v>1656</v>
       </c>
       <c r="B326" s="0" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="C326" s="0" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D326" s="0" t="s">
         <v>13</v>
@@ -13898,10 +13900,10 @@
         <v>1664</v>
       </c>
       <c r="B327" s="0" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C327" s="0" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="D327" s="0" t="s">
         <v>13</v>
@@ -13933,10 +13935,10 @@
         <v>1669</v>
       </c>
       <c r="B328" s="0" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C328" s="0" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D328" s="0" t="s">
         <v>13</v>
@@ -13968,10 +13970,10 @@
         <v>1677</v>
       </c>
       <c r="B329" s="0" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C329" s="0" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="D329" s="0" t="s">
         <v>13</v>
@@ -14003,10 +14005,10 @@
         <v>1678</v>
       </c>
       <c r="B330" s="0" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C330" s="0" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D330" s="0" t="s">
         <v>13</v>
@@ -14038,10 +14040,10 @@
         <v>1681</v>
       </c>
       <c r="B331" s="0" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C331" s="0" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="D331" s="0" t="s">
         <v>13</v>
@@ -14073,10 +14075,10 @@
         <v>1689</v>
       </c>
       <c r="B332" s="0" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C332" s="0" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D332" s="0" t="s">
         <v>13</v>
@@ -14108,10 +14110,10 @@
         <v>1692</v>
       </c>
       <c r="B333" s="0" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C333" s="0" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D333" s="0" t="s">
         <v>13</v>
@@ -14143,10 +14145,10 @@
         <v>1696</v>
       </c>
       <c r="B334" s="0" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C334" s="0" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="D334" s="0" t="s">
         <v>13</v>
@@ -14178,10 +14180,10 @@
         <v>1701</v>
       </c>
       <c r="B335" s="0" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C335" s="0" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="D335" s="0" t="s">
         <v>13</v>
@@ -14213,10 +14215,10 @@
         <v>1705</v>
       </c>
       <c r="B336" s="0" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C336" s="0" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D336" s="0" t="s">
         <v>13</v>
@@ -14248,10 +14250,10 @@
         <v>1711</v>
       </c>
       <c r="B337" s="0" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C337" s="0" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D337" s="0" t="s">
         <v>13</v>
@@ -14283,10 +14285,10 @@
         <v>1715</v>
       </c>
       <c r="B338" s="0" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="C338" s="0" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D338" s="0" t="s">
         <v>13</v>
@@ -14318,10 +14320,10 @@
         <v>1720</v>
       </c>
       <c r="B339" s="0" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="C339" s="0" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="D339" s="0" t="s">
         <v>13</v>
@@ -14353,10 +14355,10 @@
         <v>1725</v>
       </c>
       <c r="B340" s="0" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C340" s="0" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D340" s="0" t="s">
         <v>13</v>
@@ -14388,10 +14390,10 @@
         <v>1733</v>
       </c>
       <c r="B341" s="0" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C341" s="0" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D341" s="0" t="s">
         <v>13</v>
@@ -14423,10 +14425,10 @@
         <v>1744</v>
       </c>
       <c r="B342" s="0" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="C342" s="0" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="D342" s="0" t="s">
         <v>13</v>
@@ -14458,10 +14460,10 @@
         <v>1753</v>
       </c>
       <c r="B343" s="0" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C343" s="0" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D343" s="0" t="s">
         <v>13</v>
@@ -14493,10 +14495,10 @@
         <v>1756</v>
       </c>
       <c r="B344" s="0" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C344" s="0" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D344" s="0" t="s">
         <v>13</v>
@@ -14528,10 +14530,10 @@
         <v>1769</v>
       </c>
       <c r="B345" s="0" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C345" s="0" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="D345" s="0" t="s">
         <v>13</v>
@@ -14563,10 +14565,10 @@
         <v>1775</v>
       </c>
       <c r="B346" s="0" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C346" s="0" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D346" s="0" t="s">
         <v>13</v>
@@ -14598,10 +14600,10 @@
         <v>1779</v>
       </c>
       <c r="B347" s="0" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C347" s="0" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D347" s="0" t="s">
         <v>13</v>
@@ -14633,10 +14635,10 @@
         <v>1790</v>
       </c>
       <c r="B348" s="0" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C348" s="0" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D348" s="0" t="s">
         <v>13</v>
@@ -14668,10 +14670,10 @@
         <v>1800</v>
       </c>
       <c r="B349" s="0" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="C349" s="0" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="D349" s="0" t="s">
         <v>13</v>
@@ -14703,10 +14705,10 @@
         <v>1810</v>
       </c>
       <c r="B350" s="0" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="C350" s="0" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="D350" s="0" t="s">
         <v>13</v>
@@ -14738,10 +14740,10 @@
         <v>1812</v>
       </c>
       <c r="B351" s="0" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C351" s="0" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D351" s="0" t="s">
         <v>13</v>
@@ -14773,10 +14775,10 @@
         <v>1818</v>
       </c>
       <c r="B352" s="0" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C352" s="0" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="D352" s="0" t="s">
         <v>13</v>
@@ -14808,10 +14810,10 @@
         <v>1826</v>
       </c>
       <c r="B353" s="0" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="C353" s="0" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D353" s="0" t="s">
         <v>13</v>
@@ -14843,10 +14845,10 @@
         <v>1831</v>
       </c>
       <c r="B354" s="0" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C354" s="0" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D354" s="0" t="s">
         <v>13</v>
@@ -14878,10 +14880,10 @@
         <v>1838</v>
       </c>
       <c r="B355" s="0" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="C355" s="0" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="D355" s="0" t="s">
         <v>13</v>
@@ -14893,7 +14895,7 @@
         <v>20</v>
       </c>
       <c r="G355" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H355" s="0" t="s">
         <v>16</v>
@@ -14913,10 +14915,10 @@
         <v>1846</v>
       </c>
       <c r="B356" s="0" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C356" s="0" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D356" s="0" t="s">
         <v>13</v>
@@ -14948,10 +14950,10 @@
         <v>1850</v>
       </c>
       <c r="B357" s="0" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="C357" s="0" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="D357" s="0" t="s">
         <v>13</v>
@@ -14983,10 +14985,10 @@
         <v>1852</v>
       </c>
       <c r="B358" s="0" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C358" s="0" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D358" s="0" t="s">
         <v>13</v>
@@ -15018,10 +15020,10 @@
         <v>1868</v>
       </c>
       <c r="B359" s="0" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C359" s="0" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="D359" s="0" t="s">
         <v>13</v>
@@ -15053,10 +15055,10 @@
         <v>1876</v>
       </c>
       <c r="B360" s="0" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C360" s="0" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="D360" s="0" t="s">
         <v>13</v>
@@ -15088,10 +15090,10 @@
         <v>1877</v>
       </c>
       <c r="B361" s="0" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C361" s="0" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D361" s="0" t="s">
         <v>13</v>
@@ -15123,10 +15125,10 @@
         <v>1878</v>
       </c>
       <c r="B362" s="0" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C362" s="0" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="D362" s="0" t="s">
         <v>13</v>
@@ -15158,10 +15160,10 @@
         <v>1880</v>
       </c>
       <c r="B363" s="0" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C363" s="0" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="D363" s="0" t="s">
         <v>13</v>
@@ -15193,10 +15195,10 @@
         <v>1887</v>
       </c>
       <c r="B364" s="0" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="C364" s="0" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="D364" s="0" t="s">
         <v>13</v>
@@ -15228,10 +15230,10 @@
         <v>1890</v>
       </c>
       <c r="B365" s="0" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C365" s="0" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D365" s="0" t="s">
         <v>13</v>
@@ -15263,10 +15265,10 @@
         <v>1893</v>
       </c>
       <c r="B366" s="0" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="C366" s="0" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D366" s="0" t="s">
         <v>13</v>
@@ -15298,10 +15300,10 @@
         <v>1894</v>
       </c>
       <c r="B367" s="0" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C367" s="0" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="D367" s="0" t="s">
         <v>13</v>
@@ -15333,10 +15335,10 @@
         <v>1899</v>
       </c>
       <c r="B368" s="0" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C368" s="0" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="D368" s="0" t="s">
         <v>13</v>
@@ -15368,10 +15370,10 @@
         <v>1915</v>
       </c>
       <c r="B369" s="0" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C369" s="0" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="D369" s="0" t="s">
         <v>13</v>
@@ -15403,10 +15405,10 @@
         <v>1928</v>
       </c>
       <c r="B370" s="0" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C370" s="0" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D370" s="0" t="s">
         <v>13</v>
@@ -15438,10 +15440,10 @@
         <v>1933</v>
       </c>
       <c r="B371" s="0" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C371" s="0" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="D371" s="0" t="s">
         <v>13</v>
@@ -15473,10 +15475,10 @@
         <v>1960</v>
       </c>
       <c r="B372" s="0" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C372" s="0" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="D372" s="0" t="s">
         <v>13</v>
@@ -15508,10 +15510,10 @@
         <v>1966</v>
       </c>
       <c r="B373" s="0" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C373" s="0" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D373" s="0" t="s">
         <v>13</v>
@@ -15520,7 +15522,7 @@
         <v>20</v>
       </c>
       <c r="F373" s="0" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="G373" s="0" t="s">
         <v>16</v>
@@ -15543,10 +15545,10 @@
         <v>11000</v>
       </c>
       <c r="B374" s="0" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C374" s="0" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="D374" s="0" t="s">
         <v>13</v>
@@ -15578,10 +15580,10 @@
         <v>11050</v>
       </c>
       <c r="B375" s="0" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="C375" s="0" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="D375" s="0" t="s">
         <v>13</v>
@@ -15613,10 +15615,10 @@
         <v>11100</v>
       </c>
       <c r="B376" s="0" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C376" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D376" s="0" t="s">
         <v>13</v>
@@ -15648,10 +15650,10 @@
         <v>11150</v>
       </c>
       <c r="B377" s="0" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="C377" s="0" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="D377" s="0" t="s">
         <v>13</v>
@@ -15683,10 +15685,10 @@
         <v>11200</v>
       </c>
       <c r="B378" s="0" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C378" s="0" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D378" s="0" t="s">
         <v>13</v>
@@ -15718,10 +15720,10 @@
         <v>11250</v>
       </c>
       <c r="B379" s="0" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="C379" s="0" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D379" s="0" t="s">
         <v>13</v>
@@ -15753,10 +15755,10 @@
         <v>11300</v>
       </c>
       <c r="B380" s="0" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C380" s="0" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="D380" s="0" t="s">
         <v>13</v>
@@ -15788,10 +15790,10 @@
         <v>11350</v>
       </c>
       <c r="B381" s="0" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C381" s="0" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="D381" s="0" t="s">
         <v>13</v>
@@ -15803,7 +15805,7 @@
         <v>20</v>
       </c>
       <c r="G381" s="0" t="s">
-        <v>16</v>
+        <v>264</v>
       </c>
       <c r="H381" s="0" t="s">
         <v>16</v>
@@ -15823,10 +15825,10 @@
         <v>11400</v>
       </c>
       <c r="B382" s="0" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="C382" s="0" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D382" s="0" t="s">
         <v>13</v>
@@ -15858,10 +15860,10 @@
         <v>11450</v>
       </c>
       <c r="B383" s="0" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C383" s="0" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="D383" s="0" t="s">
         <v>13</v>
@@ -15893,10 +15895,10 @@
         <v>11500</v>
       </c>
       <c r="B384" s="0" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="C384" s="0" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="D384" s="0" t="s">
         <v>13</v>
@@ -15928,10 +15930,10 @@
         <v>11550</v>
       </c>
       <c r="B385" s="0" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C385" s="0" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="D385" s="0" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
initial attempt for #73
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -13,6 +13,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">atlas_list!$A$1:$K$51</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">atlas_list!$A$1:$K$51</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">atlas_list!$A$1:$K$51</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
   <si>
     <t xml:space="preserve">species_order</t>
   </si>
@@ -59,6 +60,9 @@
     <t xml:space="preserve">distribution</t>
   </si>
   <si>
+    <t xml:space="preserve">profile_url</t>
+  </si>
+  <si>
     <t xml:space="preserve">Anseranas semipalmata</t>
   </si>
   <si>
@@ -78,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">land</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://farm2.staticflickr.com/1883/44747039332_0666291b70_o_d.png</t>
   </si>
   <si>
     <t xml:space="preserve">Columba livia</t>
@@ -263,28 +270,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5714285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.984693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="80.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1224489795918"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.3469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.3520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.984693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5357142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="13.1683673469388"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -318,31 +325,34 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>1700</v>
@@ -351,33 +361,36 @@
         <v>1700</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>81</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>1700</v>
@@ -386,7 +399,7 @@
         <v>1700</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,25 +407,25 @@
         <v>128</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>1700</v>
@@ -421,7 +434,7 @@
         <v>1700</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,25 +442,25 @@
         <v>173</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>1700</v>
@@ -456,7 +469,7 @@
         <v>1700</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,25 +477,25 @@
         <v>201</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>1700</v>
@@ -491,7 +504,7 @@
         <v>1700</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,25 +512,25 @@
         <v>218</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>1700</v>
@@ -526,7 +539,7 @@
         <v>1700</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,25 +547,25 @@
         <v>330</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>1700</v>
@@ -561,7 +574,7 @@
         <v>1700</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,25 +582,25 @@
         <v>340</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="G9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>1700</v>
@@ -596,7 +609,7 @@
         <v>1700</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,25 +617,25 @@
         <v>411</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>1700</v>
@@ -631,7 +644,7 @@
         <v>1700</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,19 +652,19 @@
         <v>493</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>1700</v>
@@ -660,7 +673,7 @@
         <v>1700</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added a few photo links
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="838">
   <si>
     <t>species_order</t>
   </si>
@@ -2490,6 +2490,54 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4844/45748208141_d9644b3842_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4865/44849846555_7f59f7c99e_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1927/30823273837_2772163664_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4861/44849823975_13a79ac5fb_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4839/45713194162_6e3c91bbfa_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4804/30823257747_3b99e4059c_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4820/45038273264_a70c862dca_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1934/45038271104_90620a4f83_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1912/45038269094_bc40949d24_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4824/43945599780_c431c35de5_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4857/45763352411_ca8876b80b_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4827/44850284545_d1c1a05c32_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4851/45763822791_e7a4985ed6_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4830/43946076730_cb74142588_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4817/43946076920_855c9ce67c_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4903/43946078610_32800b179c_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4897/43946083370_c13241a0f1_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2808,8 +2856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2937,6 +2985,9 @@
       <c r="K3" t="s">
         <v>18</v>
       </c>
+      <c r="L3" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2972,6 +3023,9 @@
       <c r="K4" t="s">
         <v>18</v>
       </c>
+      <c r="L4" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -3077,6 +3131,9 @@
       <c r="K7" t="s">
         <v>18</v>
       </c>
+      <c r="L7" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -3182,6 +3239,9 @@
       <c r="K10" t="s">
         <v>18</v>
       </c>
+      <c r="L10" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -3287,6 +3347,9 @@
       <c r="K13" t="s">
         <v>18</v>
       </c>
+      <c r="L13" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3322,6 +3385,9 @@
       <c r="K14" t="s">
         <v>18</v>
       </c>
+      <c r="L14" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -3392,6 +3458,9 @@
       <c r="K16" t="s">
         <v>18</v>
       </c>
+      <c r="L16" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -3953,7 +4022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>128</v>
       </c>
@@ -3988,7 +4057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>134</v>
       </c>
@@ -4023,7 +4092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>145</v>
       </c>
@@ -4058,7 +4127,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>149</v>
       </c>
@@ -4093,7 +4162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>151</v>
       </c>
@@ -4128,7 +4197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>158</v>
       </c>
@@ -4163,7 +4232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>161</v>
       </c>
@@ -4198,7 +4267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>167</v>
       </c>
@@ -4233,7 +4302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>171</v>
       </c>
@@ -4268,7 +4337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>173</v>
       </c>
@@ -4303,7 +4372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>175</v>
       </c>
@@ -4338,7 +4407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>178</v>
       </c>
@@ -4373,7 +4442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>184</v>
       </c>
@@ -4408,7 +4477,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>186</v>
       </c>
@@ -4443,7 +4512,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>189</v>
       </c>
@@ -4477,8 +4546,11 @@
       <c r="K47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>192</v>
       </c>
@@ -4513,7 +4585,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>195</v>
       </c>
@@ -4548,7 +4620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>201</v>
       </c>
@@ -4583,7 +4655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>206</v>
       </c>
@@ -4618,7 +4690,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>213</v>
       </c>
@@ -4653,7 +4725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>218</v>
       </c>
@@ -4688,7 +4760,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>223</v>
       </c>
@@ -4723,7 +4795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>228</v>
       </c>
@@ -4758,7 +4830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>234</v>
       </c>
@@ -4793,7 +4865,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>241</v>
       </c>
@@ -4828,7 +4900,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>246</v>
       </c>
@@ -4863,7 +4935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>249</v>
       </c>
@@ -4897,8 +4969,11 @@
       <c r="K59" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>251</v>
       </c>
@@ -4933,7 +5008,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>253</v>
       </c>
@@ -4968,7 +5043,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>259</v>
       </c>
@@ -5003,7 +5078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>265</v>
       </c>
@@ -5038,7 +5113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>267</v>
       </c>
@@ -5839,6 +5914,9 @@
       <c r="K86" t="s">
         <v>18</v>
       </c>
+      <c r="L86" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
@@ -8557,6 +8635,9 @@
       <c r="K167" t="s">
         <v>18</v>
       </c>
+      <c r="L167" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168">
@@ -8662,6 +8743,9 @@
       <c r="K170" t="s">
         <v>18</v>
       </c>
+      <c r="L170" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171">
@@ -14452,7 +14536,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1711</v>
       </c>
@@ -14487,7 +14571,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>1715</v>
       </c>
@@ -14522,7 +14606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>1720</v>
       </c>
@@ -14557,7 +14641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>1725</v>
       </c>
@@ -14592,7 +14676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>1733</v>
       </c>
@@ -14626,8 +14710,11 @@
       <c r="K341" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L341" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>1744</v>
       </c>
@@ -14662,7 +14749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>1753</v>
       </c>
@@ -14697,7 +14784,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>1756</v>
       </c>
@@ -14732,7 +14819,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>1769</v>
       </c>
@@ -14767,7 +14854,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>1775</v>
       </c>
@@ -14802,7 +14889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>1779</v>
       </c>
@@ -14836,8 +14923,11 @@
       <c r="K347" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L347" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>1790</v>
       </c>
@@ -14871,8 +14961,11 @@
       <c r="K348" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L348" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>1800</v>
       </c>
@@ -14907,7 +15000,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1810</v>
       </c>
@@ -14942,7 +15035,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>1812</v>
       </c>
@@ -14977,7 +15070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>1818</v>
       </c>
@@ -15012,7 +15105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>1826</v>
       </c>
@@ -15047,7 +15140,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>1831</v>
       </c>
@@ -15082,7 +15175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>1838</v>
       </c>
@@ -15114,7 +15207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>1846</v>
       </c>
@@ -15149,7 +15242,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>1850</v>
       </c>
@@ -15184,7 +15277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>1852</v>
       </c>
@@ -15219,7 +15312,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>1868</v>
       </c>
@@ -15254,7 +15347,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>1876</v>
       </c>
@@ -15289,7 +15382,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>1877</v>
       </c>
@@ -15324,7 +15417,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>1878</v>
       </c>
@@ -15359,7 +15452,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>1880</v>
       </c>
@@ -15394,7 +15487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>1887</v>
       </c>
@@ -15429,7 +15522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>1890</v>
       </c>
@@ -15461,7 +15554,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>1893</v>
       </c>
@@ -15496,7 +15589,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>1894</v>
       </c>
@@ -15531,7 +15624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>1899</v>
       </c>
@@ -15564,6 +15657,9 @@
       </c>
       <c r="K368" t="s">
         <v>18</v>
+      </c>
+      <c r="L368" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Remove American Golden Plover from Species List
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0B3378D-9F91-4F5C-BE3D-6CEB4FDD5469}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="836">
   <si>
     <t>species_order</t>
   </si>
@@ -531,12 +532,6 @@
   </si>
   <si>
     <t>Pacific Golden Plover</t>
-  </si>
-  <si>
-    <t>Pluvialis dominica</t>
-  </si>
-  <si>
-    <t>American Golden Plover</t>
   </si>
   <si>
     <t>Charadrius ruficapillus</t>
@@ -2543,7 +2538,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2853,11 +2848,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2981,7 @@
         <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3024,7 +3019,7 @@
         <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3102,7 +3097,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -3129,7 +3124,7 @@
         <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3237,7 +3232,7 @@
         <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3342,7 +3337,7 @@
         <v>17</v>
       </c>
       <c r="L13" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3377,7 +3372,7 @@
         <v>17</v>
       </c>
       <c r="L14" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3450,7 +3445,7 @@
         <v>17</v>
       </c>
       <c r="L16" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -3645,7 +3640,7 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="H22">
         <v>6</v>
@@ -4529,7 +4524,7 @@
         <v>17</v>
       </c>
       <c r="L47" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -4946,7 +4941,7 @@
         <v>17</v>
       </c>
       <c r="L59" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -5226,7 +5221,7 @@
         <v>17</v>
       </c>
       <c r="L67" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -5401,7 +5396,7 @@
         <v>17</v>
       </c>
       <c r="L72" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -5528,8 +5523,11 @@
       <c r="F76" t="s">
         <v>21</v>
       </c>
-      <c r="H76">
-        <v>6</v>
+      <c r="G76" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" t="s">
+        <v>16</v>
       </c>
       <c r="I76">
         <v>2005</v>
@@ -5555,7 +5553,7 @@
         <v>14</v>
       </c>
       <c r="E77" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="F77" t="s">
         <v>21</v>
@@ -5581,19 +5579,19 @@
         <v>298</v>
       </c>
       <c r="B78" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C78" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D78" t="s">
         <v>14</v>
       </c>
       <c r="E78" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F78" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="G78" t="s">
         <v>16</v>
@@ -5616,19 +5614,19 @@
         <v>300</v>
       </c>
       <c r="B79" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C79" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D79" t="s">
         <v>14</v>
       </c>
       <c r="E79" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F79" t="s">
-        <v>179</v>
+        <v>114</v>
       </c>
       <c r="G79" t="s">
         <v>16</v>
@@ -5651,19 +5649,19 @@
         <v>303</v>
       </c>
       <c r="B80" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C80" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
       </c>
       <c r="E80" t="s">
-        <v>182</v>
+        <v>21</v>
       </c>
       <c r="F80" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G80" t="s">
         <v>16</v>
@@ -5700,9 +5698,6 @@
       <c r="F81" t="s">
         <v>21</v>
       </c>
-      <c r="G81" t="s">
-        <v>16</v>
-      </c>
       <c r="H81" t="s">
         <v>16</v>
       </c>
@@ -5735,6 +5730,9 @@
       <c r="F82" t="s">
         <v>21</v>
       </c>
+      <c r="G82" t="s">
+        <v>16</v>
+      </c>
       <c r="H82" t="s">
         <v>16</v>
       </c>
@@ -5782,6 +5780,9 @@
       <c r="K83" t="s">
         <v>17</v>
       </c>
+      <c r="L83" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -5794,19 +5795,16 @@
         <v>190</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="E84" t="s">
-        <v>21</v>
+        <v>191</v>
       </c>
       <c r="F84" t="s">
-        <v>21</v>
-      </c>
-      <c r="G84" t="s">
-        <v>16</v>
-      </c>
-      <c r="H84" t="s">
-        <v>16</v>
+        <v>114</v>
+      </c>
+      <c r="H84">
+        <v>6</v>
       </c>
       <c r="I84">
         <v>2005</v>
@@ -5816,9 +5814,6 @@
       </c>
       <c r="K84" t="s">
         <v>17</v>
-      </c>
-      <c r="L84" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5826,22 +5821,25 @@
         <v>319</v>
       </c>
       <c r="B85" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C85" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D85" t="s">
-        <v>179</v>
+        <v>14</v>
       </c>
       <c r="E85" t="s">
-        <v>193</v>
+        <v>21</v>
       </c>
       <c r="F85" t="s">
-        <v>114</v>
-      </c>
-      <c r="H85">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="G85" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" t="s">
+        <v>16</v>
       </c>
       <c r="I85">
         <v>2005</v>
@@ -5851,6 +5849,9 @@
       </c>
       <c r="K85" t="s">
         <v>17</v>
+      </c>
+      <c r="L85" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -5867,7 +5868,7 @@
         <v>14</v>
       </c>
       <c r="E86" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="F86" t="s">
         <v>21</v>
@@ -5886,9 +5887,6 @@
       </c>
       <c r="K86" t="s">
         <v>17</v>
-      </c>
-      <c r="L86" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -5910,11 +5908,8 @@
       <c r="F87" t="s">
         <v>21</v>
       </c>
-      <c r="G87" t="s">
-        <v>16</v>
-      </c>
-      <c r="H87" t="s">
-        <v>16</v>
+      <c r="H87">
+        <v>6</v>
       </c>
       <c r="I87">
         <v>2005</v>
@@ -5937,16 +5932,19 @@
         <v>199</v>
       </c>
       <c r="D88" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="E88" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="F88" t="s">
-        <v>21</v>
-      </c>
-      <c r="H88">
-        <v>6</v>
+        <v>177</v>
+      </c>
+      <c r="G88" t="s">
+        <v>16</v>
+      </c>
+      <c r="H88" t="s">
+        <v>16</v>
       </c>
       <c r="I88">
         <v>2005</v>
@@ -5963,19 +5961,19 @@
         <v>330</v>
       </c>
       <c r="B89" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D89" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="E89" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F89" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="G89" t="s">
         <v>16</v>
@@ -5998,19 +5996,19 @@
         <v>331</v>
       </c>
       <c r="B90" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C90" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D90" t="s">
         <v>153</v>
       </c>
       <c r="E90" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="F90" t="s">
-        <v>206</v>
+        <v>21</v>
       </c>
       <c r="G90" t="s">
         <v>16</v>
@@ -6039,7 +6037,7 @@
         <v>208</v>
       </c>
       <c r="D91" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E91" t="s">
         <v>166</v>
@@ -6074,13 +6072,13 @@
         <v>210</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="E92" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="F92" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="G92" t="s">
         <v>16</v>
@@ -6109,13 +6107,13 @@
         <v>212</v>
       </c>
       <c r="D93" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="E93" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="F93" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G93" t="s">
         <v>16</v>
@@ -6144,13 +6142,13 @@
         <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E94" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="F94" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="G94" t="s">
         <v>16</v>
@@ -6237,6 +6235,9 @@
       <c r="K96" t="s">
         <v>17</v>
       </c>
+      <c r="L96" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -6249,13 +6250,13 @@
         <v>220</v>
       </c>
       <c r="D97" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E97" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="F97" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="G97" t="s">
         <v>16</v>
@@ -6273,7 +6274,7 @@
         <v>17</v>
       </c>
       <c r="L97" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -6287,19 +6288,16 @@
         <v>222</v>
       </c>
       <c r="D98" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E98" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="F98" t="s">
-        <v>179</v>
-      </c>
-      <c r="G98" t="s">
-        <v>16</v>
-      </c>
-      <c r="H98" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="H98">
+        <v>6</v>
       </c>
       <c r="I98">
         <v>2005</v>
@@ -6309,9 +6307,6 @@
       </c>
       <c r="K98" t="s">
         <v>17</v>
-      </c>
-      <c r="L98" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -6333,8 +6328,11 @@
       <c r="F99" t="s">
         <v>21</v>
       </c>
-      <c r="H99">
-        <v>6</v>
+      <c r="G99" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" t="s">
+        <v>16</v>
       </c>
       <c r="I99">
         <v>2005</v>
@@ -6365,9 +6363,6 @@
       <c r="F100" t="s">
         <v>21</v>
       </c>
-      <c r="G100" t="s">
-        <v>16</v>
-      </c>
       <c r="H100" t="s">
         <v>16</v>
       </c>
@@ -6400,8 +6395,11 @@
       <c r="F101" t="s">
         <v>21</v>
       </c>
-      <c r="H101" t="s">
-        <v>16</v>
+      <c r="G101" t="s">
+        <v>835</v>
+      </c>
+      <c r="H101">
+        <v>6</v>
       </c>
       <c r="I101">
         <v>2005</v>
@@ -6424,16 +6422,13 @@
         <v>230</v>
       </c>
       <c r="D102" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E102" t="s">
         <v>166</v>
       </c>
       <c r="F102" t="s">
         <v>21</v>
-      </c>
-      <c r="G102" t="s">
-        <v>837</v>
       </c>
       <c r="H102">
         <v>6</v>
@@ -6459,7 +6454,7 @@
         <v>232</v>
       </c>
       <c r="D103" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E103" t="s">
         <v>166</v>
@@ -6467,8 +6462,11 @@
       <c r="F103" t="s">
         <v>21</v>
       </c>
-      <c r="H103">
-        <v>6</v>
+      <c r="G103" t="s">
+        <v>16</v>
+      </c>
+      <c r="H103" t="s">
+        <v>16</v>
       </c>
       <c r="I103">
         <v>2005</v>
@@ -6599,16 +6597,13 @@
         <v>14</v>
       </c>
       <c r="E107" t="s">
-        <v>166</v>
+        <v>241</v>
       </c>
       <c r="F107" t="s">
         <v>21</v>
       </c>
-      <c r="G107" t="s">
-        <v>16</v>
-      </c>
-      <c r="H107" t="s">
-        <v>16</v>
+      <c r="H107">
+        <v>6</v>
       </c>
       <c r="I107">
         <v>2005</v>
@@ -6625,16 +6620,16 @@
         <v>370</v>
       </c>
       <c r="B108" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C108" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D108" t="s">
         <v>14</v>
       </c>
       <c r="E108" t="s">
-        <v>243</v>
+        <v>21</v>
       </c>
       <c r="F108" t="s">
         <v>21</v>
@@ -6666,13 +6661,16 @@
         <v>14</v>
       </c>
       <c r="E109" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="F109" t="s">
         <v>21</v>
       </c>
-      <c r="H109">
-        <v>6</v>
+      <c r="G109" t="s">
+        <v>16</v>
+      </c>
+      <c r="H109" t="s">
+        <v>16</v>
       </c>
       <c r="I109">
         <v>2005</v>
@@ -6768,7 +6766,7 @@
         <v>14</v>
       </c>
       <c r="E112" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="F112" t="s">
         <v>21</v>
@@ -6800,13 +6798,13 @@
         <v>253</v>
       </c>
       <c r="D113" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E113" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="F113" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G113" t="s">
         <v>16</v>
@@ -6829,19 +6827,19 @@
         <v>384</v>
       </c>
       <c r="B114" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C114" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="D114" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E114" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="F114" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G114" t="s">
         <v>16</v>
@@ -6878,9 +6876,6 @@
       <c r="F115" t="s">
         <v>21</v>
       </c>
-      <c r="G115" t="s">
-        <v>16</v>
-      </c>
       <c r="H115" t="s">
         <v>16</v>
       </c>
@@ -6908,7 +6903,7 @@
         <v>14</v>
       </c>
       <c r="E116" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F116" t="s">
         <v>21</v>
@@ -6931,23 +6926,20 @@
         <v>392</v>
       </c>
       <c r="B117" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C117" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D117" t="s">
         <v>14</v>
       </c>
       <c r="E117" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F117" t="s">
         <v>21</v>
       </c>
-      <c r="H117" t="s">
-        <v>16</v>
-      </c>
       <c r="I117">
         <v>2005</v>
       </c>
@@ -6955,7 +6947,7 @@
         <v>1700</v>
       </c>
       <c r="K117" t="s">
-        <v>17</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -6963,28 +6955,34 @@
         <v>394</v>
       </c>
       <c r="B118" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C118" t="s">
+        <v>267</v>
+      </c>
+      <c r="D118" t="s">
+        <v>14</v>
+      </c>
+      <c r="E118" t="s">
+        <v>111</v>
+      </c>
+      <c r="F118" t="s">
+        <v>21</v>
+      </c>
+      <c r="G118" t="s">
+        <v>16</v>
+      </c>
+      <c r="H118" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118">
+        <v>2005</v>
+      </c>
+      <c r="J118">
+        <v>1700</v>
+      </c>
+      <c r="K118" t="s">
         <v>265</v>
-      </c>
-      <c r="D118" t="s">
-        <v>14</v>
-      </c>
-      <c r="E118" t="s">
-        <v>266</v>
-      </c>
-      <c r="F118" t="s">
-        <v>21</v>
-      </c>
-      <c r="I118">
-        <v>2005</v>
-      </c>
-      <c r="J118">
-        <v>1700</v>
-      </c>
-      <c r="K118" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -7001,7 +6999,7 @@
         <v>14</v>
       </c>
       <c r="E119" t="s">
-        <v>111</v>
+        <v>264</v>
       </c>
       <c r="F119" t="s">
         <v>21</v>
@@ -7019,7 +7017,7 @@
         <v>1700</v>
       </c>
       <c r="K119" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -7036,14 +7034,11 @@
         <v>14</v>
       </c>
       <c r="E120" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F120" t="s">
         <v>21</v>
       </c>
-      <c r="G120" t="s">
-        <v>16</v>
-      </c>
       <c r="H120" t="s">
         <v>16</v>
       </c>
@@ -7054,7 +7049,7 @@
         <v>1700</v>
       </c>
       <c r="K120" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -7071,7 +7066,7 @@
         <v>14</v>
       </c>
       <c r="E121" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F121" t="s">
         <v>21</v>
@@ -7086,7 +7081,7 @@
         <v>1700</v>
       </c>
       <c r="K121" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -7103,11 +7098,14 @@
         <v>14</v>
       </c>
       <c r="E122" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F122" t="s">
         <v>21</v>
       </c>
+      <c r="G122" t="s">
+        <v>16</v>
+      </c>
       <c r="H122" t="s">
         <v>16</v>
       </c>
@@ -7118,7 +7116,7 @@
         <v>1700</v>
       </c>
       <c r="K122" t="s">
-        <v>267</v>
+        <v>17</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -7135,13 +7133,10 @@
         <v>14</v>
       </c>
       <c r="E123" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F123" t="s">
         <v>21</v>
-      </c>
-      <c r="G123" t="s">
-        <v>16</v>
       </c>
       <c r="H123" t="s">
         <v>16</v>
@@ -7170,7 +7165,7 @@
         <v>14</v>
       </c>
       <c r="E124" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F124" t="s">
         <v>21</v>
@@ -7202,7 +7197,7 @@
         <v>14</v>
       </c>
       <c r="E125" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F125" t="s">
         <v>21</v>
@@ -7234,7 +7229,7 @@
         <v>14</v>
       </c>
       <c r="E126" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F126" t="s">
         <v>21</v>
@@ -7249,7 +7244,7 @@
         <v>1700</v>
       </c>
       <c r="K126" t="s">
-        <v>17</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -7266,11 +7261,14 @@
         <v>14</v>
       </c>
       <c r="E127" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F127" t="s">
         <v>21</v>
       </c>
+      <c r="G127" t="s">
+        <v>16</v>
+      </c>
       <c r="H127" t="s">
         <v>16</v>
       </c>
@@ -7281,7 +7279,7 @@
         <v>1700</v>
       </c>
       <c r="K127" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -7298,7 +7296,7 @@
         <v>14</v>
       </c>
       <c r="E128" t="s">
-        <v>266</v>
+        <v>166</v>
       </c>
       <c r="F128" t="s">
         <v>21</v>
@@ -7316,7 +7314,7 @@
         <v>1700</v>
       </c>
       <c r="K128" t="s">
-        <v>267</v>
+        <v>17</v>
       </c>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
@@ -7333,7 +7331,7 @@
         <v>14</v>
       </c>
       <c r="E129" t="s">
-        <v>166</v>
+        <v>290</v>
       </c>
       <c r="F129" t="s">
         <v>21</v>
@@ -7359,16 +7357,16 @@
         <v>442</v>
       </c>
       <c r="B130" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C130" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D130" t="s">
         <v>14</v>
       </c>
       <c r="E130" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F130" t="s">
         <v>21</v>
@@ -7394,16 +7392,16 @@
         <v>443</v>
       </c>
       <c r="B131" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C131" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D131" t="s">
         <v>14</v>
       </c>
       <c r="E131" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
       <c r="F131" t="s">
         <v>21</v>
@@ -7438,7 +7436,7 @@
         <v>14</v>
       </c>
       <c r="E132" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="F132" t="s">
         <v>21</v>
@@ -7508,7 +7506,7 @@
         <v>14</v>
       </c>
       <c r="E134" t="s">
-        <v>111</v>
+        <v>261</v>
       </c>
       <c r="F134" t="s">
         <v>21</v>
@@ -7543,7 +7541,7 @@
         <v>14</v>
       </c>
       <c r="E135" t="s">
-        <v>263</v>
+        <v>293</v>
       </c>
       <c r="F135" t="s">
         <v>21</v>
@@ -7561,7 +7559,7 @@
         <v>1700</v>
       </c>
       <c r="K135" t="s">
-        <v>17</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
@@ -7578,17 +7576,11 @@
         <v>14</v>
       </c>
       <c r="E136" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F136" t="s">
         <v>21</v>
       </c>
-      <c r="G136" t="s">
-        <v>16</v>
-      </c>
-      <c r="H136" t="s">
-        <v>16</v>
-      </c>
       <c r="I136">
         <v>2005</v>
       </c>
@@ -7596,7 +7588,7 @@
         <v>1700</v>
       </c>
       <c r="K136" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
@@ -7613,7 +7605,7 @@
         <v>14</v>
       </c>
       <c r="E137" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
       <c r="F137" t="s">
         <v>21</v>
@@ -7625,7 +7617,7 @@
         <v>1700</v>
       </c>
       <c r="K137" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
@@ -7642,7 +7634,7 @@
         <v>14</v>
       </c>
       <c r="E138" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F138" t="s">
         <v>21</v>
@@ -7654,7 +7646,7 @@
         <v>1700</v>
       </c>
       <c r="K138" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
@@ -7668,13 +7660,16 @@
         <v>311</v>
       </c>
       <c r="D139" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="E139" t="s">
-        <v>263</v>
+        <v>312</v>
       </c>
       <c r="F139" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="H139" t="s">
+        <v>16</v>
       </c>
       <c r="I139">
         <v>2005</v>
@@ -7683,7 +7678,7 @@
         <v>1700</v>
       </c>
       <c r="K139" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
@@ -7691,22 +7686,19 @@
         <v>517</v>
       </c>
       <c r="B140" t="s">
+        <v>313</v>
+      </c>
+      <c r="C140" t="s">
+        <v>314</v>
+      </c>
+      <c r="D140" t="s">
+        <v>14</v>
+      </c>
+      <c r="E140" t="s">
         <v>312</v>
       </c>
-      <c r="C140" t="s">
-        <v>313</v>
-      </c>
-      <c r="D140" t="s">
-        <v>179</v>
-      </c>
-      <c r="E140" t="s">
-        <v>314</v>
-      </c>
       <c r="F140" t="s">
-        <v>114</v>
-      </c>
-      <c r="H140" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I140">
         <v>2005</v>
@@ -7715,7 +7707,7 @@
         <v>1700</v>
       </c>
       <c r="K140" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
@@ -7732,10 +7724,10 @@
         <v>14</v>
       </c>
       <c r="E141" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F141" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="I141">
         <v>2005</v>
@@ -7744,7 +7736,7 @@
         <v>1700</v>
       </c>
       <c r="K141" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
@@ -7752,19 +7744,19 @@
         <v>534</v>
       </c>
       <c r="B142" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C142" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D142" t="s">
         <v>14</v>
       </c>
       <c r="E142" t="s">
-        <v>319</v>
+        <v>261</v>
       </c>
       <c r="F142" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="I142">
         <v>2005</v>
@@ -7773,7 +7765,7 @@
         <v>1700</v>
       </c>
       <c r="K142" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
@@ -7790,7 +7782,7 @@
         <v>14</v>
       </c>
       <c r="E143" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F143" t="s">
         <v>21</v>
@@ -7802,7 +7794,7 @@
         <v>1700</v>
       </c>
       <c r="K143" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
@@ -7819,7 +7811,7 @@
         <v>14</v>
       </c>
       <c r="E144" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F144" t="s">
         <v>21</v>
@@ -7831,7 +7823,7 @@
         <v>1700</v>
       </c>
       <c r="K144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
@@ -7848,7 +7840,7 @@
         <v>14</v>
       </c>
       <c r="E145" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F145" t="s">
         <v>21</v>
@@ -7860,7 +7852,7 @@
         <v>1700</v>
       </c>
       <c r="K145" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
@@ -7874,14 +7866,17 @@
         <v>327</v>
       </c>
       <c r="D146" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="E146" t="s">
-        <v>263</v>
+        <v>328</v>
       </c>
       <c r="F146" t="s">
         <v>21</v>
       </c>
+      <c r="H146" t="s">
+        <v>16</v>
+      </c>
       <c r="I146">
         <v>2005</v>
       </c>
@@ -7889,7 +7884,7 @@
         <v>1700</v>
       </c>
       <c r="K146" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
@@ -7897,23 +7892,20 @@
         <v>555</v>
       </c>
       <c r="B147" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C147" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D147" t="s">
         <v>114</v>
       </c>
       <c r="E147" t="s">
-        <v>330</v>
+        <v>261</v>
       </c>
       <c r="F147" t="s">
         <v>21</v>
       </c>
-      <c r="H147" t="s">
-        <v>16</v>
-      </c>
       <c r="I147">
         <v>2005</v>
       </c>
@@ -7921,7 +7913,7 @@
         <v>1700</v>
       </c>
       <c r="K147" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
@@ -7935,10 +7927,10 @@
         <v>332</v>
       </c>
       <c r="D148" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="E148" t="s">
-        <v>263</v>
+        <v>333</v>
       </c>
       <c r="F148" t="s">
         <v>21</v>
@@ -7950,7 +7942,7 @@
         <v>1700</v>
       </c>
       <c r="K148" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
@@ -7958,19 +7950,25 @@
         <v>564</v>
       </c>
       <c r="B149" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C149" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D149" t="s">
         <v>14</v>
       </c>
       <c r="E149" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
       <c r="F149" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="G149" t="s">
+        <v>16</v>
+      </c>
+      <c r="H149" t="s">
+        <v>16</v>
       </c>
       <c r="I149">
         <v>2005</v>
@@ -7979,7 +7977,7 @@
         <v>1700</v>
       </c>
       <c r="K149" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
@@ -7996,10 +7994,10 @@
         <v>14</v>
       </c>
       <c r="E150" t="s">
-        <v>295</v>
+        <v>111</v>
       </c>
       <c r="F150" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G150" t="s">
         <v>16</v>
@@ -8014,7 +8012,7 @@
         <v>1700</v>
       </c>
       <c r="K150" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
@@ -8028,20 +8026,14 @@
         <v>339</v>
       </c>
       <c r="D151" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E151" t="s">
-        <v>111</v>
+        <v>340</v>
       </c>
       <c r="F151" t="s">
         <v>21</v>
       </c>
-      <c r="G151" t="s">
-        <v>16</v>
-      </c>
-      <c r="H151" t="s">
-        <v>16</v>
-      </c>
       <c r="I151">
         <v>2005</v>
       </c>
@@ -8049,7 +8041,7 @@
         <v>1700</v>
       </c>
       <c r="K151" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
@@ -8057,16 +8049,16 @@
         <v>587</v>
       </c>
       <c r="B152" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C152" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D152" t="s">
         <v>153</v>
       </c>
       <c r="E152" t="s">
-        <v>342</v>
+        <v>111</v>
       </c>
       <c r="F152" t="s">
         <v>21</v>
@@ -8078,7 +8070,7 @@
         <v>1700</v>
       </c>
       <c r="K152" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
@@ -8092,14 +8084,17 @@
         <v>344</v>
       </c>
       <c r="D153" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E153" t="s">
-        <v>111</v>
+        <v>261</v>
       </c>
       <c r="F153" t="s">
         <v>21</v>
       </c>
+      <c r="H153" t="s">
+        <v>16</v>
+      </c>
       <c r="I153">
         <v>2005</v>
       </c>
@@ -8107,7 +8102,7 @@
         <v>1700</v>
       </c>
       <c r="K153" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
@@ -8121,14 +8116,17 @@
         <v>346</v>
       </c>
       <c r="D154" t="s">
-        <v>14</v>
+        <v>177</v>
       </c>
       <c r="E154" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F154" t="s">
         <v>21</v>
       </c>
+      <c r="G154" t="s">
+        <v>16</v>
+      </c>
       <c r="H154" t="s">
         <v>16</v>
       </c>
@@ -8139,7 +8137,7 @@
         <v>1700</v>
       </c>
       <c r="K154" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
@@ -8153,10 +8151,10 @@
         <v>348</v>
       </c>
       <c r="D155" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="E155" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F155" t="s">
         <v>21</v>
@@ -8174,7 +8172,7 @@
         <v>1700</v>
       </c>
       <c r="K155" t="s">
-        <v>267</v>
+        <v>17</v>
       </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
@@ -8188,10 +8186,10 @@
         <v>350</v>
       </c>
       <c r="D156" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E156" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F156" t="s">
         <v>21</v>
@@ -8226,7 +8224,7 @@
         <v>14</v>
       </c>
       <c r="E157" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F157" t="s">
         <v>21</v>
@@ -8296,7 +8294,7 @@
         <v>14</v>
       </c>
       <c r="E159" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F159" t="s">
         <v>21</v>
@@ -8331,7 +8329,7 @@
         <v>14</v>
       </c>
       <c r="E160" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F160" t="s">
         <v>21</v>
@@ -8366,7 +8364,7 @@
         <v>14</v>
       </c>
       <c r="E161" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F161" t="s">
         <v>21</v>
@@ -8401,7 +8399,7 @@
         <v>14</v>
       </c>
       <c r="E162" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F162" t="s">
         <v>21</v>
@@ -8420,6 +8418,9 @@
       </c>
       <c r="K162" t="s">
         <v>17</v>
+      </c>
+      <c r="L162" t="s">
+        <v>814</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -8436,7 +8437,7 @@
         <v>14</v>
       </c>
       <c r="E163" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F163" t="s">
         <v>21</v>
@@ -8455,9 +8456,6 @@
       </c>
       <c r="K163" t="s">
         <v>17</v>
-      </c>
-      <c r="L163" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -8474,7 +8472,7 @@
         <v>14</v>
       </c>
       <c r="E164" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F164" t="s">
         <v>21</v>
@@ -8509,7 +8507,7 @@
         <v>14</v>
       </c>
       <c r="E165" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F165" t="s">
         <v>21</v>
@@ -8544,7 +8542,7 @@
         <v>14</v>
       </c>
       <c r="E166" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F166" t="s">
         <v>21</v>
@@ -8563,6 +8561,9 @@
       </c>
       <c r="K166" t="s">
         <v>17</v>
+      </c>
+      <c r="L166" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
@@ -8579,7 +8580,7 @@
         <v>14</v>
       </c>
       <c r="E167" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F167" t="s">
         <v>21</v>
@@ -8598,9 +8599,6 @@
       </c>
       <c r="K167" t="s">
         <v>17</v>
-      </c>
-      <c r="L167" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -8617,7 +8615,7 @@
         <v>14</v>
       </c>
       <c r="E168" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F168" t="s">
         <v>21</v>
@@ -8652,7 +8650,7 @@
         <v>14</v>
       </c>
       <c r="E169" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F169" t="s">
         <v>21</v>
@@ -8671,6 +8669,9 @@
       </c>
       <c r="K169" t="s">
         <v>17</v>
+      </c>
+      <c r="L169" t="s">
+        <v>824</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
@@ -8687,7 +8688,7 @@
         <v>14</v>
       </c>
       <c r="E170" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F170" t="s">
         <v>21</v>
@@ -8706,9 +8707,6 @@
       </c>
       <c r="K170" t="s">
         <v>17</v>
-      </c>
-      <c r="L170" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
@@ -8760,7 +8758,7 @@
         <v>14</v>
       </c>
       <c r="E172" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="F172" t="s">
         <v>21</v>
@@ -8795,14 +8793,11 @@
         <v>14</v>
       </c>
       <c r="E173" t="s">
-        <v>175</v>
+        <v>111</v>
       </c>
       <c r="F173" t="s">
         <v>21</v>
       </c>
-      <c r="G173" t="s">
-        <v>16</v>
-      </c>
       <c r="H173" t="s">
         <v>16</v>
       </c>
@@ -8813,7 +8808,7 @@
         <v>1700</v>
       </c>
       <c r="K173" t="s">
-        <v>17</v>
+        <v>265</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
@@ -8830,11 +8825,14 @@
         <v>14</v>
       </c>
       <c r="E174" t="s">
-        <v>111</v>
+        <v>261</v>
       </c>
       <c r="F174" t="s">
         <v>21</v>
       </c>
+      <c r="G174" t="s">
+        <v>16</v>
+      </c>
       <c r="H174" t="s">
         <v>16</v>
       </c>
@@ -8845,7 +8843,7 @@
         <v>1700</v>
       </c>
       <c r="K174" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
@@ -8862,7 +8860,7 @@
         <v>14</v>
       </c>
       <c r="E175" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F175" t="s">
         <v>21</v>
@@ -8880,7 +8878,7 @@
         <v>1700</v>
       </c>
       <c r="K175" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
@@ -8897,14 +8895,11 @@
         <v>14</v>
       </c>
       <c r="E176" t="s">
-        <v>266</v>
+        <v>111</v>
       </c>
       <c r="F176" t="s">
         <v>21</v>
       </c>
-      <c r="G176" t="s">
-        <v>16</v>
-      </c>
       <c r="H176" t="s">
         <v>16</v>
       </c>
@@ -8915,7 +8910,7 @@
         <v>1700</v>
       </c>
       <c r="K176" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
@@ -8932,11 +8927,14 @@
         <v>14</v>
       </c>
       <c r="E177" t="s">
-        <v>111</v>
+        <v>340</v>
       </c>
       <c r="F177" t="s">
         <v>21</v>
       </c>
+      <c r="G177" t="s">
+        <v>16</v>
+      </c>
       <c r="H177" t="s">
         <v>16</v>
       </c>
@@ -8947,7 +8945,7 @@
         <v>1700</v>
       </c>
       <c r="K177" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
@@ -8964,7 +8962,7 @@
         <v>14</v>
       </c>
       <c r="E178" t="s">
-        <v>342</v>
+        <v>21</v>
       </c>
       <c r="F178" t="s">
         <v>21</v>
@@ -8982,7 +8980,7 @@
         <v>1700</v>
       </c>
       <c r="K178" t="s">
-        <v>267</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
@@ -9139,7 +9137,7 @@
         <v>14</v>
       </c>
       <c r="E183" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="F183" t="s">
         <v>21</v>
@@ -9174,7 +9172,7 @@
         <v>14</v>
       </c>
       <c r="E184" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="F184" t="s">
         <v>21</v>
@@ -9214,9 +9212,6 @@
       <c r="F185" t="s">
         <v>21</v>
       </c>
-      <c r="G185" t="s">
-        <v>16</v>
-      </c>
       <c r="H185" t="s">
         <v>16</v>
       </c>
@@ -9249,6 +9244,9 @@
       <c r="F186" t="s">
         <v>21</v>
       </c>
+      <c r="G186" t="s">
+        <v>16</v>
+      </c>
       <c r="H186" t="s">
         <v>16</v>
       </c>
@@ -9381,7 +9379,7 @@
         <v>14</v>
       </c>
       <c r="E190" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F190" t="s">
         <v>21</v>
@@ -9416,7 +9414,7 @@
         <v>14</v>
       </c>
       <c r="E191" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F191" t="s">
         <v>21</v>
@@ -9486,7 +9484,7 @@
         <v>14</v>
       </c>
       <c r="E193" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F193" t="s">
         <v>21</v>
@@ -9521,7 +9519,7 @@
         <v>14</v>
       </c>
       <c r="E194" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F194" t="s">
         <v>21</v>
@@ -9556,7 +9554,7 @@
         <v>14</v>
       </c>
       <c r="E195" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F195" t="s">
         <v>21</v>
@@ -9591,7 +9589,7 @@
         <v>14</v>
       </c>
       <c r="E196" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F196" t="s">
         <v>21</v>
@@ -9626,7 +9624,7 @@
         <v>14</v>
       </c>
       <c r="E197" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F197" t="s">
         <v>21</v>
@@ -9661,7 +9659,7 @@
         <v>14</v>
       </c>
       <c r="E198" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F198" t="s">
         <v>21</v>
@@ -9839,7 +9837,7 @@
         <v>21</v>
       </c>
       <c r="F203" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G203" t="s">
         <v>16</v>
@@ -9874,7 +9872,7 @@
         <v>21</v>
       </c>
       <c r="F204" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G204" t="s">
         <v>16</v>
@@ -9906,7 +9904,7 @@
         <v>14</v>
       </c>
       <c r="E205" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F205" t="s">
         <v>21</v>
@@ -9941,7 +9939,7 @@
         <v>14</v>
       </c>
       <c r="E206" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F206" t="s">
         <v>21</v>
@@ -9976,7 +9974,7 @@
         <v>14</v>
       </c>
       <c r="E207" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F207" t="s">
         <v>21</v>
@@ -10011,7 +10009,7 @@
         <v>14</v>
       </c>
       <c r="E208" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F208" t="s">
         <v>21</v>
@@ -10046,7 +10044,7 @@
         <v>14</v>
       </c>
       <c r="E209" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F209" t="s">
         <v>21</v>
@@ -10081,7 +10079,7 @@
         <v>14</v>
       </c>
       <c r="E210" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F210" t="s">
         <v>21</v>
@@ -10116,7 +10114,7 @@
         <v>14</v>
       </c>
       <c r="E211" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F211" t="s">
         <v>21</v>
@@ -10151,7 +10149,7 @@
         <v>14</v>
       </c>
       <c r="E212" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F212" t="s">
         <v>21</v>
@@ -10226,9 +10224,6 @@
       <c r="F214" t="s">
         <v>21</v>
       </c>
-      <c r="G214" t="s">
-        <v>16</v>
-      </c>
       <c r="H214" t="s">
         <v>16</v>
       </c>
@@ -10256,10 +10251,13 @@
         <v>14</v>
       </c>
       <c r="E215" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F215" t="s">
         <v>21</v>
+      </c>
+      <c r="G215" t="s">
+        <v>16</v>
       </c>
       <c r="H215" t="s">
         <v>16</v>
@@ -10288,7 +10286,7 @@
         <v>14</v>
       </c>
       <c r="E216" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F216" t="s">
         <v>21</v>
@@ -10501,7 +10499,7 @@
         <v>21</v>
       </c>
       <c r="F222" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G222" t="s">
         <v>16</v>
@@ -10536,7 +10534,7 @@
         <v>21</v>
       </c>
       <c r="F223" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G223" t="s">
         <v>16</v>
@@ -10950,16 +10948,13 @@
         <v>508</v>
       </c>
       <c r="D235" t="s">
-        <v>14</v>
+        <v>509</v>
       </c>
       <c r="E235" t="s">
-        <v>21</v>
+        <v>510</v>
       </c>
       <c r="F235" t="s">
-        <v>21</v>
-      </c>
-      <c r="G235" t="s">
-        <v>16</v>
+        <v>177</v>
       </c>
       <c r="H235" t="s">
         <v>16</v>
@@ -10979,19 +10974,22 @@
         <v>914</v>
       </c>
       <c r="B236" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C236" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D236" t="s">
-        <v>511</v>
+        <v>14</v>
       </c>
       <c r="E236" t="s">
-        <v>512</v>
+        <v>21</v>
       </c>
       <c r="F236" t="s">
-        <v>179</v>
+        <v>21</v>
+      </c>
+      <c r="G236" t="s">
+        <v>16</v>
       </c>
       <c r="H236" t="s">
         <v>16</v>
@@ -11160,7 +11158,7 @@
         <v>14</v>
       </c>
       <c r="E241" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F241" t="s">
         <v>21</v>
@@ -11195,7 +11193,7 @@
         <v>14</v>
       </c>
       <c r="E242" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F242" t="s">
         <v>21</v>
@@ -11375,9 +11373,6 @@
       <c r="F247" t="s">
         <v>21</v>
       </c>
-      <c r="G247" t="s">
-        <v>16</v>
-      </c>
       <c r="H247" t="s">
         <v>16</v>
       </c>
@@ -11410,6 +11405,9 @@
       <c r="F248" t="s">
         <v>21</v>
       </c>
+      <c r="G248" t="s">
+        <v>16</v>
+      </c>
       <c r="H248" t="s">
         <v>16</v>
       </c>
@@ -11574,13 +11572,13 @@
         <v>546</v>
       </c>
       <c r="D253" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="E253" t="s">
-        <v>21</v>
+        <v>254</v>
       </c>
       <c r="F253" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G253" t="s">
         <v>16</v>
@@ -11609,13 +11607,13 @@
         <v>548</v>
       </c>
       <c r="D254" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="E254" t="s">
-        <v>256</v>
+        <v>21</v>
       </c>
       <c r="F254" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G254" t="s">
         <v>16</v>
@@ -12134,13 +12132,13 @@
         <v>578</v>
       </c>
       <c r="D269" t="s">
-        <v>14</v>
+        <v>509</v>
       </c>
       <c r="E269" t="s">
-        <v>21</v>
+        <v>579</v>
       </c>
       <c r="F269" t="s">
-        <v>21</v>
+        <v>177</v>
       </c>
       <c r="G269" t="s">
         <v>16</v>
@@ -12163,19 +12161,19 @@
         <v>1214</v>
       </c>
       <c r="B270" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C270" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="D270" t="s">
-        <v>511</v>
+        <v>14</v>
       </c>
       <c r="E270" t="s">
-        <v>581</v>
+        <v>21</v>
       </c>
       <c r="F270" t="s">
-        <v>179</v>
+        <v>21</v>
       </c>
       <c r="G270" t="s">
         <v>16</v>
@@ -12717,6 +12715,9 @@
       <c r="K285" t="s">
         <v>17</v>
       </c>
+      <c r="L285" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286">
@@ -12752,9 +12753,6 @@
       <c r="K286" t="s">
         <v>17</v>
       </c>
-      <c r="L286" t="s">
-        <v>815</v>
-      </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287">
@@ -13055,9 +13053,6 @@
       <c r="F295" t="s">
         <v>21</v>
       </c>
-      <c r="G295" t="s">
-        <v>16</v>
-      </c>
       <c r="H295" t="s">
         <v>16</v>
       </c>
@@ -13090,6 +13085,9 @@
       <c r="F296" t="s">
         <v>21</v>
       </c>
+      <c r="G296" t="s">
+        <v>16</v>
+      </c>
       <c r="H296" t="s">
         <v>16</v>
       </c>
@@ -13117,7 +13115,7 @@
         <v>14</v>
       </c>
       <c r="E297" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F297" t="s">
         <v>21</v>
@@ -13152,7 +13150,7 @@
         <v>14</v>
       </c>
       <c r="E298" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F298" t="s">
         <v>21</v>
@@ -13187,7 +13185,7 @@
         <v>14</v>
       </c>
       <c r="E299" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F299" t="s">
         <v>21</v>
@@ -13222,7 +13220,7 @@
         <v>14</v>
       </c>
       <c r="E300" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F300" t="s">
         <v>21</v>
@@ -13893,7 +13891,7 @@
         <v>21</v>
       </c>
       <c r="G319" t="s">
-        <v>16</v>
+        <v>680</v>
       </c>
       <c r="H319" t="s">
         <v>16</v>
@@ -13913,10 +13911,10 @@
         <v>1622</v>
       </c>
       <c r="B320" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C320" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D320" t="s">
         <v>14</v>
@@ -13928,7 +13926,7 @@
         <v>21</v>
       </c>
       <c r="G320" t="s">
-        <v>682</v>
+        <v>16</v>
       </c>
       <c r="H320" t="s">
         <v>16</v>
@@ -13957,7 +13955,7 @@
         <v>14</v>
       </c>
       <c r="E321" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F321" t="s">
         <v>21</v>
@@ -13992,7 +13990,7 @@
         <v>14</v>
       </c>
       <c r="E322" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F322" t="s">
         <v>21</v>
@@ -14027,7 +14025,7 @@
         <v>14</v>
       </c>
       <c r="E323" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="F323" t="s">
         <v>21</v>
@@ -14062,7 +14060,7 @@
         <v>14</v>
       </c>
       <c r="E324" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="F324" t="s">
         <v>21</v>
@@ -14137,9 +14135,6 @@
       <c r="F326" t="s">
         <v>21</v>
       </c>
-      <c r="G326" t="s">
-        <v>16</v>
-      </c>
       <c r="H326" t="s">
         <v>16</v>
       </c>
@@ -14172,6 +14167,9 @@
       <c r="F327" t="s">
         <v>21</v>
       </c>
+      <c r="G327" t="s">
+        <v>16</v>
+      </c>
       <c r="H327" t="s">
         <v>16</v>
       </c>
@@ -14199,7 +14197,7 @@
         <v>14</v>
       </c>
       <c r="E328" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="F328" t="s">
         <v>21</v>
@@ -14234,7 +14232,7 @@
         <v>14</v>
       </c>
       <c r="E329" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="F329" t="s">
         <v>21</v>
@@ -14304,7 +14302,7 @@
         <v>14</v>
       </c>
       <c r="E331" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F331" t="s">
         <v>21</v>
@@ -14339,7 +14337,7 @@
         <v>14</v>
       </c>
       <c r="E332" t="s">
-        <v>263</v>
+        <v>173</v>
       </c>
       <c r="F332" t="s">
         <v>21</v>
@@ -14374,7 +14372,7 @@
         <v>14</v>
       </c>
       <c r="E333" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="F333" t="s">
         <v>21</v>
@@ -14409,7 +14407,7 @@
         <v>14</v>
       </c>
       <c r="E334" t="s">
-        <v>21</v>
+        <v>173</v>
       </c>
       <c r="F334" t="s">
         <v>21</v>
@@ -14444,7 +14442,7 @@
         <v>14</v>
       </c>
       <c r="E335" t="s">
-        <v>175</v>
+        <v>21</v>
       </c>
       <c r="F335" t="s">
         <v>21</v>
@@ -14639,6 +14637,9 @@
       <c r="K340" t="s">
         <v>17</v>
       </c>
+      <c r="L340" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341">
@@ -14674,9 +14675,6 @@
       <c r="K341" t="s">
         <v>17</v>
       </c>
-      <c r="L341" t="s">
-        <v>822</v>
-      </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342">
@@ -14852,6 +14850,9 @@
       <c r="K346" t="s">
         <v>17</v>
       </c>
+      <c r="L346" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347">
@@ -14888,7 +14889,7 @@
         <v>17</v>
       </c>
       <c r="L347" t="s">
-        <v>829</v>
+        <v>819</v>
       </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
@@ -14925,9 +14926,6 @@
       <c r="K348" t="s">
         <v>17</v>
       </c>
-      <c r="L348" t="s">
-        <v>821</v>
-      </c>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349">
@@ -15048,7 +15046,7 @@
         <v>14</v>
       </c>
       <c r="E352" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F352" t="s">
         <v>21</v>
@@ -15083,7 +15081,7 @@
         <v>14</v>
       </c>
       <c r="E353" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="F353" t="s">
         <v>21</v>
@@ -15118,13 +15116,10 @@
         <v>14</v>
       </c>
       <c r="E354" t="s">
-        <v>111</v>
+        <v>261</v>
       </c>
       <c r="F354" t="s">
         <v>21</v>
-      </c>
-      <c r="G354" t="s">
-        <v>16</v>
       </c>
       <c r="H354" t="s">
         <v>16</v>
@@ -15153,10 +15148,13 @@
         <v>14</v>
       </c>
       <c r="E355" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F355" t="s">
         <v>21</v>
+      </c>
+      <c r="G355" t="s">
+        <v>16</v>
       </c>
       <c r="H355" t="s">
         <v>16</v>
@@ -15430,7 +15428,7 @@
         <v>14</v>
       </c>
       <c r="E363" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F363" t="s">
         <v>21</v>
@@ -15465,13 +15463,10 @@
         <v>14</v>
       </c>
       <c r="E364" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F364" t="s">
         <v>21</v>
-      </c>
-      <c r="G364" t="s">
-        <v>16</v>
       </c>
       <c r="H364" t="s">
         <v>16</v>
@@ -15505,6 +15500,9 @@
       <c r="F365" t="s">
         <v>21</v>
       </c>
+      <c r="G365" t="s">
+        <v>16</v>
+      </c>
       <c r="H365" t="s">
         <v>16</v>
       </c>
@@ -15532,7 +15530,7 @@
         <v>14</v>
       </c>
       <c r="E366" t="s">
-        <v>21</v>
+        <v>261</v>
       </c>
       <c r="F366" t="s">
         <v>21</v>
@@ -15567,7 +15565,7 @@
         <v>14</v>
       </c>
       <c r="E367" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F367" t="s">
         <v>21</v>
@@ -15586,6 +15584,9 @@
       </c>
       <c r="K367" t="s">
         <v>17</v>
+      </c>
+      <c r="L367" t="s">
+        <v>823</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
@@ -15602,7 +15603,7 @@
         <v>14</v>
       </c>
       <c r="E368" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F368" t="s">
         <v>21</v>
@@ -15621,9 +15622,6 @@
       </c>
       <c r="K368" t="s">
         <v>17</v>
-      </c>
-      <c r="L368" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
@@ -15640,7 +15638,7 @@
         <v>14</v>
       </c>
       <c r="E369" t="s">
-        <v>263</v>
+        <v>21</v>
       </c>
       <c r="F369" t="s">
         <v>21</v>
@@ -15748,7 +15746,7 @@
         <v>21</v>
       </c>
       <c r="F372" t="s">
-        <v>21</v>
+        <v>787</v>
       </c>
       <c r="G372" t="s">
         <v>16</v>
@@ -15771,10 +15769,10 @@
         <v>1966</v>
       </c>
       <c r="B373" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="C373" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="D373" t="s">
         <v>14</v>
@@ -15783,7 +15781,7 @@
         <v>21</v>
       </c>
       <c r="F373" t="s">
-        <v>789</v>
+        <v>21</v>
       </c>
       <c r="G373" t="s">
         <v>16</v>
@@ -15844,7 +15842,7 @@
         <v>792</v>
       </c>
       <c r="C375" t="s">
-        <v>793</v>
+        <v>478</v>
       </c>
       <c r="D375" t="s">
         <v>14</v>
@@ -15876,10 +15874,10 @@
         <v>11100</v>
       </c>
       <c r="B376" t="s">
+        <v>793</v>
+      </c>
+      <c r="C376" t="s">
         <v>794</v>
-      </c>
-      <c r="C376" t="s">
-        <v>480</v>
       </c>
       <c r="D376" t="s">
         <v>14</v>
@@ -16030,9 +16028,6 @@
       <c r="F380" t="s">
         <v>21</v>
       </c>
-      <c r="G380" t="s">
-        <v>16</v>
-      </c>
       <c r="H380" t="s">
         <v>16</v>
       </c>
@@ -16065,6 +16060,9 @@
       <c r="F381" t="s">
         <v>21</v>
       </c>
+      <c r="G381" t="s">
+        <v>16</v>
+      </c>
       <c r="H381" t="s">
         <v>16</v>
       </c>
@@ -16183,39 +16181,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>11550</v>
-      </c>
-      <c r="B385" t="s">
-        <v>811</v>
-      </c>
-      <c r="C385" t="s">
-        <v>812</v>
-      </c>
-      <c r="D385" t="s">
-        <v>14</v>
-      </c>
-      <c r="E385" t="s">
-        <v>21</v>
-      </c>
-      <c r="F385" t="s">
-        <v>21</v>
-      </c>
-      <c r="G385" t="s">
-        <v>16</v>
-      </c>
-      <c r="H385" t="s">
-        <v>16</v>
-      </c>
-      <c r="I385">
-        <v>2005</v>
-      </c>
-      <c r="J385">
-        <v>1700</v>
-      </c>
-      <c r="K385" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix end row in species list
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0B3378D-9F91-4F5C-BE3D-6CEB4FDD5469}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{888B0FFE-488B-479B-8610-592EE3C0CE7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2849,10 +2849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L385"/>
+  <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A385" sqref="A385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16181,11 +16181,6 @@
         <v>17</v>
       </c>
     </row>
-    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A385">
-        <v>11550</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Adjust map field to fix build
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{888B0FFE-488B-479B-8610-592EE3C0CE7B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="836">
   <si>
     <t>species_order</t>
   </si>
@@ -2538,7 +2537,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2848,11 +2847,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A385" sqref="A385"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3111,8 +3110,8 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="H7">
-        <v>6</v>
+      <c r="H7" t="s">
+        <v>16</v>
       </c>
       <c r="I7">
         <v>2005</v>
@@ -3324,8 +3323,8 @@
       <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="H13">
-        <v>6</v>
+      <c r="H13" t="s">
+        <v>16</v>
       </c>
       <c r="I13">
         <v>2005</v>
@@ -3359,8 +3358,8 @@
       <c r="F14" t="s">
         <v>21</v>
       </c>
-      <c r="H14">
-        <v>6</v>
+      <c r="H14" t="s">
+        <v>16</v>
       </c>
       <c r="I14">
         <v>2005</v>
@@ -3502,8 +3501,8 @@
       <c r="F18" t="s">
         <v>21</v>
       </c>
-      <c r="H18">
-        <v>6</v>
+      <c r="H18" t="s">
+        <v>16</v>
       </c>
       <c r="I18">
         <v>2005</v>
@@ -3642,8 +3641,8 @@
       <c r="G22" t="s">
         <v>835</v>
       </c>
-      <c r="H22">
-        <v>6</v>
+      <c r="H22" t="s">
+        <v>16</v>
       </c>
       <c r="I22">
         <v>2005</v>
@@ -3954,8 +3953,8 @@
       <c r="F31" t="s">
         <v>21</v>
       </c>
-      <c r="H31">
-        <v>6</v>
+      <c r="H31" t="s">
+        <v>16</v>
       </c>
       <c r="I31">
         <v>2005</v>
@@ -4126,8 +4125,8 @@
       <c r="F36" t="s">
         <v>21</v>
       </c>
-      <c r="H36">
-        <v>6</v>
+      <c r="H36" t="s">
+        <v>16</v>
       </c>
       <c r="I36">
         <v>2005</v>
@@ -4756,8 +4755,8 @@
       <c r="F54" t="s">
         <v>21</v>
       </c>
-      <c r="H54">
-        <v>6</v>
+      <c r="H54" t="s">
+        <v>16</v>
       </c>
       <c r="I54">
         <v>2005</v>
@@ -4893,8 +4892,8 @@
       <c r="F58" t="s">
         <v>21</v>
       </c>
-      <c r="H58">
-        <v>6</v>
+      <c r="H58" t="s">
+        <v>16</v>
       </c>
       <c r="I58">
         <v>2005</v>
@@ -5103,8 +5102,8 @@
       <c r="F64" t="s">
         <v>21</v>
       </c>
-      <c r="H64">
-        <v>6</v>
+      <c r="H64" t="s">
+        <v>16</v>
       </c>
       <c r="I64">
         <v>2005</v>
@@ -5278,8 +5277,8 @@
       <c r="F69" t="s">
         <v>21</v>
       </c>
-      <c r="H69">
-        <v>6</v>
+      <c r="H69" t="s">
+        <v>16</v>
       </c>
       <c r="I69">
         <v>2005</v>
@@ -5803,8 +5802,8 @@
       <c r="F84" t="s">
         <v>114</v>
       </c>
-      <c r="H84">
-        <v>6</v>
+      <c r="H84" t="s">
+        <v>16</v>
       </c>
       <c r="I84">
         <v>2005</v>
@@ -5908,8 +5907,8 @@
       <c r="F87" t="s">
         <v>21</v>
       </c>
-      <c r="H87">
-        <v>6</v>
+      <c r="H87" t="s">
+        <v>16</v>
       </c>
       <c r="I87">
         <v>2005</v>
@@ -6296,8 +6295,8 @@
       <c r="F98" t="s">
         <v>21</v>
       </c>
-      <c r="H98">
-        <v>6</v>
+      <c r="H98" t="s">
+        <v>16</v>
       </c>
       <c r="I98">
         <v>2005</v>
@@ -6398,8 +6397,8 @@
       <c r="G101" t="s">
         <v>835</v>
       </c>
-      <c r="H101">
-        <v>6</v>
+      <c r="H101" t="s">
+        <v>16</v>
       </c>
       <c r="I101">
         <v>2005</v>
@@ -6430,8 +6429,8 @@
       <c r="F102" t="s">
         <v>21</v>
       </c>
-      <c r="H102">
-        <v>6</v>
+      <c r="H102" t="s">
+        <v>16</v>
       </c>
       <c r="I102">
         <v>2005</v>
@@ -6602,8 +6601,8 @@
       <c r="F107" t="s">
         <v>21</v>
       </c>
-      <c r="H107">
-        <v>6</v>
+      <c r="H107" t="s">
+        <v>16</v>
       </c>
       <c r="I107">
         <v>2005</v>
@@ -6634,8 +6633,8 @@
       <c r="F108" t="s">
         <v>21</v>
       </c>
-      <c r="H108">
-        <v>6</v>
+      <c r="H108" t="s">
+        <v>16</v>
       </c>
       <c r="I108">
         <v>2005</v>

</xml_diff>

<commit_message>
Added some profile image links
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3043" uniqueCount="847">
   <si>
     <t>species_order</t>
   </si>
@@ -2532,6 +2532,39 @@
   </si>
   <si>
     <t>3_6</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1905/45055136544_f0c9da9688_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4905/45055137744_3958182c8e_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4889/45729776412_7afe946f98_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4881/45055142214_663d8fa110_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1967/45729763972_428499f54f_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4850/45055131014_8d032f5775_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4861/45729766702_157f300a29_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4905/45055134774_2ca1b1cc23_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1925/45055135844_d170ae8d49_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4860/45729769952_fb28cb236b_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4878/45055143344_21583d31e5_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2850,9 +2883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3447,7 +3478,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3481,8 +3512,11 @@
       <c r="K17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3514,7 +3548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3549,7 +3583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64</v>
       </c>
@@ -3584,7 +3618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>76</v>
       </c>
@@ -3619,7 +3653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>78</v>
       </c>
@@ -3654,7 +3688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>79</v>
       </c>
@@ -3689,7 +3723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -3724,7 +3758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
@@ -3758,8 +3792,11 @@
       <c r="K25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>91</v>
       </c>
@@ -3793,8 +3830,11 @@
       <c r="K26" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>96</v>
       </c>
@@ -3828,8 +3868,11 @@
       <c r="K27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -3864,7 +3907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>115</v>
       </c>
@@ -3898,8 +3941,11 @@
       <c r="K29" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>120</v>
       </c>
@@ -3933,8 +3979,11 @@
       <c r="K30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>123</v>
       </c>
@@ -3965,8 +4014,11 @@
       <c r="K31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4070,6 +4122,9 @@
       <c r="K34" t="s">
         <v>17</v>
       </c>
+      <c r="L34" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -4172,6 +4227,9 @@
       <c r="K37" t="s">
         <v>17</v>
       </c>
+      <c r="L37" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -4242,6 +4300,9 @@
       <c r="K39" t="s">
         <v>17</v>
       </c>
+      <c r="L39" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -4311,6 +4372,9 @@
       </c>
       <c r="K41" t="s">
         <v>17</v>
+      </c>
+      <c r="L41" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add golden whistler image
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7AE816C-C939-4D62-AA72-1B131230C1F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3043" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="848">
   <si>
     <t>species_order</t>
   </si>
@@ -2565,12 +2566,15 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4878/45055143344_21583d31e5_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4865/31933987778_eb8a8ec938_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2880,24 +2884,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625"/>
-    <col min="2" max="2" width="46.453125"/>
-    <col min="3" max="3" width="38.08984375"/>
-    <col min="4" max="4" width="26.08984375"/>
-    <col min="5" max="5" width="105.1796875"/>
-    <col min="6" max="6" width="40.81640625"/>
-    <col min="7" max="8" width="17.08984375"/>
-    <col min="9" max="9" width="28.81640625"/>
-    <col min="10" max="10" width="26.453125"/>
-    <col min="11" max="11" width="14.08984375"/>
-    <col min="12" max="1025" width="9.453125"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="59.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="9.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -12887,7 +12894,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1394</v>
       </c>
@@ -12922,7 +12929,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1398</v>
       </c>
@@ -12957,7 +12964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1411</v>
       </c>
@@ -12992,7 +12999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1424</v>
       </c>
@@ -13027,7 +13034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1430</v>
       </c>
@@ -13062,7 +13069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1434</v>
       </c>
@@ -13097,7 +13104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1444</v>
       </c>
@@ -13129,7 +13136,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1450</v>
       </c>
@@ -13164,7 +13171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1451</v>
       </c>
@@ -13199,7 +13206,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1453</v>
       </c>
@@ -13234,7 +13241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1457</v>
       </c>
@@ -13269,7 +13276,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1463</v>
       </c>
@@ -13304,7 +13311,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1466</v>
       </c>
@@ -13339,7 +13346,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1469</v>
       </c>
@@ -13374,7 +13381,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1474</v>
       </c>
@@ -13409,7 +13416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>1500</v>
       </c>
@@ -13442,6 +13449,9 @@
       </c>
       <c r="K304" t="s">
         <v>17</v>
+      </c>
+      <c r="L304" t="s">
+        <v>847</v>
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 5 species image links
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7AE816C-C939-4D62-AA72-1B131230C1F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A21C1E22-322B-424B-AC0C-F1D4D83C6D77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3044" uniqueCount="848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3049" uniqueCount="853">
   <si>
     <t>species_order</t>
   </si>
@@ -2569,6 +2569,21 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4865/31933987778_eb8a8ec938_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4877/45804873881_4fb0d70105_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4803/31934053238_2319e70998_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4806/44892069075_f7dc4b022e_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4806/45804865371_a7c91623c2_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4833/30865310147_47f78e9421_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2887,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4523,6 +4538,9 @@
       <c r="K45" t="s">
         <v>17</v>
       </c>
+      <c r="L45" t="s">
+        <v>852</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -7896,7 +7914,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>547</v>
       </c>
@@ -7925,7 +7943,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>548</v>
       </c>
@@ -7957,7 +7975,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>555</v>
       </c>
@@ -7986,7 +8004,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>563</v>
       </c>
@@ -8015,7 +8033,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>564</v>
       </c>
@@ -8050,7 +8068,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>582</v>
       </c>
@@ -8085,7 +8103,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>584</v>
       </c>
@@ -8114,7 +8132,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>587</v>
       </c>
@@ -8143,7 +8161,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>589</v>
       </c>
@@ -8175,7 +8193,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>590</v>
       </c>
@@ -8210,7 +8228,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>591</v>
       </c>
@@ -8245,7 +8263,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>611</v>
       </c>
@@ -8279,8 +8297,11 @@
       <c r="K156" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L156" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>613</v>
       </c>
@@ -8315,7 +8336,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>615</v>
       </c>
@@ -8350,7 +8371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>619</v>
       </c>
@@ -8385,7 +8406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>627</v>
       </c>
@@ -13454,7 +13475,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1509</v>
       </c>
@@ -13489,7 +13510,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1520</v>
       </c>
@@ -13524,7 +13545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1529</v>
       </c>
@@ -13559,7 +13580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1536</v>
       </c>
@@ -13594,7 +13615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>1543</v>
       </c>
@@ -13629,7 +13650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>1553</v>
       </c>
@@ -13664,7 +13685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>1557</v>
       </c>
@@ -13699,7 +13720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>1573</v>
       </c>
@@ -13734,7 +13755,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>1592</v>
       </c>
@@ -13768,8 +13789,11 @@
       <c r="K313" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L313" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1601</v>
       </c>
@@ -13804,7 +13828,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>1604</v>
       </c>
@@ -13839,7 +13863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>1612</v>
       </c>
@@ -13874,7 +13898,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>1613</v>
       </c>
@@ -13909,7 +13933,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1614</v>
       </c>
@@ -13944,7 +13968,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>1617</v>
       </c>
@@ -13979,7 +14003,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1622</v>
       </c>
@@ -14014,7 +14038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>1625</v>
       </c>
@@ -14049,7 +14073,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1627</v>
       </c>
@@ -14084,7 +14108,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>1635</v>
       </c>
@@ -14119,7 +14143,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1639</v>
       </c>
@@ -14153,8 +14177,11 @@
       <c r="K324" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L324" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1644</v>
       </c>
@@ -14189,7 +14216,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>1656</v>
       </c>
@@ -14221,7 +14248,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>1664</v>
       </c>
@@ -14256,7 +14283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>1669</v>
       </c>
@@ -14291,7 +14318,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>1677</v>
       </c>
@@ -14326,7 +14353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1678</v>
       </c>
@@ -14361,7 +14388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>1681</v>
       </c>
@@ -14396,7 +14423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1689</v>
       </c>
@@ -14431,7 +14458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1692</v>
       </c>
@@ -14466,7 +14493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>1696</v>
       </c>
@@ -14501,7 +14528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1701</v>
       </c>
@@ -14536,7 +14563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>1705</v>
       </c>
@@ -14604,6 +14631,9 @@
       </c>
       <c r="K337" t="s">
         <v>17</v>
+      </c>
+      <c r="L337" t="s">
+        <v>850</v>
       </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add 5 more images to species list
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A21C1E22-322B-424B-AC0C-F1D4D83C6D77}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{915F3F54-13D9-4628-92E7-2E950B5B2502}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3049" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="858">
   <si>
     <t>species_order</t>
   </si>
@@ -2584,6 +2584,21 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4833/30865310147_47f78e9421_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4906/43990773760_8dd63615e9_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4819/43990773190_8d5ba5d1b0_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4889/43990772210_de90e643fd_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4807/43990772850_662f6350c8_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4879/44894529005_1493d275c4_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2902,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="C52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5521,6 +5536,9 @@
       <c r="K73" t="s">
         <v>17</v>
       </c>
+      <c r="L73" t="s">
+        <v>857</v>
+      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -7405,7 +7423,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>434</v>
       </c>
@@ -7440,7 +7458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>442</v>
       </c>
@@ -7475,7 +7493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>443</v>
       </c>
@@ -7510,7 +7528,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>444</v>
       </c>
@@ -7545,7 +7563,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>446</v>
       </c>
@@ -7580,7 +7598,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>456</v>
       </c>
@@ -7615,7 +7633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>463</v>
       </c>
@@ -7649,8 +7667,11 @@
       <c r="K135" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L135" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>465</v>
       </c>
@@ -7679,7 +7700,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>493</v>
       </c>
@@ -7708,7 +7729,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>497</v>
       </c>
@@ -7737,7 +7758,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>501</v>
       </c>
@@ -7769,7 +7790,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>517</v>
       </c>
@@ -7798,7 +7819,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>519</v>
       </c>
@@ -7827,7 +7848,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>534</v>
       </c>
@@ -7856,7 +7877,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>535</v>
       </c>
@@ -7885,7 +7906,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>537</v>
       </c>
@@ -10678,7 +10699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>838</v>
       </c>
@@ -10713,7 +10734,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>842</v>
       </c>
@@ -10748,7 +10769,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>845</v>
       </c>
@@ -10783,7 +10804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>849</v>
       </c>
@@ -10817,8 +10838,11 @@
       <c r="K228" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L228" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>853</v>
       </c>
@@ -10853,7 +10877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>861</v>
       </c>
@@ -10888,7 +10912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>864</v>
       </c>
@@ -10923,7 +10947,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>871</v>
       </c>
@@ -10958,7 +10982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>887</v>
       </c>
@@ -10993,7 +11017,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>898</v>
       </c>
@@ -11028,7 +11052,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>901</v>
       </c>
@@ -11060,7 +11084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>914</v>
       </c>
@@ -11095,7 +11119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>933</v>
       </c>
@@ -11130,7 +11154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>935</v>
       </c>
@@ -11165,7 +11189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>938</v>
       </c>
@@ -11200,7 +11224,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>943</v>
       </c>
@@ -14107,6 +14131,9 @@
       <c r="K322" t="s">
         <v>17</v>
       </c>
+      <c r="L322" t="s">
+        <v>854</v>
+      </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A323">
@@ -15617,6 +15644,9 @@
       </c>
       <c r="K365" t="s">
         <v>17</v>
+      </c>
+      <c r="L365" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added yellow-rumped thornbill pic
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3053" uniqueCount="858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="859">
   <si>
     <t>species_order</t>
   </si>
@@ -2598,6 +2598,9 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4879/44894529005_1493d275c4_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4838/44090300790_5c07f9ee01_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2916,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="D269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L287" sqref="L287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -12902,6 +12905,9 @@
       <c r="K287" t="s">
         <v>17</v>
       </c>
+      <c r="L287" t="s">
+        <v>858</v>
+      </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288">

</xml_diff>

<commit_message>
change YRTB photo and start on STTB
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{03E885A6-84E0-4C23-8AEE-AC9793339DF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -2600,13 +2601,13 @@
     <t>https://c1.staticflickr.com/5/4879/44894529005_1493d275c4_b_d.jpg</t>
   </si>
   <si>
-    <t>https://c1.staticflickr.com/5/4838/44090300790_5c07f9ee01_b_d.jpg</t>
+    <t>https://c1.staticflickr.com/5/4838/44090300790_af0d27d9ba_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2916,10 +2917,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L287" sqref="L287"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
try using jpg for magpie goose (#98)
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{03E885A6-84E0-4C23-8AEE-AC9793339DF6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="838">
   <si>
     <t>species_order</t>
   </si>
@@ -534,6 +533,12 @@
     <t>Pacific Golden Plover</t>
   </si>
   <si>
+    <t>Pluvialis dominica</t>
+  </si>
+  <si>
+    <t>American Golden Plover</t>
+  </si>
+  <si>
     <t>Charadrius ruficapillus</t>
   </si>
   <si>
@@ -2533,81 +2538,12 @@
   </si>
   <si>
     <t>3_6</t>
-  </si>
-  <si>
-    <t>https://c2.staticflickr.com/2/1905/45055136544_f0c9da9688_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4905/45055137744_3958182c8e_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4889/45729776412_7afe946f98_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4881/45055142214_663d8fa110_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c2.staticflickr.com/2/1967/45729763972_428499f54f_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4850/45055131014_8d032f5775_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4861/45729766702_157f300a29_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4905/45055134774_2ca1b1cc23_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c2.staticflickr.com/2/1925/45055135844_d170ae8d49_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4860/45729769952_fb28cb236b_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4878/45055143344_21583d31e5_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4865/31933987778_eb8a8ec938_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4877/45804873881_4fb0d70105_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4803/31934053238_2319e70998_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4806/44892069075_f7dc4b022e_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4806/45804865371_a7c91623c2_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4833/30865310147_47f78e9421_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4906/43990773760_8dd63615e9_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4819/43990773190_8d5ba5d1b0_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4889/43990772210_de90e643fd_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4807/43990772850_662f6350c8_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4879/44894529005_1493d275c4_b_d.jpg</t>
-  </si>
-  <si>
-    <t>https://c1.staticflickr.com/5/4838/44090300790_af0d27d9ba_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2917,27 +2853,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L384"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C269" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L287" sqref="L287"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.54296875" customWidth="1"/>
-    <col min="6" max="6" width="16.08984375" customWidth="1"/>
-    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="59.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="9.453125"/>
+    <col min="1" max="1" width="17.7265625"/>
+    <col min="2" max="2" width="46.453125"/>
+    <col min="3" max="3" width="38.08984375"/>
+    <col min="4" max="4" width="26.08984375"/>
+    <col min="5" max="5" width="105.1796875"/>
+    <col min="6" max="6" width="40.81640625"/>
+    <col min="7" max="8" width="17.08984375"/>
+    <col min="9" max="9" width="28.81640625"/>
+    <col min="10" max="10" width="26.453125"/>
+    <col min="11" max="11" width="14.08984375"/>
+    <col min="12" max="1025" width="9.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3051,7 +2986,7 @@
         <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3089,7 +3024,7 @@
         <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3167,7 +3102,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -3194,7 +3129,7 @@
         <v>17</v>
       </c>
       <c r="L7" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3302,7 +3237,7 @@
         <v>17</v>
       </c>
       <c r="L10" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3394,8 +3329,8 @@
       <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="H13" t="s">
-        <v>16</v>
+      <c r="H13">
+        <v>6</v>
       </c>
       <c r="I13">
         <v>2005</v>
@@ -3407,7 +3342,7 @@
         <v>17</v>
       </c>
       <c r="L13" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3429,8 +3364,8 @@
       <c r="F14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" t="s">
-        <v>16</v>
+      <c r="H14">
+        <v>6</v>
       </c>
       <c r="I14">
         <v>2005</v>
@@ -3442,7 +3377,7 @@
         <v>17</v>
       </c>
       <c r="L14" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3515,10 +3450,10 @@
         <v>17</v>
       </c>
       <c r="L16" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3552,11 +3487,8 @@
       <c r="K17" t="s">
         <v>17</v>
       </c>
-      <c r="L17" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3575,8 +3507,8 @@
       <c r="F18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" t="s">
-        <v>16</v>
+      <c r="H18">
+        <v>6</v>
       </c>
       <c r="I18">
         <v>2005</v>
@@ -3588,7 +3520,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3623,7 +3555,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64</v>
       </c>
@@ -3658,7 +3590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>76</v>
       </c>
@@ -3693,7 +3625,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>78</v>
       </c>
@@ -3713,10 +3645,10 @@
         <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>835</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
+        <v>837</v>
+      </c>
+      <c r="H22">
+        <v>6</v>
       </c>
       <c r="I22">
         <v>2005</v>
@@ -3728,7 +3660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>79</v>
       </c>
@@ -3763,7 +3695,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -3798,7 +3730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
@@ -3832,11 +3764,8 @@
       <c r="K25" t="s">
         <v>17</v>
       </c>
-      <c r="L25" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>91</v>
       </c>
@@ -3870,11 +3799,8 @@
       <c r="K26" t="s">
         <v>17</v>
       </c>
-      <c r="L26" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>96</v>
       </c>
@@ -3908,11 +3834,8 @@
       <c r="K27" t="s">
         <v>17</v>
       </c>
-      <c r="L27" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -3947,7 +3870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>115</v>
       </c>
@@ -3981,11 +3904,8 @@
       <c r="K29" t="s">
         <v>17</v>
       </c>
-      <c r="L29" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>120</v>
       </c>
@@ -4019,11 +3939,8 @@
       <c r="K30" t="s">
         <v>17</v>
       </c>
-      <c r="L30" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>123</v>
       </c>
@@ -4042,8 +3959,8 @@
       <c r="F31" t="s">
         <v>21</v>
       </c>
-      <c r="H31" t="s">
-        <v>16</v>
+      <c r="H31">
+        <v>6</v>
       </c>
       <c r="I31">
         <v>2005</v>
@@ -4054,11 +3971,8 @@
       <c r="K31" t="s">
         <v>17</v>
       </c>
-      <c r="L31" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4162,9 +4076,6 @@
       <c r="K34" t="s">
         <v>17</v>
       </c>
-      <c r="L34" t="s">
-        <v>840</v>
-      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -4220,8 +4131,8 @@
       <c r="F36" t="s">
         <v>21</v>
       </c>
-      <c r="H36" t="s">
-        <v>16</v>
+      <c r="H36">
+        <v>6</v>
       </c>
       <c r="I36">
         <v>2005</v>
@@ -4267,9 +4178,6 @@
       <c r="K37" t="s">
         <v>17</v>
       </c>
-      <c r="L37" t="s">
-        <v>845</v>
-      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -4340,9 +4248,6 @@
       <c r="K39" t="s">
         <v>17</v>
       </c>
-      <c r="L39" t="s">
-        <v>841</v>
-      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -4413,9 +4318,6 @@
       <c r="K41" t="s">
         <v>17</v>
       </c>
-      <c r="L41" t="s">
-        <v>844</v>
-      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -4556,9 +4458,6 @@
       <c r="K45" t="s">
         <v>17</v>
       </c>
-      <c r="L45" t="s">
-        <v>852</v>
-      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -4630,7 +4529,7 @@
         <v>17</v>
       </c>
       <c r="L47" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -4862,8 +4761,8 @@
       <c r="F54" t="s">
         <v>21</v>
       </c>
-      <c r="H54" t="s">
-        <v>16</v>
+      <c r="H54">
+        <v>6</v>
       </c>
       <c r="I54">
         <v>2005</v>
@@ -4999,8 +4898,8 @@
       <c r="F58" t="s">
         <v>21</v>
       </c>
-      <c r="H58" t="s">
-        <v>16</v>
+      <c r="H58">
+        <v>6</v>
       </c>
       <c r="I58">
         <v>2005</v>
@@ -5047,7 +4946,7 @@
         <v>17</v>
       </c>
       <c r="L59" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -5209,8 +5108,8 @@
       <c r="F64" t="s">
         <v>21</v>
       </c>
-      <c r="H64" t="s">
-        <v>16</v>
+      <c r="H64">
+        <v>6</v>
       </c>
       <c r="I64">
         <v>2005</v>
@@ -5327,7 +5226,7 @@
         <v>17</v>
       </c>
       <c r="L67" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -5384,8 +5283,8 @@
       <c r="F69" t="s">
         <v>21</v>
       </c>
-      <c r="H69" t="s">
-        <v>16</v>
+      <c r="H69">
+        <v>6</v>
       </c>
       <c r="I69">
         <v>2005</v>
@@ -5502,7 +5401,7 @@
         <v>17</v>
       </c>
       <c r="L72" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -5539,9 +5438,6 @@
       <c r="K73" t="s">
         <v>17</v>
       </c>
-      <c r="L73" t="s">
-        <v>857</v>
-      </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -5632,11 +5528,8 @@
       <c r="F76" t="s">
         <v>21</v>
       </c>
-      <c r="G76" t="s">
-        <v>16</v>
-      </c>
-      <c r="H76" t="s">
-        <v>16</v>
+      <c r="H76">
+        <v>6</v>
       </c>
       <c r="I76">
         <v>2005</v>
@@ -5662,7 +5555,7 @@
         <v>14</v>
       </c>
       <c r="E77" t="s">
-        <v>173</v>
+        <v>15</v>
       </c>
       <c r="F77" t="s">
         <v>21</v>
@@ -5688,19 +5581,19 @@
         <v>298</v>
       </c>
       <c r="B78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C78" t="s">
         <v>174</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
+        <v>14</v>
+      </c>
+      <c r="E78" t="s">
         <v>175</v>
       </c>
-      <c r="D78" t="s">
-        <v>14</v>
-      </c>
-      <c r="E78" t="s">
-        <v>176</v>
-      </c>
       <c r="F78" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="G78" t="s">
         <v>16</v>
@@ -5723,19 +5616,19 @@
         <v>300</v>
       </c>
       <c r="B79" t="s">
+        <v>176</v>
+      </c>
+      <c r="C79" t="s">
+        <v>177</v>
+      </c>
+      <c r="D79" t="s">
+        <v>14</v>
+      </c>
+      <c r="E79" t="s">
         <v>178</v>
       </c>
-      <c r="C79" t="s">
+      <c r="F79" t="s">
         <v>179</v>
-      </c>
-      <c r="D79" t="s">
-        <v>14</v>
-      </c>
-      <c r="E79" t="s">
-        <v>180</v>
-      </c>
-      <c r="F79" t="s">
-        <v>114</v>
       </c>
       <c r="G79" t="s">
         <v>16</v>
@@ -5758,19 +5651,19 @@
         <v>303</v>
       </c>
       <c r="B80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C80" t="s">
         <v>181</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
+        <v>14</v>
+      </c>
+      <c r="E80" t="s">
         <v>182</v>
       </c>
-      <c r="D80" t="s">
-        <v>14</v>
-      </c>
-      <c r="E80" t="s">
-        <v>21</v>
-      </c>
       <c r="F80" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G80" t="s">
         <v>16</v>
@@ -5807,6 +5700,9 @@
       <c r="F81" t="s">
         <v>21</v>
       </c>
+      <c r="G81" t="s">
+        <v>16</v>
+      </c>
       <c r="H81" t="s">
         <v>16</v>
       </c>
@@ -5839,9 +5735,6 @@
       <c r="F82" t="s">
         <v>21</v>
       </c>
-      <c r="G82" t="s">
-        <v>16</v>
-      </c>
       <c r="H82" t="s">
         <v>16</v>
       </c>
@@ -5889,9 +5782,6 @@
       <c r="K83" t="s">
         <v>17</v>
       </c>
-      <c r="L83" t="s">
-        <v>817</v>
-      </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -5904,13 +5794,16 @@
         <v>190</v>
       </c>
       <c r="D84" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="E84" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="F84" t="s">
-        <v>114</v>
+        <v>21</v>
+      </c>
+      <c r="G84" t="s">
+        <v>16</v>
       </c>
       <c r="H84" t="s">
         <v>16</v>
@@ -5923,6 +5816,9 @@
       </c>
       <c r="K84" t="s">
         <v>17</v>
+      </c>
+      <c r="L84" t="s">
+        <v>819</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5930,25 +5826,22 @@
         <v>319</v>
       </c>
       <c r="B85" t="s">
+        <v>191</v>
+      </c>
+      <c r="C85" t="s">
         <v>192</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
+        <v>179</v>
+      </c>
+      <c r="E85" t="s">
         <v>193</v>
       </c>
-      <c r="D85" t="s">
-        <v>14</v>
-      </c>
-      <c r="E85" t="s">
-        <v>21</v>
-      </c>
       <c r="F85" t="s">
-        <v>21</v>
-      </c>
-      <c r="G85" t="s">
-        <v>16</v>
-      </c>
-      <c r="H85" t="s">
-        <v>16</v>
+        <v>114</v>
+      </c>
+      <c r="H85">
+        <v>6</v>
       </c>
       <c r="I85">
         <v>2005</v>
@@ -5958,9 +5851,6 @@
       </c>
       <c r="K85" t="s">
         <v>17</v>
-      </c>
-      <c r="L85" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -5977,7 +5867,7 @@
         <v>14</v>
       </c>
       <c r="E86" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="F86" t="s">
         <v>21</v>
@@ -5996,6 +5886,9 @@
       </c>
       <c r="K86" t="s">
         <v>17</v>
+      </c>
+      <c r="L86" t="s">
+        <v>823</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -6017,6 +5910,9 @@
       <c r="F87" t="s">
         <v>21</v>
       </c>
+      <c r="G87" t="s">
+        <v>16</v>
+      </c>
       <c r="H87" t="s">
         <v>16</v>
       </c>
@@ -6041,19 +5937,16 @@
         <v>199</v>
       </c>
       <c r="D88" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="E88" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="F88" t="s">
-        <v>177</v>
-      </c>
-      <c r="G88" t="s">
-        <v>16</v>
-      </c>
-      <c r="H88" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="H88">
+        <v>6</v>
       </c>
       <c r="I88">
         <v>2005</v>
@@ -6070,19 +5963,19 @@
         <v>330</v>
       </c>
       <c r="B89" t="s">
+        <v>200</v>
+      </c>
+      <c r="C89" t="s">
         <v>201</v>
       </c>
-      <c r="C89" t="s">
+      <c r="D89" t="s">
+        <v>179</v>
+      </c>
+      <c r="E89" t="s">
         <v>202</v>
       </c>
-      <c r="D89" t="s">
-        <v>153</v>
-      </c>
-      <c r="E89" t="s">
-        <v>203</v>
-      </c>
       <c r="F89" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="G89" t="s">
         <v>16</v>
@@ -6105,19 +5998,19 @@
         <v>331</v>
       </c>
       <c r="B90" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C90" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D90" t="s">
         <v>153</v>
       </c>
       <c r="E90" t="s">
-        <v>166</v>
+        <v>205</v>
       </c>
       <c r="F90" t="s">
-        <v>21</v>
+        <v>206</v>
       </c>
       <c r="G90" t="s">
         <v>16</v>
@@ -6146,7 +6039,7 @@
         <v>208</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E91" t="s">
         <v>166</v>
@@ -6181,13 +6074,13 @@
         <v>210</v>
       </c>
       <c r="D92" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="E92" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="F92" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="G92" t="s">
         <v>16</v>
@@ -6216,13 +6109,13 @@
         <v>212</v>
       </c>
       <c r="D93" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="E93" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="F93" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G93" t="s">
         <v>16</v>
@@ -6251,13 +6144,13 @@
         <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E94" t="s">
-        <v>166</v>
+        <v>178</v>
       </c>
       <c r="F94" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="G94" t="s">
         <v>16</v>
@@ -6344,9 +6237,6 @@
       <c r="K96" t="s">
         <v>17</v>
       </c>
-      <c r="L96" t="s">
-        <v>815</v>
-      </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
@@ -6359,13 +6249,13 @@
         <v>220</v>
       </c>
       <c r="D97" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E97" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="F97" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="G97" t="s">
         <v>16</v>
@@ -6383,7 +6273,7 @@
         <v>17</v>
       </c>
       <c r="L97" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -6397,13 +6287,16 @@
         <v>222</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E98" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="F98" t="s">
-        <v>21</v>
+        <v>179</v>
+      </c>
+      <c r="G98" t="s">
+        <v>16</v>
       </c>
       <c r="H98" t="s">
         <v>16</v>
@@ -6416,6 +6309,9 @@
       </c>
       <c r="K98" t="s">
         <v>17</v>
+      </c>
+      <c r="L98" t="s">
+        <v>820</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -6437,11 +6333,8 @@
       <c r="F99" t="s">
         <v>21</v>
       </c>
-      <c r="G99" t="s">
-        <v>16</v>
-      </c>
-      <c r="H99" t="s">
-        <v>16</v>
+      <c r="H99">
+        <v>6</v>
       </c>
       <c r="I99">
         <v>2005</v>
@@ -6472,6 +6365,9 @@
       <c r="F100" t="s">
         <v>21</v>
       </c>
+      <c r="G100" t="s">
+        <v>16</v>
+      </c>
       <c r="H100" t="s">
         <v>16</v>
       </c>
@@ -6504,9 +6400,6 @@
       <c r="F101" t="s">
         <v>21</v>
       </c>
-      <c r="G101" t="s">
-        <v>835</v>
-      </c>
       <c r="H101" t="s">
         <v>16</v>
       </c>
@@ -6531,7 +6424,7 @@
         <v>230</v>
       </c>
       <c r="D102" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E102" t="s">
         <v>166</v>
@@ -6539,8 +6432,11 @@
       <c r="F102" t="s">
         <v>21</v>
       </c>
-      <c r="H102" t="s">
-        <v>16</v>
+      <c r="G102" t="s">
+        <v>837</v>
+      </c>
+      <c r="H102">
+        <v>6</v>
       </c>
       <c r="I102">
         <v>2005</v>
@@ -6563,7 +6459,7 @@
         <v>232</v>
       </c>
       <c r="D103" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E103" t="s">
         <v>166</v>
@@ -6571,11 +6467,8 @@
       <c r="F103" t="s">
         <v>21</v>
       </c>
-      <c r="G103" t="s">
-        <v>16</v>
-      </c>
-      <c r="H103" t="s">
-        <v>16</v>
+      <c r="H103">
+        <v>6</v>
       </c>
       <c r="I103">
         <v>2005</v>
@@ -6706,10 +6599,13 @@
         <v>14</v>
       </c>
       <c r="E107" t="s">
-        <v>241</v>
+        <v>166</v>
       </c>
       <c r="F107" t="s">
         <v>21</v>
+      </c>
+      <c r="G107" t="s">
+        <v>16</v>
       </c>
       <c r="H107" t="s">
         <v>16</v>
@@ -6729,22 +6625,22 @@
         <v>370</v>
       </c>
       <c r="B108" t="s">
+        <v>241</v>
+      </c>
+      <c r="C108" t="s">
         <v>242</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>14</v>
+      </c>
+      <c r="E108" t="s">
         <v>243</v>
       </c>
-      <c r="D108" t="s">
-        <v>14</v>
-      </c>
-      <c r="E108" t="s">
-        <v>21</v>
-      </c>
       <c r="F108" t="s">
         <v>21</v>
       </c>
-      <c r="H108" t="s">
-        <v>16</v>
+      <c r="H108">
+        <v>6</v>
       </c>
       <c r="I108">
         <v>2005</v>
@@ -6770,16 +6666,13 @@
         <v>14</v>
       </c>
       <c r="E109" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="F109" t="s">
         <v>21</v>
       </c>
-      <c r="G109" t="s">
-        <v>16</v>
-      </c>
-      <c r="H109" t="s">
-        <v>16</v>
+      <c r="H109">
+        <v>6</v>
       </c>
       <c r="I109">
         <v>2005</v>
@@ -6875,7 +6768,7 @@
         <v>14</v>
       </c>
       <c r="E112" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="F112" t="s">
         <v>21</v>
@@ -6907,13 +6800,13 @@
         <v>253</v>
       </c>
       <c r="D113" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E113" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
       <c r="F113" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G113" t="s">
         <v>16</v>
@@ -6936,19 +6829,19 @@
         <v>384</v>
       </c>
       <c r="B114" t="s">
+        <v>254</v>
+      </c>
+      <c r="C114" t="s">
         <v>255</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
+        <v>153</v>
+      </c>
+      <c r="E114" t="s">
         <v>256</v>
       </c>
-      <c r="D114" t="s">
-        <v>14</v>
-      </c>
-      <c r="E114" t="s">
-        <v>21</v>
-      </c>
       <c r="F114" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G114" t="s">
         <v>16</v>
@@ -6985,6 +6878,9 @@
       <c r="F115" t="s">
         <v>21</v>
       </c>
+      <c r="G115" t="s">
+        <v>16</v>
+      </c>
       <c r="H115" t="s">
         <v>16</v>
       </c>
@@ -7012,7 +6908,7 @@
         <v>14</v>
       </c>
       <c r="E116" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F116" t="s">
         <v>21</v>
@@ -7035,20 +6931,23 @@
         <v>392</v>
       </c>
       <c r="B117" t="s">
+        <v>261</v>
+      </c>
+      <c r="C117" t="s">
         <v>262</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
+        <v>14</v>
+      </c>
+      <c r="E117" t="s">
         <v>263</v>
       </c>
-      <c r="D117" t="s">
-        <v>14</v>
-      </c>
-      <c r="E117" t="s">
-        <v>264</v>
-      </c>
       <c r="F117" t="s">
         <v>21</v>
       </c>
+      <c r="H117" t="s">
+        <v>16</v>
+      </c>
       <c r="I117">
         <v>2005</v>
       </c>
@@ -7056,7 +6955,7 @@
         <v>1700</v>
       </c>
       <c r="K117" t="s">
-        <v>265</v>
+        <v>17</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -7064,34 +6963,28 @@
         <v>394</v>
       </c>
       <c r="B118" t="s">
+        <v>264</v>
+      </c>
+      <c r="C118" t="s">
+        <v>265</v>
+      </c>
+      <c r="D118" t="s">
+        <v>14</v>
+      </c>
+      <c r="E118" t="s">
         <v>266</v>
       </c>
-      <c r="C118" t="s">
+      <c r="F118" t="s">
+        <v>21</v>
+      </c>
+      <c r="I118">
+        <v>2005</v>
+      </c>
+      <c r="J118">
+        <v>1700</v>
+      </c>
+      <c r="K118" t="s">
         <v>267</v>
-      </c>
-      <c r="D118" t="s">
-        <v>14</v>
-      </c>
-      <c r="E118" t="s">
-        <v>111</v>
-      </c>
-      <c r="F118" t="s">
-        <v>21</v>
-      </c>
-      <c r="G118" t="s">
-        <v>16</v>
-      </c>
-      <c r="H118" t="s">
-        <v>16</v>
-      </c>
-      <c r="I118">
-        <v>2005</v>
-      </c>
-      <c r="J118">
-        <v>1700</v>
-      </c>
-      <c r="K118" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -7108,7 +7001,7 @@
         <v>14</v>
       </c>
       <c r="E119" t="s">
-        <v>264</v>
+        <v>111</v>
       </c>
       <c r="F119" t="s">
         <v>21</v>
@@ -7126,7 +7019,7 @@
         <v>1700</v>
       </c>
       <c r="K119" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
@@ -7143,11 +7036,14 @@
         <v>14</v>
       </c>
       <c r="E120" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F120" t="s">
         <v>21</v>
       </c>
+      <c r="G120" t="s">
+        <v>16</v>
+      </c>
       <c r="H120" t="s">
         <v>16</v>
       </c>
@@ -7158,7 +7054,7 @@
         <v>1700</v>
       </c>
       <c r="K120" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
@@ -7175,7 +7071,7 @@
         <v>14</v>
       </c>
       <c r="E121" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="F121" t="s">
         <v>21</v>
@@ -7190,7 +7086,7 @@
         <v>1700</v>
       </c>
       <c r="K121" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -7207,14 +7103,11 @@
         <v>14</v>
       </c>
       <c r="E122" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F122" t="s">
         <v>21</v>
       </c>
-      <c r="G122" t="s">
-        <v>16</v>
-      </c>
       <c r="H122" t="s">
         <v>16</v>
       </c>
@@ -7225,7 +7118,7 @@
         <v>1700</v>
       </c>
       <c r="K122" t="s">
-        <v>17</v>
+        <v>267</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -7242,10 +7135,13 @@
         <v>14</v>
       </c>
       <c r="E123" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F123" t="s">
         <v>21</v>
+      </c>
+      <c r="G123" t="s">
+        <v>16</v>
       </c>
       <c r="H123" t="s">
         <v>16</v>
@@ -7274,7 +7170,7 @@
         <v>14</v>
       </c>
       <c r="E124" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F124" t="s">
         <v>21</v>
@@ -7306,7 +7202,7 @@
         <v>14</v>
       </c>
       <c r="E125" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F125" t="s">
         <v>21</v>
@@ -7338,7 +7234,7 @@
         <v>14</v>
       </c>
       <c r="E126" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F126" t="s">
         <v>21</v>
@@ -7353,7 +7249,7 @@
         <v>1700</v>
       </c>
       <c r="K126" t="s">
-        <v>265</v>
+        <v>17</v>
       </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
@@ -7370,14 +7266,11 @@
         <v>14</v>
       </c>
       <c r="E127" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F127" t="s">
         <v>21</v>
       </c>
-      <c r="G127" t="s">
-        <v>16</v>
-      </c>
       <c r="H127" t="s">
         <v>16</v>
       </c>
@@ -7388,7 +7281,7 @@
         <v>1700</v>
       </c>
       <c r="K127" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -7405,7 +7298,7 @@
         <v>14</v>
       </c>
       <c r="E128" t="s">
-        <v>166</v>
+        <v>266</v>
       </c>
       <c r="F128" t="s">
         <v>21</v>
@@ -7423,10 +7316,10 @@
         <v>1700</v>
       </c>
       <c r="K128" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>434</v>
       </c>
@@ -7440,7 +7333,7 @@
         <v>14</v>
       </c>
       <c r="E129" t="s">
-        <v>290</v>
+        <v>166</v>
       </c>
       <c r="F129" t="s">
         <v>21</v>
@@ -7461,22 +7354,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>442</v>
       </c>
       <c r="B130" t="s">
+        <v>290</v>
+      </c>
+      <c r="C130" t="s">
         <v>291</v>
       </c>
-      <c r="C130" t="s">
+      <c r="D130" t="s">
+        <v>14</v>
+      </c>
+      <c r="E130" t="s">
         <v>292</v>
       </c>
-      <c r="D130" t="s">
-        <v>14</v>
-      </c>
-      <c r="E130" t="s">
-        <v>293</v>
-      </c>
       <c r="F130" t="s">
         <v>21</v>
       </c>
@@ -7496,22 +7389,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>443</v>
       </c>
       <c r="B131" t="s">
+        <v>293</v>
+      </c>
+      <c r="C131" t="s">
         <v>294</v>
       </c>
-      <c r="C131" t="s">
+      <c r="D131" t="s">
+        <v>14</v>
+      </c>
+      <c r="E131" t="s">
         <v>295</v>
       </c>
-      <c r="D131" t="s">
-        <v>14</v>
-      </c>
-      <c r="E131" t="s">
-        <v>261</v>
-      </c>
       <c r="F131" t="s">
         <v>21</v>
       </c>
@@ -7531,7 +7424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>444</v>
       </c>
@@ -7545,7 +7438,7 @@
         <v>14</v>
       </c>
       <c r="E132" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="F132" t="s">
         <v>21</v>
@@ -7566,7 +7459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>446</v>
       </c>
@@ -7601,7 +7494,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>456</v>
       </c>
@@ -7615,7 +7508,7 @@
         <v>14</v>
       </c>
       <c r="E134" t="s">
-        <v>261</v>
+        <v>111</v>
       </c>
       <c r="F134" t="s">
         <v>21</v>
@@ -7636,7 +7529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>463</v>
       </c>
@@ -7650,7 +7543,7 @@
         <v>14</v>
       </c>
       <c r="E135" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="F135" t="s">
         <v>21</v>
@@ -7668,13 +7561,10 @@
         <v>1700</v>
       </c>
       <c r="K135" t="s">
-        <v>265</v>
-      </c>
-      <c r="L135" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>465</v>
       </c>
@@ -7688,11 +7578,17 @@
         <v>14</v>
       </c>
       <c r="E136" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="F136" t="s">
         <v>21</v>
       </c>
+      <c r="G136" t="s">
+        <v>16</v>
+      </c>
+      <c r="H136" t="s">
+        <v>16</v>
+      </c>
       <c r="I136">
         <v>2005</v>
       </c>
@@ -7700,10 +7596,10 @@
         <v>1700</v>
       </c>
       <c r="K136" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>493</v>
       </c>
@@ -7717,7 +7613,7 @@
         <v>14</v>
       </c>
       <c r="E137" t="s">
-        <v>261</v>
+        <v>295</v>
       </c>
       <c r="F137" t="s">
         <v>21</v>
@@ -7729,10 +7625,10 @@
         <v>1700</v>
       </c>
       <c r="K137" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>497</v>
       </c>
@@ -7746,7 +7642,7 @@
         <v>14</v>
       </c>
       <c r="E138" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F138" t="s">
         <v>21</v>
@@ -7758,10 +7654,10 @@
         <v>1700</v>
       </c>
       <c r="K138" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>501</v>
       </c>
@@ -7772,16 +7668,13 @@
         <v>311</v>
       </c>
       <c r="D139" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="E139" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
       <c r="F139" t="s">
-        <v>114</v>
-      </c>
-      <c r="H139" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I139">
         <v>2005</v>
@@ -7790,27 +7683,30 @@
         <v>1700</v>
       </c>
       <c r="K139" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>517</v>
       </c>
       <c r="B140" t="s">
+        <v>312</v>
+      </c>
+      <c r="C140" t="s">
         <v>313</v>
       </c>
-      <c r="C140" t="s">
+      <c r="D140" t="s">
+        <v>179</v>
+      </c>
+      <c r="E140" t="s">
         <v>314</v>
       </c>
-      <c r="D140" t="s">
-        <v>14</v>
-      </c>
-      <c r="E140" t="s">
-        <v>312</v>
-      </c>
       <c r="F140" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="H140" t="s">
+        <v>16</v>
       </c>
       <c r="I140">
         <v>2005</v>
@@ -7819,10 +7715,10 @@
         <v>1700</v>
       </c>
       <c r="K140" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>519</v>
       </c>
@@ -7836,10 +7732,10 @@
         <v>14</v>
       </c>
       <c r="E141" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F141" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="I141">
         <v>2005</v>
@@ -7848,27 +7744,27 @@
         <v>1700</v>
       </c>
       <c r="K141" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>534</v>
       </c>
       <c r="B142" t="s">
+        <v>317</v>
+      </c>
+      <c r="C142" t="s">
         <v>318</v>
       </c>
-      <c r="C142" t="s">
+      <c r="D142" t="s">
+        <v>14</v>
+      </c>
+      <c r="E142" t="s">
         <v>319</v>
       </c>
-      <c r="D142" t="s">
-        <v>14</v>
-      </c>
-      <c r="E142" t="s">
-        <v>261</v>
-      </c>
       <c r="F142" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="I142">
         <v>2005</v>
@@ -7877,10 +7773,10 @@
         <v>1700</v>
       </c>
       <c r="K142" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>535</v>
       </c>
@@ -7894,7 +7790,7 @@
         <v>14</v>
       </c>
       <c r="E143" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F143" t="s">
         <v>21</v>
@@ -7906,10 +7802,10 @@
         <v>1700</v>
       </c>
       <c r="K143" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>537</v>
       </c>
@@ -7923,7 +7819,7 @@
         <v>14</v>
       </c>
       <c r="E144" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F144" t="s">
         <v>21</v>
@@ -7935,10 +7831,10 @@
         <v>1700</v>
       </c>
       <c r="K144" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>547</v>
       </c>
@@ -7952,7 +7848,7 @@
         <v>14</v>
       </c>
       <c r="E145" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F145" t="s">
         <v>21</v>
@@ -7964,10 +7860,10 @@
         <v>1700</v>
       </c>
       <c r="K145" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>548</v>
       </c>
@@ -7978,17 +7874,14 @@
         <v>327</v>
       </c>
       <c r="D146" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="E146" t="s">
-        <v>328</v>
+        <v>263</v>
       </c>
       <c r="F146" t="s">
         <v>21</v>
       </c>
-      <c r="H146" t="s">
-        <v>16</v>
-      </c>
       <c r="I146">
         <v>2005</v>
       </c>
@@ -7996,28 +7889,31 @@
         <v>1700</v>
       </c>
       <c r="K146" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>555</v>
       </c>
       <c r="B147" t="s">
+        <v>328</v>
+      </c>
+      <c r="C147" t="s">
         <v>329</v>
-      </c>
-      <c r="C147" t="s">
-        <v>330</v>
       </c>
       <c r="D147" t="s">
         <v>114</v>
       </c>
       <c r="E147" t="s">
-        <v>261</v>
+        <v>330</v>
       </c>
       <c r="F147" t="s">
         <v>21</v>
       </c>
+      <c r="H147" t="s">
+        <v>16</v>
+      </c>
       <c r="I147">
         <v>2005</v>
       </c>
@@ -8025,10 +7921,10 @@
         <v>1700</v>
       </c>
       <c r="K147" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>563</v>
       </c>
@@ -8039,10 +7935,10 @@
         <v>332</v>
       </c>
       <c r="D148" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="E148" t="s">
-        <v>333</v>
+        <v>263</v>
       </c>
       <c r="F148" t="s">
         <v>21</v>
@@ -8054,33 +7950,27 @@
         <v>1700</v>
       </c>
       <c r="K148" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>564</v>
       </c>
       <c r="B149" t="s">
+        <v>333</v>
+      </c>
+      <c r="C149" t="s">
         <v>334</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
+        <v>14</v>
+      </c>
+      <c r="E149" t="s">
         <v>335</v>
       </c>
-      <c r="D149" t="s">
-        <v>14</v>
-      </c>
-      <c r="E149" t="s">
-        <v>293</v>
-      </c>
       <c r="F149" t="s">
-        <v>114</v>
-      </c>
-      <c r="G149" t="s">
-        <v>16</v>
-      </c>
-      <c r="H149" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I149">
         <v>2005</v>
@@ -8089,10 +7979,10 @@
         <v>1700</v>
       </c>
       <c r="K149" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>582</v>
       </c>
@@ -8106,10 +7996,10 @@
         <v>14</v>
       </c>
       <c r="E150" t="s">
-        <v>111</v>
+        <v>295</v>
       </c>
       <c r="F150" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G150" t="s">
         <v>16</v>
@@ -8124,10 +8014,10 @@
         <v>1700</v>
       </c>
       <c r="K150" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>584</v>
       </c>
@@ -8138,14 +8028,20 @@
         <v>339</v>
       </c>
       <c r="D151" t="s">
-        <v>153</v>
+        <v>14</v>
       </c>
       <c r="E151" t="s">
-        <v>340</v>
+        <v>111</v>
       </c>
       <c r="F151" t="s">
         <v>21</v>
       </c>
+      <c r="G151" t="s">
+        <v>16</v>
+      </c>
+      <c r="H151" t="s">
+        <v>16</v>
+      </c>
       <c r="I151">
         <v>2005</v>
       </c>
@@ -8153,24 +8049,24 @@
         <v>1700</v>
       </c>
       <c r="K151" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>587</v>
       </c>
       <c r="B152" t="s">
+        <v>340</v>
+      </c>
+      <c r="C152" t="s">
         <v>341</v>
-      </c>
-      <c r="C152" t="s">
-        <v>342</v>
       </c>
       <c r="D152" t="s">
         <v>153</v>
       </c>
       <c r="E152" t="s">
-        <v>111</v>
+        <v>342</v>
       </c>
       <c r="F152" t="s">
         <v>21</v>
@@ -8182,10 +8078,10 @@
         <v>1700</v>
       </c>
       <c r="K152" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>589</v>
       </c>
@@ -8196,17 +8092,14 @@
         <v>344</v>
       </c>
       <c r="D153" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E153" t="s">
-        <v>261</v>
+        <v>111</v>
       </c>
       <c r="F153" t="s">
         <v>21</v>
       </c>
-      <c r="H153" t="s">
-        <v>16</v>
-      </c>
       <c r="I153">
         <v>2005</v>
       </c>
@@ -8214,10 +8107,10 @@
         <v>1700</v>
       </c>
       <c r="K153" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>590</v>
       </c>
@@ -8228,17 +8121,14 @@
         <v>346</v>
       </c>
       <c r="D154" t="s">
-        <v>177</v>
+        <v>14</v>
       </c>
       <c r="E154" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F154" t="s">
         <v>21</v>
       </c>
-      <c r="G154" t="s">
-        <v>16</v>
-      </c>
       <c r="H154" t="s">
         <v>16</v>
       </c>
@@ -8249,10 +8139,10 @@
         <v>1700</v>
       </c>
       <c r="K154" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>591</v>
       </c>
@@ -8263,10 +8153,10 @@
         <v>348</v>
       </c>
       <c r="D155" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="E155" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F155" t="s">
         <v>21</v>
@@ -8284,10 +8174,10 @@
         <v>1700</v>
       </c>
       <c r="K155" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>611</v>
       </c>
@@ -8298,10 +8188,10 @@
         <v>350</v>
       </c>
       <c r="D156" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="E156" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F156" t="s">
         <v>21</v>
@@ -8321,11 +8211,8 @@
       <c r="K156" t="s">
         <v>17</v>
       </c>
-      <c r="L156" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>613</v>
       </c>
@@ -8339,7 +8226,7 @@
         <v>14</v>
       </c>
       <c r="E157" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F157" t="s">
         <v>21</v>
@@ -8360,7 +8247,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>615</v>
       </c>
@@ -8395,7 +8282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>619</v>
       </c>
@@ -8409,7 +8296,7 @@
         <v>14</v>
       </c>
       <c r="E159" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F159" t="s">
         <v>21</v>
@@ -8430,7 +8317,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>627</v>
       </c>
@@ -8444,7 +8331,7 @@
         <v>14</v>
       </c>
       <c r="E160" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F160" t="s">
         <v>21</v>
@@ -8479,7 +8366,7 @@
         <v>14</v>
       </c>
       <c r="E161" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F161" t="s">
         <v>21</v>
@@ -8514,7 +8401,7 @@
         <v>14</v>
       </c>
       <c r="E162" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F162" t="s">
         <v>21</v>
@@ -8533,9 +8420,6 @@
       </c>
       <c r="K162" t="s">
         <v>17</v>
-      </c>
-      <c r="L162" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -8552,7 +8436,7 @@
         <v>14</v>
       </c>
       <c r="E163" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F163" t="s">
         <v>21</v>
@@ -8571,6 +8455,9 @@
       </c>
       <c r="K163" t="s">
         <v>17</v>
+      </c>
+      <c r="L163" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -8587,7 +8474,7 @@
         <v>14</v>
       </c>
       <c r="E164" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F164" t="s">
         <v>21</v>
@@ -8622,7 +8509,7 @@
         <v>14</v>
       </c>
       <c r="E165" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F165" t="s">
         <v>21</v>
@@ -8657,7 +8544,7 @@
         <v>14</v>
       </c>
       <c r="E166" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F166" t="s">
         <v>21</v>
@@ -8676,9 +8563,6 @@
       </c>
       <c r="K166" t="s">
         <v>17</v>
-      </c>
-      <c r="L166" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.25">
@@ -8695,7 +8579,7 @@
         <v>14</v>
       </c>
       <c r="E167" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F167" t="s">
         <v>21</v>
@@ -8714,6 +8598,9 @@
       </c>
       <c r="K167" t="s">
         <v>17</v>
+      </c>
+      <c r="L167" t="s">
+        <v>828</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -8730,7 +8617,7 @@
         <v>14</v>
       </c>
       <c r="E168" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F168" t="s">
         <v>21</v>
@@ -8765,7 +8652,7 @@
         <v>14</v>
       </c>
       <c r="E169" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F169" t="s">
         <v>21</v>
@@ -8784,9 +8671,6 @@
       </c>
       <c r="K169" t="s">
         <v>17</v>
-      </c>
-      <c r="L169" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.25">
@@ -8803,7 +8687,7 @@
         <v>14</v>
       </c>
       <c r="E170" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F170" t="s">
         <v>21</v>
@@ -8822,6 +8706,9 @@
       </c>
       <c r="K170" t="s">
         <v>17</v>
+      </c>
+      <c r="L170" t="s">
+        <v>826</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
@@ -8873,7 +8760,7 @@
         <v>14</v>
       </c>
       <c r="E172" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="F172" t="s">
         <v>21</v>
@@ -8908,11 +8795,14 @@
         <v>14</v>
       </c>
       <c r="E173" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="F173" t="s">
         <v>21</v>
       </c>
+      <c r="G173" t="s">
+        <v>16</v>
+      </c>
       <c r="H173" t="s">
         <v>16</v>
       </c>
@@ -8923,7 +8813,7 @@
         <v>1700</v>
       </c>
       <c r="K173" t="s">
-        <v>265</v>
+        <v>17</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.25">
@@ -8940,14 +8830,11 @@
         <v>14</v>
       </c>
       <c r="E174" t="s">
-        <v>261</v>
+        <v>111</v>
       </c>
       <c r="F174" t="s">
         <v>21</v>
       </c>
-      <c r="G174" t="s">
-        <v>16</v>
-      </c>
       <c r="H174" t="s">
         <v>16</v>
       </c>
@@ -8958,7 +8845,7 @@
         <v>1700</v>
       </c>
       <c r="K174" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.25">
@@ -8975,7 +8862,7 @@
         <v>14</v>
       </c>
       <c r="E175" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F175" t="s">
         <v>21</v>
@@ -8993,7 +8880,7 @@
         <v>1700</v>
       </c>
       <c r="K175" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.25">
@@ -9010,11 +8897,14 @@
         <v>14</v>
       </c>
       <c r="E176" t="s">
-        <v>111</v>
+        <v>266</v>
       </c>
       <c r="F176" t="s">
         <v>21</v>
       </c>
+      <c r="G176" t="s">
+        <v>16</v>
+      </c>
       <c r="H176" t="s">
         <v>16</v>
       </c>
@@ -9025,7 +8915,7 @@
         <v>1700</v>
       </c>
       <c r="K176" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
@@ -9042,14 +8932,11 @@
         <v>14</v>
       </c>
       <c r="E177" t="s">
-        <v>340</v>
+        <v>111</v>
       </c>
       <c r="F177" t="s">
         <v>21</v>
       </c>
-      <c r="G177" t="s">
-        <v>16</v>
-      </c>
       <c r="H177" t="s">
         <v>16</v>
       </c>
@@ -9060,7 +8947,7 @@
         <v>1700</v>
       </c>
       <c r="K177" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
@@ -9077,7 +8964,7 @@
         <v>14</v>
       </c>
       <c r="E178" t="s">
-        <v>21</v>
+        <v>342</v>
       </c>
       <c r="F178" t="s">
         <v>21</v>
@@ -9095,7 +8982,7 @@
         <v>1700</v>
       </c>
       <c r="K178" t="s">
-        <v>17</v>
+        <v>267</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
@@ -9252,7 +9139,7 @@
         <v>14</v>
       </c>
       <c r="E183" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="F183" t="s">
         <v>21</v>
@@ -9287,7 +9174,7 @@
         <v>14</v>
       </c>
       <c r="E184" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F184" t="s">
         <v>21</v>
@@ -9327,6 +9214,9 @@
       <c r="F185" t="s">
         <v>21</v>
       </c>
+      <c r="G185" t="s">
+        <v>16</v>
+      </c>
       <c r="H185" t="s">
         <v>16</v>
       </c>
@@ -9359,9 +9249,6 @@
       <c r="F186" t="s">
         <v>21</v>
       </c>
-      <c r="G186" t="s">
-        <v>16</v>
-      </c>
       <c r="H186" t="s">
         <v>16</v>
       </c>
@@ -9494,7 +9381,7 @@
         <v>14</v>
       </c>
       <c r="E190" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F190" t="s">
         <v>21</v>
@@ -9529,7 +9416,7 @@
         <v>14</v>
       </c>
       <c r="E191" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F191" t="s">
         <v>21</v>
@@ -9599,7 +9486,7 @@
         <v>14</v>
       </c>
       <c r="E193" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F193" t="s">
         <v>21</v>
@@ -9634,7 +9521,7 @@
         <v>14</v>
       </c>
       <c r="E194" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F194" t="s">
         <v>21</v>
@@ -9669,7 +9556,7 @@
         <v>14</v>
       </c>
       <c r="E195" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F195" t="s">
         <v>21</v>
@@ -9704,7 +9591,7 @@
         <v>14</v>
       </c>
       <c r="E196" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F196" t="s">
         <v>21</v>
@@ -9739,7 +9626,7 @@
         <v>14</v>
       </c>
       <c r="E197" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F197" t="s">
         <v>21</v>
@@ -9774,7 +9661,7 @@
         <v>14</v>
       </c>
       <c r="E198" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F198" t="s">
         <v>21</v>
@@ -9952,7 +9839,7 @@
         <v>21</v>
       </c>
       <c r="F203" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G203" t="s">
         <v>16</v>
@@ -9987,7 +9874,7 @@
         <v>21</v>
       </c>
       <c r="F204" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G204" t="s">
         <v>16</v>
@@ -10019,7 +9906,7 @@
         <v>14</v>
       </c>
       <c r="E205" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F205" t="s">
         <v>21</v>
@@ -10054,7 +9941,7 @@
         <v>14</v>
       </c>
       <c r="E206" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F206" t="s">
         <v>21</v>
@@ -10089,7 +9976,7 @@
         <v>14</v>
       </c>
       <c r="E207" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F207" t="s">
         <v>21</v>
@@ -10124,7 +10011,7 @@
         <v>14</v>
       </c>
       <c r="E208" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F208" t="s">
         <v>21</v>
@@ -10159,7 +10046,7 @@
         <v>14</v>
       </c>
       <c r="E209" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F209" t="s">
         <v>21</v>
@@ -10194,7 +10081,7 @@
         <v>14</v>
       </c>
       <c r="E210" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F210" t="s">
         <v>21</v>
@@ -10229,7 +10116,7 @@
         <v>14</v>
       </c>
       <c r="E211" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F211" t="s">
         <v>21</v>
@@ -10264,7 +10151,7 @@
         <v>14</v>
       </c>
       <c r="E212" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F212" t="s">
         <v>21</v>
@@ -10339,6 +10226,9 @@
       <c r="F214" t="s">
         <v>21</v>
       </c>
+      <c r="G214" t="s">
+        <v>16</v>
+      </c>
       <c r="H214" t="s">
         <v>16</v>
       </c>
@@ -10366,13 +10256,10 @@
         <v>14</v>
       </c>
       <c r="E215" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F215" t="s">
         <v>21</v>
-      </c>
-      <c r="G215" t="s">
-        <v>16</v>
       </c>
       <c r="H215" t="s">
         <v>16</v>
@@ -10401,7 +10288,7 @@
         <v>14</v>
       </c>
       <c r="E216" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F216" t="s">
         <v>21</v>
@@ -10614,7 +10501,7 @@
         <v>21</v>
       </c>
       <c r="F222" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G222" t="s">
         <v>16</v>
@@ -10649,7 +10536,7 @@
         <v>21</v>
       </c>
       <c r="F223" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G223" t="s">
         <v>16</v>
@@ -10702,7 +10589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>838</v>
       </c>
@@ -10737,7 +10624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>842</v>
       </c>
@@ -10772,7 +10659,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>845</v>
       </c>
@@ -10807,7 +10694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>849</v>
       </c>
@@ -10841,11 +10728,8 @@
       <c r="K228" t="s">
         <v>17</v>
       </c>
-      <c r="L228" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>853</v>
       </c>
@@ -10880,7 +10764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>861</v>
       </c>
@@ -10915,7 +10799,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>864</v>
       </c>
@@ -10950,7 +10834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>871</v>
       </c>
@@ -10985,7 +10869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>887</v>
       </c>
@@ -11020,7 +10904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>898</v>
       </c>
@@ -11055,7 +10939,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>901</v>
       </c>
@@ -11066,13 +10950,16 @@
         <v>508</v>
       </c>
       <c r="D235" t="s">
-        <v>509</v>
+        <v>14</v>
       </c>
       <c r="E235" t="s">
-        <v>510</v>
+        <v>21</v>
       </c>
       <c r="F235" t="s">
-        <v>177</v>
+        <v>21</v>
+      </c>
+      <c r="G235" t="s">
+        <v>16</v>
       </c>
       <c r="H235" t="s">
         <v>16</v>
@@ -11087,27 +10974,24 @@
         <v>17</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>914</v>
       </c>
       <c r="B236" t="s">
+        <v>509</v>
+      </c>
+      <c r="C236" t="s">
+        <v>510</v>
+      </c>
+      <c r="D236" t="s">
         <v>511</v>
       </c>
-      <c r="C236" t="s">
+      <c r="E236" t="s">
         <v>512</v>
       </c>
-      <c r="D236" t="s">
-        <v>14</v>
-      </c>
-      <c r="E236" t="s">
-        <v>21</v>
-      </c>
       <c r="F236" t="s">
-        <v>21</v>
-      </c>
-      <c r="G236" t="s">
-        <v>16</v>
+        <v>179</v>
       </c>
       <c r="H236" t="s">
         <v>16</v>
@@ -11122,7 +11006,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>933</v>
       </c>
@@ -11157,7 +11041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>935</v>
       </c>
@@ -11192,7 +11076,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>938</v>
       </c>
@@ -11227,7 +11111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>943</v>
       </c>
@@ -11276,7 +11160,7 @@
         <v>14</v>
       </c>
       <c r="E241" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F241" t="s">
         <v>21</v>
@@ -11311,7 +11195,7 @@
         <v>14</v>
       </c>
       <c r="E242" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F242" t="s">
         <v>21</v>
@@ -11491,6 +11375,9 @@
       <c r="F247" t="s">
         <v>21</v>
       </c>
+      <c r="G247" t="s">
+        <v>16</v>
+      </c>
       <c r="H247" t="s">
         <v>16</v>
       </c>
@@ -11523,9 +11410,6 @@
       <c r="F248" t="s">
         <v>21</v>
       </c>
-      <c r="G248" t="s">
-        <v>16</v>
-      </c>
       <c r="H248" t="s">
         <v>16</v>
       </c>
@@ -11690,13 +11574,13 @@
         <v>546</v>
       </c>
       <c r="D253" t="s">
-        <v>114</v>
+        <v>14</v>
       </c>
       <c r="E253" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
       <c r="F253" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="G253" t="s">
         <v>16</v>
@@ -11725,13 +11609,13 @@
         <v>548</v>
       </c>
       <c r="D254" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="E254" t="s">
-        <v>21</v>
+        <v>256</v>
       </c>
       <c r="F254" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="G254" t="s">
         <v>16</v>
@@ -12250,13 +12134,13 @@
         <v>578</v>
       </c>
       <c r="D269" t="s">
-        <v>509</v>
+        <v>14</v>
       </c>
       <c r="E269" t="s">
-        <v>579</v>
+        <v>21</v>
       </c>
       <c r="F269" t="s">
-        <v>177</v>
+        <v>21</v>
       </c>
       <c r="G269" t="s">
         <v>16</v>
@@ -12279,19 +12163,19 @@
         <v>1214</v>
       </c>
       <c r="B270" t="s">
+        <v>579</v>
+      </c>
+      <c r="C270" t="s">
         <v>580</v>
       </c>
-      <c r="C270" t="s">
+      <c r="D270" t="s">
+        <v>511</v>
+      </c>
+      <c r="E270" t="s">
         <v>581</v>
       </c>
-      <c r="D270" t="s">
-        <v>14</v>
-      </c>
-      <c r="E270" t="s">
-        <v>21</v>
-      </c>
       <c r="F270" t="s">
-        <v>21</v>
+        <v>179</v>
       </c>
       <c r="G270" t="s">
         <v>16</v>
@@ -12833,9 +12717,6 @@
       <c r="K285" t="s">
         <v>17</v>
       </c>
-      <c r="L285" t="s">
-        <v>813</v>
-      </c>
     </row>
     <row r="286" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A286">
@@ -12871,6 +12752,9 @@
       <c r="K286" t="s">
         <v>17</v>
       </c>
+      <c r="L286" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287">
@@ -12906,9 +12790,6 @@
       <c r="K287" t="s">
         <v>17</v>
       </c>
-      <c r="L287" t="s">
-        <v>858</v>
-      </c>
     </row>
     <row r="288" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A288">
@@ -12945,7 +12826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1394</v>
       </c>
@@ -12980,7 +12861,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1398</v>
       </c>
@@ -13015,7 +12896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1411</v>
       </c>
@@ -13050,7 +12931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1424</v>
       </c>
@@ -13085,7 +12966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1430</v>
       </c>
@@ -13120,7 +13001,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1434</v>
       </c>
@@ -13155,7 +13036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1444</v>
       </c>
@@ -13174,6 +13055,9 @@
       <c r="F295" t="s">
         <v>21</v>
       </c>
+      <c r="G295" t="s">
+        <v>16</v>
+      </c>
       <c r="H295" t="s">
         <v>16</v>
       </c>
@@ -13187,7 +13071,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1450</v>
       </c>
@@ -13206,9 +13090,6 @@
       <c r="F296" t="s">
         <v>21</v>
       </c>
-      <c r="G296" t="s">
-        <v>16</v>
-      </c>
       <c r="H296" t="s">
         <v>16</v>
       </c>
@@ -13222,7 +13103,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1451</v>
       </c>
@@ -13236,7 +13117,7 @@
         <v>14</v>
       </c>
       <c r="E297" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F297" t="s">
         <v>21</v>
@@ -13257,7 +13138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1453</v>
       </c>
@@ -13271,7 +13152,7 @@
         <v>14</v>
       </c>
       <c r="E298" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F298" t="s">
         <v>21</v>
@@ -13292,7 +13173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1457</v>
       </c>
@@ -13306,7 +13187,7 @@
         <v>14</v>
       </c>
       <c r="E299" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F299" t="s">
         <v>21</v>
@@ -13327,7 +13208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1463</v>
       </c>
@@ -13341,7 +13222,7 @@
         <v>14</v>
       </c>
       <c r="E300" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F300" t="s">
         <v>21</v>
@@ -13362,7 +13243,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1466</v>
       </c>
@@ -13397,7 +13278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1469</v>
       </c>
@@ -13432,7 +13313,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1474</v>
       </c>
@@ -13467,7 +13348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>1500</v>
       </c>
@@ -13501,11 +13382,8 @@
       <c r="K304" t="s">
         <v>17</v>
       </c>
-      <c r="L304" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1509</v>
       </c>
@@ -13540,7 +13418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1520</v>
       </c>
@@ -13575,7 +13453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1529</v>
       </c>
@@ -13610,7 +13488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1536</v>
       </c>
@@ -13645,7 +13523,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>1543</v>
       </c>
@@ -13680,7 +13558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>1553</v>
       </c>
@@ -13715,7 +13593,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>1557</v>
       </c>
@@ -13750,7 +13628,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>1573</v>
       </c>
@@ -13785,7 +13663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>1592</v>
       </c>
@@ -13819,11 +13697,8 @@
       <c r="K313" t="s">
         <v>17</v>
       </c>
-      <c r="L313" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1601</v>
       </c>
@@ -13858,7 +13733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>1604</v>
       </c>
@@ -13893,7 +13768,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>1612</v>
       </c>
@@ -13928,7 +13803,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>1613</v>
       </c>
@@ -13963,7 +13838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1614</v>
       </c>
@@ -13998,7 +13873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>1617</v>
       </c>
@@ -14018,7 +13893,7 @@
         <v>21</v>
       </c>
       <c r="G319" t="s">
-        <v>680</v>
+        <v>16</v>
       </c>
       <c r="H319" t="s">
         <v>16</v>
@@ -14033,28 +13908,28 @@
         <v>17</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1622</v>
       </c>
       <c r="B320" t="s">
+        <v>680</v>
+      </c>
+      <c r="C320" t="s">
         <v>681</v>
       </c>
-      <c r="C320" t="s">
+      <c r="D320" t="s">
+        <v>14</v>
+      </c>
+      <c r="E320" t="s">
+        <v>21</v>
+      </c>
+      <c r="F320" t="s">
+        <v>21</v>
+      </c>
+      <c r="G320" t="s">
         <v>682</v>
       </c>
-      <c r="D320" t="s">
-        <v>14</v>
-      </c>
-      <c r="E320" t="s">
-        <v>21</v>
-      </c>
-      <c r="F320" t="s">
-        <v>21</v>
-      </c>
-      <c r="G320" t="s">
-        <v>16</v>
-      </c>
       <c r="H320" t="s">
         <v>16</v>
       </c>
@@ -14068,7 +13943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>1625</v>
       </c>
@@ -14082,7 +13957,7 @@
         <v>14</v>
       </c>
       <c r="E321" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F321" t="s">
         <v>21</v>
@@ -14103,7 +13978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1627</v>
       </c>
@@ -14117,7 +13992,7 @@
         <v>14</v>
       </c>
       <c r="E322" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F322" t="s">
         <v>21</v>
@@ -14137,11 +14012,8 @@
       <c r="K322" t="s">
         <v>17</v>
       </c>
-      <c r="L322" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>1635</v>
       </c>
@@ -14155,7 +14027,7 @@
         <v>14</v>
       </c>
       <c r="E323" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="F323" t="s">
         <v>21</v>
@@ -14176,7 +14048,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1639</v>
       </c>
@@ -14190,7 +14062,7 @@
         <v>14</v>
       </c>
       <c r="E324" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F324" t="s">
         <v>21</v>
@@ -14210,11 +14082,8 @@
       <c r="K324" t="s">
         <v>17</v>
       </c>
-      <c r="L324" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1644</v>
       </c>
@@ -14249,7 +14118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>1656</v>
       </c>
@@ -14268,6 +14137,9 @@
       <c r="F326" t="s">
         <v>21</v>
       </c>
+      <c r="G326" t="s">
+        <v>16</v>
+      </c>
       <c r="H326" t="s">
         <v>16</v>
       </c>
@@ -14281,7 +14153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>1664</v>
       </c>
@@ -14300,9 +14172,6 @@
       <c r="F327" t="s">
         <v>21</v>
       </c>
-      <c r="G327" t="s">
-        <v>16</v>
-      </c>
       <c r="H327" t="s">
         <v>16</v>
       </c>
@@ -14316,7 +14185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>1669</v>
       </c>
@@ -14330,7 +14199,7 @@
         <v>14</v>
       </c>
       <c r="E328" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="F328" t="s">
         <v>21</v>
@@ -14351,7 +14220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>1677</v>
       </c>
@@ -14365,7 +14234,7 @@
         <v>14</v>
       </c>
       <c r="E329" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F329" t="s">
         <v>21</v>
@@ -14386,7 +14255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1678</v>
       </c>
@@ -14421,7 +14290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>1681</v>
       </c>
@@ -14435,7 +14304,7 @@
         <v>14</v>
       </c>
       <c r="E331" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F331" t="s">
         <v>21</v>
@@ -14456,7 +14325,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1689</v>
       </c>
@@ -14470,7 +14339,7 @@
         <v>14</v>
       </c>
       <c r="E332" t="s">
-        <v>173</v>
+        <v>263</v>
       </c>
       <c r="F332" t="s">
         <v>21</v>
@@ -14491,7 +14360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1692</v>
       </c>
@@ -14505,7 +14374,7 @@
         <v>14</v>
       </c>
       <c r="E333" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F333" t="s">
         <v>21</v>
@@ -14526,7 +14395,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>1696</v>
       </c>
@@ -14540,7 +14409,7 @@
         <v>14</v>
       </c>
       <c r="E334" t="s">
-        <v>173</v>
+        <v>21</v>
       </c>
       <c r="F334" t="s">
         <v>21</v>
@@ -14561,7 +14430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1701</v>
       </c>
@@ -14575,7 +14444,7 @@
         <v>14</v>
       </c>
       <c r="E335" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="F335" t="s">
         <v>21</v>
@@ -14596,7 +14465,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>1705</v>
       </c>
@@ -14665,9 +14534,6 @@
       <c r="K337" t="s">
         <v>17</v>
       </c>
-      <c r="L337" t="s">
-        <v>850</v>
-      </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A338">
@@ -14773,9 +14639,6 @@
       <c r="K340" t="s">
         <v>17</v>
       </c>
-      <c r="L340" t="s">
-        <v>820</v>
-      </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A341">
@@ -14811,6 +14674,9 @@
       <c r="K341" t="s">
         <v>17</v>
       </c>
+      <c r="L341" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A342">
@@ -14986,9 +14852,6 @@
       <c r="K346" t="s">
         <v>17</v>
       </c>
-      <c r="L346" t="s">
-        <v>827</v>
-      </c>
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A347">
@@ -15025,7 +14888,7 @@
         <v>17</v>
       </c>
       <c r="L347" t="s">
-        <v>819</v>
+        <v>829</v>
       </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
@@ -15062,6 +14925,9 @@
       <c r="K348" t="s">
         <v>17</v>
       </c>
+      <c r="L348" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A349">
@@ -15182,7 +15048,7 @@
         <v>14</v>
       </c>
       <c r="E352" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F352" t="s">
         <v>21</v>
@@ -15217,7 +15083,7 @@
         <v>14</v>
       </c>
       <c r="E353" t="s">
-        <v>111</v>
+        <v>263</v>
       </c>
       <c r="F353" t="s">
         <v>21</v>
@@ -15252,10 +15118,13 @@
         <v>14</v>
       </c>
       <c r="E354" t="s">
-        <v>261</v>
+        <v>111</v>
       </c>
       <c r="F354" t="s">
         <v>21</v>
+      </c>
+      <c r="G354" t="s">
+        <v>16</v>
       </c>
       <c r="H354" t="s">
         <v>16</v>
@@ -15284,13 +15153,10 @@
         <v>14</v>
       </c>
       <c r="E355" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F355" t="s">
         <v>21</v>
-      </c>
-      <c r="G355" t="s">
-        <v>16</v>
       </c>
       <c r="H355" t="s">
         <v>16</v>
@@ -15564,7 +15430,7 @@
         <v>14</v>
       </c>
       <c r="E363" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F363" t="s">
         <v>21</v>
@@ -15599,10 +15465,13 @@
         <v>14</v>
       </c>
       <c r="E364" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F364" t="s">
         <v>21</v>
+      </c>
+      <c r="G364" t="s">
+        <v>16</v>
       </c>
       <c r="H364" t="s">
         <v>16</v>
@@ -15636,9 +15505,6 @@
       <c r="F365" t="s">
         <v>21</v>
       </c>
-      <c r="G365" t="s">
-        <v>16</v>
-      </c>
       <c r="H365" t="s">
         <v>16</v>
       </c>
@@ -15650,9 +15516,6 @@
       </c>
       <c r="K365" t="s">
         <v>17</v>
-      </c>
-      <c r="L365" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="366" spans="1:12" x14ac:dyDescent="0.25">
@@ -15669,7 +15532,7 @@
         <v>14</v>
       </c>
       <c r="E366" t="s">
-        <v>261</v>
+        <v>21</v>
       </c>
       <c r="F366" t="s">
         <v>21</v>
@@ -15704,7 +15567,7 @@
         <v>14</v>
       </c>
       <c r="E367" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F367" t="s">
         <v>21</v>
@@ -15723,9 +15586,6 @@
       </c>
       <c r="K367" t="s">
         <v>17</v>
-      </c>
-      <c r="L367" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="368" spans="1:12" x14ac:dyDescent="0.25">
@@ -15742,7 +15602,7 @@
         <v>14</v>
       </c>
       <c r="E368" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F368" t="s">
         <v>21</v>
@@ -15761,6 +15621,9 @@
       </c>
       <c r="K368" t="s">
         <v>17</v>
+      </c>
+      <c r="L368" t="s">
+        <v>825</v>
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
@@ -15777,7 +15640,7 @@
         <v>14</v>
       </c>
       <c r="E369" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="F369" t="s">
         <v>21</v>
@@ -15885,7 +15748,7 @@
         <v>21</v>
       </c>
       <c r="F372" t="s">
-        <v>787</v>
+        <v>21</v>
       </c>
       <c r="G372" t="s">
         <v>16</v>
@@ -15908,19 +15771,19 @@
         <v>1966</v>
       </c>
       <c r="B373" t="s">
+        <v>787</v>
+      </c>
+      <c r="C373" t="s">
         <v>788</v>
       </c>
-      <c r="C373" t="s">
+      <c r="D373" t="s">
+        <v>14</v>
+      </c>
+      <c r="E373" t="s">
+        <v>21</v>
+      </c>
+      <c r="F373" t="s">
         <v>789</v>
-      </c>
-      <c r="D373" t="s">
-        <v>14</v>
-      </c>
-      <c r="E373" t="s">
-        <v>21</v>
-      </c>
-      <c r="F373" t="s">
-        <v>21</v>
       </c>
       <c r="G373" t="s">
         <v>16</v>
@@ -15981,7 +15844,7 @@
         <v>792</v>
       </c>
       <c r="C375" t="s">
-        <v>478</v>
+        <v>793</v>
       </c>
       <c r="D375" t="s">
         <v>14</v>
@@ -16013,10 +15876,10 @@
         <v>11100</v>
       </c>
       <c r="B376" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C376" t="s">
-        <v>794</v>
+        <v>480</v>
       </c>
       <c r="D376" t="s">
         <v>14</v>
@@ -16167,6 +16030,9 @@
       <c r="F380" t="s">
         <v>21</v>
       </c>
+      <c r="G380" t="s">
+        <v>16</v>
+      </c>
       <c r="H380" t="s">
         <v>16</v>
       </c>
@@ -16199,9 +16065,6 @@
       <c r="F381" t="s">
         <v>21</v>
       </c>
-      <c r="G381" t="s">
-        <v>16</v>
-      </c>
       <c r="H381" t="s">
         <v>16</v>
       </c>
@@ -16317,6 +16180,41 @@
         <v>1700</v>
       </c>
       <c r="K384" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>11550</v>
+      </c>
+      <c r="B385" t="s">
+        <v>811</v>
+      </c>
+      <c r="C385" t="s">
+        <v>812</v>
+      </c>
+      <c r="D385" t="s">
+        <v>14</v>
+      </c>
+      <c r="E385" t="s">
+        <v>21</v>
+      </c>
+      <c r="F385" t="s">
+        <v>21</v>
+      </c>
+      <c r="G385" t="s">
+        <v>16</v>
+      </c>
+      <c r="H385" t="s">
+        <v>16</v>
+      </c>
+      <c r="I385">
+        <v>2005</v>
+      </c>
+      <c r="J385">
+        <v>1700</v>
+      </c>
+      <c r="K385" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Linked to 16:9 profile pic for magpie goose
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhanson\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="1000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -2600,7 +2600,7 @@
     <t>https://c1.staticflickr.com/5/4838/44090300790_af0d27d9ba_b_d.jpg</t>
   </si>
   <si>
-    <t>https://farm2.staticflickr.com/1883/44747039332_66eb763022_m_d.jpg</t>
+    <t>https://c1.staticflickr.com/5/4807/45899295512_21ec97bd57_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -2919,24 +2919,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="59.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="9.44140625"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.08984375" customWidth="1"/>
+    <col min="7" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="59.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="9.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
photo link for western gerygone
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AFE86168-1421-4390-8AA1-E1169EDC2220}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="882">
   <si>
     <t>species_order</t>
   </si>
@@ -2662,12 +2661,21 @@
   </si>
   <si>
     <t>Western Gerygone</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4914/32266210568_1f08be72c8_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4811/44320660970_3a6a4a5ab1_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4886/31198431047_a6663b235c_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -2979,28 +2987,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C260" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M283" sqref="M283"/>
+    <sheetView tabSelected="1" topLeftCell="A271" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A283" sqref="A283"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13"/>
-    <col min="2" max="2" width="35.140625"/>
-    <col min="3" max="3" width="29.85546875"/>
-    <col min="4" max="4" width="19.140625"/>
-    <col min="5" max="5" width="29.5703125"/>
-    <col min="6" max="6" width="17.28515625"/>
-    <col min="7" max="8" width="12.7109375"/>
-    <col min="9" max="9" width="21.5703125"/>
-    <col min="10" max="10" width="19.85546875"/>
-    <col min="12" max="12" width="63.28515625"/>
+    <col min="2" max="2" width="35.1796875"/>
+    <col min="3" max="3" width="29.81640625"/>
+    <col min="4" max="4" width="19.1796875"/>
+    <col min="5" max="5" width="29.54296875"/>
+    <col min="6" max="6" width="17.26953125"/>
+    <col min="7" max="8" width="12.7265625"/>
+    <col min="9" max="9" width="21.54296875"/>
+    <col min="10" max="10" width="19.81640625"/>
+    <col min="12" max="12" width="63.26953125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3041,7 +3049,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3082,7 +3090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -3123,7 +3131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3164,7 +3172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -3202,7 +3210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -3240,7 +3248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>24</v>
       </c>
@@ -3278,7 +3286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
@@ -3316,7 +3324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3354,7 +3362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -3395,7 +3403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>36</v>
       </c>
@@ -3433,7 +3441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>37</v>
       </c>
@@ -3471,7 +3479,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41</v>
       </c>
@@ -3509,7 +3517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>42</v>
       </c>
@@ -3547,7 +3555,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43</v>
       </c>
@@ -3585,7 +3593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -3626,7 +3634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3667,7 +3675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3702,7 +3710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3740,7 +3748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64</v>
       </c>
@@ -3778,7 +3786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>76</v>
       </c>
@@ -3816,7 +3824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>78</v>
       </c>
@@ -3854,7 +3862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>79</v>
       </c>
@@ -3892,7 +3900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -3930,7 +3938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
@@ -3971,7 +3979,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>91</v>
       </c>
@@ -4012,7 +4020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>96</v>
       </c>
@@ -4053,7 +4061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -4091,7 +4099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>115</v>
       </c>
@@ -4132,7 +4140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>120</v>
       </c>
@@ -4173,7 +4181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>123</v>
       </c>
@@ -4211,7 +4219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4249,7 +4257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>128</v>
       </c>
@@ -4287,7 +4295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>134</v>
       </c>
@@ -4328,7 +4336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>145</v>
       </c>
@@ -4366,7 +4374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>149</v>
       </c>
@@ -4401,7 +4409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>151</v>
       </c>
@@ -4442,7 +4450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>158</v>
       </c>
@@ -4480,7 +4488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>161</v>
       </c>
@@ -4521,7 +4529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>167</v>
       </c>
@@ -4559,7 +4567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>171</v>
       </c>
@@ -4600,7 +4608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>173</v>
       </c>
@@ -4638,7 +4646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>175</v>
       </c>
@@ -4676,7 +4684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>178</v>
       </c>
@@ -4714,7 +4722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>184</v>
       </c>
@@ -4755,7 +4763,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>186</v>
       </c>
@@ -4793,7 +4801,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>189</v>
       </c>
@@ -4834,7 +4842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>192</v>
       </c>
@@ -4872,7 +4880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>195</v>
       </c>
@@ -4910,7 +4918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>201</v>
       </c>
@@ -4948,7 +4956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>206</v>
       </c>
@@ -4986,7 +4994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>213</v>
       </c>
@@ -5024,7 +5032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>218</v>
       </c>
@@ -5062,7 +5070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>223</v>
       </c>
@@ -5097,7 +5105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>228</v>
       </c>
@@ -5135,7 +5143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>234</v>
       </c>
@@ -5173,7 +5181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>241</v>
       </c>
@@ -5211,7 +5219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>246</v>
       </c>
@@ -5246,7 +5254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>249</v>
       </c>
@@ -5287,7 +5295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>251</v>
       </c>
@@ -5325,7 +5333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>253</v>
       </c>
@@ -5363,7 +5371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>259</v>
       </c>
@@ -5401,7 +5409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>265</v>
       </c>
@@ -5439,7 +5447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>267</v>
       </c>
@@ -5474,7 +5482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>269</v>
       </c>
@@ -5512,7 +5520,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>273</v>
       </c>
@@ -5550,7 +5558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>274</v>
       </c>
@@ -5591,7 +5599,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>275</v>
       </c>
@@ -5629,7 +5637,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>278</v>
       </c>
@@ -5664,7 +5672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>279</v>
       </c>
@@ -5702,7 +5710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>280</v>
       </c>
@@ -5740,7 +5748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>284</v>
       </c>
@@ -5781,7 +5789,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>285</v>
       </c>
@@ -5822,7 +5830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>286</v>
       </c>
@@ -5860,7 +5868,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>288</v>
       </c>
@@ -5898,7 +5906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>297</v>
       </c>
@@ -5936,7 +5944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>298</v>
       </c>
@@ -5974,7 +5982,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>300</v>
       </c>
@@ -6012,7 +6020,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>303</v>
       </c>
@@ -6050,7 +6058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>310</v>
       </c>
@@ -6088,7 +6096,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>312</v>
       </c>
@@ -6123,7 +6131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>313</v>
       </c>
@@ -6161,7 +6169,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>316</v>
       </c>
@@ -6202,7 +6210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>319</v>
       </c>
@@ -6237,7 +6245,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>321</v>
       </c>
@@ -6278,7 +6286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>324</v>
       </c>
@@ -6316,7 +6324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>327</v>
       </c>
@@ -6351,7 +6359,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>330</v>
       </c>
@@ -6389,7 +6397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>331</v>
       </c>
@@ -6427,7 +6435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>335</v>
       </c>
@@ -6465,7 +6473,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>337</v>
       </c>
@@ -6503,7 +6511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>339</v>
       </c>
@@ -6541,7 +6549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>340</v>
       </c>
@@ -6579,7 +6587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>343</v>
       </c>
@@ -6617,7 +6625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>344</v>
       </c>
@@ -6655,7 +6663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>346</v>
       </c>
@@ -6696,7 +6704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>348</v>
       </c>
@@ -6737,7 +6745,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>349</v>
       </c>
@@ -6772,7 +6780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>350</v>
       </c>
@@ -6813,7 +6821,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>351</v>
       </c>
@@ -6848,7 +6856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>358</v>
       </c>
@@ -6886,7 +6894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>359</v>
       </c>
@@ -6924,7 +6932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>360</v>
       </c>
@@ -6959,7 +6967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>363</v>
       </c>
@@ -6997,7 +7005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>366</v>
       </c>
@@ -7035,7 +7043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>367</v>
       </c>
@@ -7076,7 +7084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>369</v>
       </c>
@@ -7114,7 +7122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>370</v>
       </c>
@@ -7149,7 +7157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>371</v>
       </c>
@@ -7184,7 +7192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>373</v>
       </c>
@@ -7222,7 +7230,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>376</v>
       </c>
@@ -7260,7 +7268,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>377</v>
       </c>
@@ -7298,7 +7306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>382</v>
       </c>
@@ -7336,7 +7344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>384</v>
       </c>
@@ -7374,7 +7382,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>385</v>
       </c>
@@ -7412,7 +7420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>390</v>
       </c>
@@ -7447,7 +7455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>392</v>
       </c>
@@ -7482,7 +7490,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>394</v>
       </c>
@@ -7514,7 +7522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>395</v>
       </c>
@@ -7552,7 +7560,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>396</v>
       </c>
@@ -7590,7 +7598,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>400</v>
       </c>
@@ -7625,7 +7633,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>404</v>
       </c>
@@ -7660,7 +7668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>411</v>
       </c>
@@ -7698,7 +7706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>416</v>
       </c>
@@ -7733,7 +7741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>417</v>
       </c>
@@ -7768,7 +7776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>423</v>
       </c>
@@ -7803,7 +7811,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>428</v>
       </c>
@@ -7838,7 +7846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>431</v>
       </c>
@@ -7876,7 +7884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>434</v>
       </c>
@@ -7914,7 +7922,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>442</v>
       </c>
@@ -7952,7 +7960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>443</v>
       </c>
@@ -7990,7 +7998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>444</v>
       </c>
@@ -8028,7 +8036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>446</v>
       </c>
@@ -8066,7 +8074,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>456</v>
       </c>
@@ -8104,7 +8112,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>463</v>
       </c>
@@ -8142,7 +8150,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>465</v>
       </c>
@@ -8183,7 +8191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>493</v>
       </c>
@@ -8215,7 +8223,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>497</v>
       </c>
@@ -8247,7 +8255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>501</v>
       </c>
@@ -8279,7 +8287,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>517</v>
       </c>
@@ -8314,7 +8322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>519</v>
       </c>
@@ -8346,7 +8354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>534</v>
       </c>
@@ -8378,7 +8386,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>535</v>
       </c>
@@ -8410,7 +8418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>537</v>
       </c>
@@ -8442,7 +8450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>547</v>
       </c>
@@ -8474,7 +8482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>548</v>
       </c>
@@ -8506,7 +8514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>555</v>
       </c>
@@ -8541,7 +8549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>563</v>
       </c>
@@ -8573,7 +8581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>564</v>
       </c>
@@ -8605,7 +8613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>582</v>
       </c>
@@ -8643,7 +8651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>584</v>
       </c>
@@ -8681,7 +8689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>587</v>
       </c>
@@ -8713,7 +8721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>589</v>
       </c>
@@ -8745,7 +8753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>590</v>
       </c>
@@ -8780,7 +8788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>591</v>
       </c>
@@ -8818,7 +8826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>611</v>
       </c>
@@ -8856,7 +8864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>613</v>
       </c>
@@ -8897,7 +8905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>615</v>
       </c>
@@ -8935,7 +8943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>619</v>
       </c>
@@ -8973,7 +8981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>627</v>
       </c>
@@ -9011,7 +9019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>629</v>
       </c>
@@ -9049,7 +9057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>636</v>
       </c>
@@ -9090,7 +9098,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>640</v>
       </c>
@@ -9131,7 +9139,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>645</v>
       </c>
@@ -9169,7 +9177,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>647</v>
       </c>
@@ -9207,7 +9215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>650</v>
       </c>
@@ -9245,7 +9253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>651</v>
       </c>
@@ -9286,7 +9294,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>656</v>
       </c>
@@ -9324,7 +9332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>658</v>
       </c>
@@ -9365,7 +9373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>659</v>
       </c>
@@ -9406,7 +9414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>660</v>
       </c>
@@ -9444,7 +9452,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>661</v>
       </c>
@@ -9485,7 +9493,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>662</v>
       </c>
@@ -9523,7 +9531,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>663</v>
       </c>
@@ -9558,7 +9566,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>669</v>
       </c>
@@ -9596,7 +9604,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>670</v>
       </c>
@@ -9634,7 +9642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>672</v>
       </c>
@@ -9669,7 +9677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>674</v>
       </c>
@@ -9707,7 +9715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>677</v>
       </c>
@@ -9745,7 +9753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>682</v>
       </c>
@@ -9783,7 +9791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>684</v>
       </c>
@@ -9821,7 +9829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>686</v>
       </c>
@@ -9859,7 +9867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>688</v>
       </c>
@@ -9900,7 +9908,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>690</v>
       </c>
@@ -9938,7 +9946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>693</v>
       </c>
@@ -9976,7 +9984,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>697</v>
       </c>
@@ -10011,7 +10019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>698</v>
       </c>
@@ -10049,7 +10057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>699</v>
       </c>
@@ -10087,7 +10095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>702</v>
       </c>
@@ -10125,7 +10133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>705</v>
       </c>
@@ -10163,7 +10171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>706</v>
       </c>
@@ -10201,7 +10209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>707</v>
       </c>
@@ -10239,7 +10247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>708</v>
       </c>
@@ -10277,7 +10285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>710</v>
       </c>
@@ -10315,7 +10323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>717</v>
       </c>
@@ -10353,7 +10361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>720</v>
       </c>
@@ -10391,7 +10399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>721</v>
       </c>
@@ -10429,7 +10437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>722</v>
       </c>
@@ -10467,7 +10475,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>724</v>
       </c>
@@ -10505,7 +10513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>726</v>
       </c>
@@ -10543,7 +10551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>728</v>
       </c>
@@ -10581,7 +10589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>730</v>
       </c>
@@ -10619,7 +10627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>735</v>
       </c>
@@ -10657,7 +10665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>741</v>
       </c>
@@ -10695,7 +10703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>742</v>
       </c>
@@ -10733,7 +10741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>746</v>
       </c>
@@ -10771,7 +10779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>764</v>
       </c>
@@ -10809,7 +10817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>765</v>
       </c>
@@ -10847,7 +10855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>773</v>
       </c>
@@ -10885,7 +10893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>782</v>
       </c>
@@ -10926,7 +10934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>785</v>
       </c>
@@ -10967,7 +10975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>789</v>
       </c>
@@ -11005,7 +11013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>793</v>
       </c>
@@ -11043,7 +11051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>797</v>
       </c>
@@ -11081,7 +11089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>800</v>
       </c>
@@ -11116,7 +11124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>803</v>
       </c>
@@ -11154,7 +11162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>807</v>
       </c>
@@ -11192,7 +11200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>810</v>
       </c>
@@ -11230,7 +11238,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>813</v>
       </c>
@@ -11268,7 +11276,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>814</v>
       </c>
@@ -11306,7 +11314,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>818</v>
       </c>
@@ -11344,7 +11352,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>819</v>
       </c>
@@ -11382,7 +11390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>825</v>
       </c>
@@ -11420,7 +11428,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>829</v>
       </c>
@@ -11458,7 +11466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>838</v>
       </c>
@@ -11496,7 +11504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>842</v>
       </c>
@@ -11534,7 +11542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>845</v>
       </c>
@@ -11572,7 +11580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>849</v>
       </c>
@@ -11610,7 +11618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>853</v>
       </c>
@@ -11651,7 +11659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>861</v>
       </c>
@@ -11692,7 +11700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>864</v>
       </c>
@@ -11730,7 +11738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>871</v>
       </c>
@@ -11768,7 +11776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>887</v>
       </c>
@@ -11806,7 +11814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>898</v>
       </c>
@@ -11844,7 +11852,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>901</v>
       </c>
@@ -11882,7 +11890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>914</v>
       </c>
@@ -11917,7 +11925,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>933</v>
       </c>
@@ -11955,7 +11963,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>935</v>
       </c>
@@ -11993,7 +12001,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>938</v>
       </c>
@@ -12031,7 +12039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>943</v>
       </c>
@@ -12069,7 +12077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>948</v>
       </c>
@@ -12107,7 +12115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>961</v>
       </c>
@@ -12145,7 +12153,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>980</v>
       </c>
@@ -12183,7 +12191,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>983</v>
       </c>
@@ -12221,7 +12229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>984</v>
       </c>
@@ -12259,7 +12267,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>995</v>
       </c>
@@ -12297,7 +12305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1001</v>
       </c>
@@ -12335,7 +12343,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1006</v>
       </c>
@@ -12370,7 +12378,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1019</v>
       </c>
@@ -12408,7 +12416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1025</v>
       </c>
@@ -12446,7 +12454,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1037</v>
       </c>
@@ -12484,7 +12492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1094</v>
       </c>
@@ -12522,7 +12530,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1101</v>
       </c>
@@ -12560,7 +12568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1103</v>
       </c>
@@ -12598,7 +12606,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>1104</v>
       </c>
@@ -12636,7 +12644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1116</v>
       </c>
@@ -12674,7 +12682,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1119</v>
       </c>
@@ -12712,7 +12720,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1123</v>
       </c>
@@ -12750,7 +12758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>1131</v>
       </c>
@@ -12788,7 +12796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>1137</v>
       </c>
@@ -12826,7 +12834,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>1145</v>
       </c>
@@ -12864,7 +12872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>1149</v>
       </c>
@@ -12902,7 +12910,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1153</v>
       </c>
@@ -12940,7 +12948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1159</v>
       </c>
@@ -12978,7 +12986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>1162</v>
       </c>
@@ -13016,7 +13024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1171</v>
       </c>
@@ -13054,7 +13062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>1195</v>
       </c>
@@ -13092,7 +13100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1208</v>
       </c>
@@ -13130,7 +13138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>1210</v>
       </c>
@@ -13168,7 +13176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1214</v>
       </c>
@@ -13206,7 +13214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1215</v>
       </c>
@@ -13244,7 +13252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1231</v>
       </c>
@@ -13282,7 +13290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1238</v>
       </c>
@@ -13320,7 +13328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1249</v>
       </c>
@@ -13358,7 +13366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>1250</v>
       </c>
@@ -13396,7 +13404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>1261</v>
       </c>
@@ -13434,7 +13442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>1262</v>
       </c>
@@ -13472,7 +13480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1274</v>
       </c>
@@ -13510,7 +13518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>1282</v>
       </c>
@@ -13548,7 +13556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>1290</v>
       </c>
@@ -13586,7 +13594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>1300</v>
       </c>
@@ -13624,7 +13632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>1313</v>
       </c>
@@ -13665,7 +13673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1317</v>
       </c>
@@ -13699,11 +13707,14 @@
       <c r="K283" t="s">
         <v>19</v>
       </c>
+      <c r="L283" t="s">
+        <v>881</v>
+      </c>
       <c r="M283" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1321</v>
       </c>
@@ -13741,7 +13752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1330</v>
       </c>
@@ -13779,7 +13790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1355</v>
       </c>
@@ -13817,7 +13828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1360</v>
       </c>
@@ -13858,7 +13869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1374</v>
       </c>
@@ -13896,7 +13907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1389</v>
       </c>
@@ -13937,7 +13948,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1394</v>
       </c>
@@ -13975,7 +13986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1398</v>
       </c>
@@ -14013,7 +14024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1411</v>
       </c>
@@ -14047,11 +14058,14 @@
       <c r="K292" t="s">
         <v>19</v>
       </c>
+      <c r="L292" t="s">
+        <v>879</v>
+      </c>
       <c r="M292" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1424</v>
       </c>
@@ -14085,11 +14099,14 @@
       <c r="K293" t="s">
         <v>19</v>
       </c>
+      <c r="L293" t="s">
+        <v>880</v>
+      </c>
       <c r="M293" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1430</v>
       </c>
@@ -14127,7 +14144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1434</v>
       </c>
@@ -14165,7 +14182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1444</v>
       </c>
@@ -14203,7 +14220,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1450</v>
       </c>
@@ -14238,7 +14255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1451</v>
       </c>
@@ -14276,7 +14293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1453</v>
       </c>
@@ -14314,7 +14331,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1457</v>
       </c>
@@ -14352,7 +14369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1463</v>
       </c>
@@ -14390,7 +14407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1466</v>
       </c>
@@ -14428,7 +14445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1469</v>
       </c>
@@ -14466,7 +14483,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>1474</v>
       </c>
@@ -14504,7 +14521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1500</v>
       </c>
@@ -14542,7 +14559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1509</v>
       </c>
@@ -14583,7 +14600,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1520</v>
       </c>
@@ -14621,7 +14638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1529</v>
       </c>
@@ -14659,7 +14676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>1536</v>
       </c>
@@ -14697,7 +14714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>1543</v>
       </c>
@@ -14735,7 +14752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>1553</v>
       </c>
@@ -14773,7 +14790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>1557</v>
       </c>
@@ -14811,7 +14828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>1573</v>
       </c>
@@ -14849,7 +14866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1592</v>
       </c>
@@ -14887,7 +14904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>1601</v>
       </c>
@@ -14928,7 +14945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>1604</v>
       </c>
@@ -14966,7 +14983,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>1612</v>
       </c>
@@ -15004,7 +15021,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1613</v>
       </c>
@@ -15042,7 +15059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>1614</v>
       </c>
@@ -15080,7 +15097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1617</v>
       </c>
@@ -15118,7 +15135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>1622</v>
       </c>
@@ -15156,7 +15173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1625</v>
       </c>
@@ -15194,7 +15211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>1627</v>
       </c>
@@ -15232,7 +15249,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1635</v>
       </c>
@@ -15273,7 +15290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1639</v>
       </c>
@@ -15311,7 +15328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>1644</v>
       </c>
@@ -15352,7 +15369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>1656</v>
       </c>
@@ -15390,7 +15407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>1664</v>
       </c>
@@ -15425,7 +15442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>1669</v>
       </c>
@@ -15463,7 +15480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1677</v>
       </c>
@@ -15501,7 +15518,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>1678</v>
       </c>
@@ -15539,7 +15556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1681</v>
       </c>
@@ -15577,7 +15594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1689</v>
       </c>
@@ -15615,7 +15632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>1692</v>
       </c>
@@ -15653,7 +15670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1696</v>
       </c>
@@ -15691,7 +15708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>1701</v>
       </c>
@@ -15729,7 +15746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1705</v>
       </c>
@@ -15767,7 +15784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>1711</v>
       </c>
@@ -15805,7 +15822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>1715</v>
       </c>
@@ -15846,7 +15863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>1720</v>
       </c>
@@ -15884,7 +15901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>1725</v>
       </c>
@@ -15922,7 +15939,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>1733</v>
       </c>
@@ -15963,7 +15980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>1744</v>
       </c>
@@ -16001,7 +16018,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>1753</v>
       </c>
@@ -16039,7 +16056,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>1756</v>
       </c>
@@ -16077,7 +16094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>1769</v>
       </c>
@@ -16115,7 +16132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>1775</v>
       </c>
@@ -16153,7 +16170,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>1779</v>
       </c>
@@ -16194,7 +16211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>1790</v>
       </c>
@@ -16235,7 +16252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1800</v>
       </c>
@@ -16273,7 +16290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>1810</v>
       </c>
@@ -16311,7 +16328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>1812</v>
       </c>
@@ -16352,7 +16369,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>1818</v>
       </c>
@@ -16390,7 +16407,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>1826</v>
       </c>
@@ -16431,7 +16448,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>1831</v>
       </c>
@@ -16469,7 +16486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>1838</v>
       </c>
@@ -16504,7 +16521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>1846</v>
       </c>
@@ -16542,7 +16559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>1850</v>
       </c>
@@ -16580,7 +16597,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>1852</v>
       </c>
@@ -16618,7 +16635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>1868</v>
       </c>
@@ -16659,7 +16676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>1876</v>
       </c>
@@ -16697,7 +16714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>1877</v>
       </c>
@@ -16735,7 +16752,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>1878</v>
       </c>
@@ -16773,7 +16790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>1880</v>
       </c>
@@ -16811,7 +16828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>1887</v>
       </c>
@@ -16849,7 +16866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>1890</v>
       </c>
@@ -16884,7 +16901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>1893</v>
       </c>
@@ -16925,7 +16942,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>1894</v>
       </c>
@@ -16963,7 +16980,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>1899</v>
       </c>
@@ -17004,7 +17021,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>1915</v>
       </c>
@@ -17042,7 +17059,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>1928</v>
       </c>
@@ -17080,7 +17097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>1933</v>
       </c>
@@ -17121,7 +17138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>1960</v>
       </c>
@@ -17159,7 +17176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>1966</v>
       </c>
@@ -17197,7 +17214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>11000</v>
       </c>
@@ -17235,7 +17252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>11050</v>
       </c>
@@ -17273,7 +17290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>11100</v>
       </c>
@@ -17311,7 +17328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>11150</v>
       </c>
@@ -17349,7 +17366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>11200</v>
       </c>
@@ -17387,7 +17404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>11250</v>
       </c>
@@ -17425,7 +17442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>11300</v>
       </c>
@@ -17463,7 +17480,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>11350</v>
       </c>
@@ -17498,7 +17515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>11400</v>
       </c>
@@ -17536,7 +17553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>11450</v>
       </c>
@@ -17574,7 +17591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>11500</v>
       </c>
@@ -17612,7 +17629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
         <v>871</v>
       </c>

</xml_diff>

<commit_message>
fixed duplicate sci name
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3489" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3489" uniqueCount="898">
   <si>
     <t>species_order</t>
   </si>
@@ -2715,6 +2715,9 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4876/46155108951_844485b3ca_b_d.jpg</t>
+  </si>
+  <si>
+    <t>Mirafra javanica</t>
   </si>
 </sst>
 </file>
@@ -3035,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+    <sheetView tabSelected="1" topLeftCell="A347" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A359" sqref="A359"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16695,7 +16698,7 @@
         <v>1852</v>
       </c>
       <c r="B359" t="s">
-        <v>704</v>
+        <v>897</v>
       </c>
       <c r="C359" t="s">
         <v>814</v>
@@ -17723,6 +17726,9 @@
       </c>
     </row>
     <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>11550</v>
+      </c>
       <c r="B386" t="s">
         <v>870</v>
       </c>

</xml_diff>

<commit_message>
Brown Quail and Black Swan photos
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{34D55D17-E1F1-4D7F-A845-6A8E82472CB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3489" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="900">
   <si>
     <t>species_order</t>
   </si>
@@ -2718,12 +2719,18 @@
   </si>
   <si>
     <t>Mirafra javanica</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4872/31216175917_b97b6572e4_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c1.staticflickr.com/5/4803/31216176627_9af339678e_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3035,28 +3042,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A347" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A359" sqref="A359"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13"/>
-    <col min="2" max="2" width="35.1796875"/>
-    <col min="3" max="3" width="29.81640625"/>
-    <col min="4" max="4" width="19.1796875"/>
-    <col min="5" max="5" width="29.54296875"/>
-    <col min="6" max="6" width="17.26953125"/>
-    <col min="7" max="8" width="12.7265625"/>
-    <col min="9" max="9" width="21.54296875"/>
-    <col min="10" max="10" width="19.81640625"/>
-    <col min="12" max="12" width="63.26953125"/>
+    <col min="2" max="2" width="35.140625"/>
+    <col min="3" max="3" width="29.85546875"/>
+    <col min="4" max="4" width="19.140625"/>
+    <col min="5" max="5" width="29.5703125"/>
+    <col min="6" max="6" width="17.28515625"/>
+    <col min="7" max="8" width="12.7109375"/>
+    <col min="9" max="9" width="21.5703125"/>
+    <col min="10" max="10" width="19.85546875"/>
+    <col min="12" max="12" width="63.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3097,7 +3104,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3138,7 +3145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
@@ -3179,7 +3186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3220,7 +3227,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
@@ -3258,7 +3265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -3292,11 +3299,14 @@
       <c r="K6" t="s">
         <v>19</v>
       </c>
+      <c r="L6" t="s">
+        <v>898</v>
+      </c>
       <c r="M6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
@@ -3334,7 +3344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>28</v>
       </c>
@@ -3375,7 +3385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3413,7 +3423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>34</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>36</v>
       </c>
@@ -3495,7 +3505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>37</v>
       </c>
@@ -3533,7 +3543,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>41</v>
       </c>
@@ -3571,7 +3581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>42</v>
       </c>
@@ -3609,7 +3619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>43</v>
       </c>
@@ -3647,7 +3657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>44</v>
       </c>
@@ -3688,7 +3698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3729,7 +3739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3764,7 +3774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3798,11 +3808,14 @@
       <c r="K19" t="s">
         <v>19</v>
       </c>
+      <c r="L19" t="s">
+        <v>899</v>
+      </c>
       <c r="M19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>64</v>
       </c>
@@ -3840,7 +3853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>76</v>
       </c>
@@ -3881,7 +3894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>78</v>
       </c>
@@ -3919,7 +3932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>79</v>
       </c>
@@ -3957,7 +3970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>81</v>
       </c>
@@ -3995,7 +4008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>85</v>
       </c>
@@ -4036,7 +4049,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>91</v>
       </c>
@@ -4077,7 +4090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>96</v>
       </c>
@@ -4118,7 +4131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>100</v>
       </c>
@@ -4156,7 +4169,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>115</v>
       </c>
@@ -4197,7 +4210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>120</v>
       </c>
@@ -4238,7 +4251,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>123</v>
       </c>
@@ -4276,7 +4289,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4317,7 +4330,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>128</v>
       </c>
@@ -4358,7 +4371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>134</v>
       </c>
@@ -4399,7 +4412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>145</v>
       </c>
@@ -4437,7 +4450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>149</v>
       </c>
@@ -4472,7 +4485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>151</v>
       </c>
@@ -4513,7 +4526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>158</v>
       </c>
@@ -4554,7 +4567,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>161</v>
       </c>
@@ -4595,7 +4608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>167</v>
       </c>
@@ -4633,7 +4646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>171</v>
       </c>
@@ -4674,7 +4687,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>173</v>
       </c>
@@ -4715,7 +4728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>175</v>
       </c>
@@ -4756,7 +4769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>178</v>
       </c>
@@ -4794,7 +4807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>184</v>
       </c>
@@ -4835,7 +4848,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>186</v>
       </c>
@@ -4873,7 +4886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>189</v>
       </c>
@@ -4914,7 +4927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>192</v>
       </c>
@@ -4955,7 +4968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>195</v>
       </c>
@@ -4993,7 +5006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>201</v>
       </c>
@@ -5034,7 +5047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>206</v>
       </c>
@@ -5072,7 +5085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>213</v>
       </c>
@@ -5110,7 +5123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>218</v>
       </c>
@@ -5151,7 +5164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>223</v>
       </c>
@@ -5186,7 +5199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>228</v>
       </c>
@@ -5224,7 +5237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>234</v>
       </c>
@@ -5262,7 +5275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>241</v>
       </c>
@@ -5303,7 +5316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>246</v>
       </c>
@@ -5338,7 +5351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>249</v>
       </c>
@@ -5379,7 +5392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>251</v>
       </c>
@@ -5420,7 +5433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>253</v>
       </c>
@@ -5461,7 +5474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>259</v>
       </c>
@@ -5502,7 +5515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>265</v>
       </c>
@@ -5540,7 +5553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>267</v>
       </c>
@@ -5575,7 +5588,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>269</v>
       </c>
@@ -5613,7 +5626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>273</v>
       </c>
@@ -5651,7 +5664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>274</v>
       </c>
@@ -5692,7 +5705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>275</v>
       </c>
@@ -5730,7 +5743,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>278</v>
       </c>
@@ -5765,7 +5778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>279</v>
       </c>
@@ -5803,7 +5816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>280</v>
       </c>
@@ -5841,7 +5854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>284</v>
       </c>
@@ -5882,7 +5895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>285</v>
       </c>
@@ -5923,7 +5936,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>286</v>
       </c>
@@ -5961,7 +5974,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>288</v>
       </c>
@@ -5999,7 +6012,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>297</v>
       </c>
@@ -6037,7 +6050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>298</v>
       </c>
@@ -6075,7 +6088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>300</v>
       </c>
@@ -6113,7 +6126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>303</v>
       </c>
@@ -6151,7 +6164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>310</v>
       </c>
@@ -6189,7 +6202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>312</v>
       </c>
@@ -6224,7 +6237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>313</v>
       </c>
@@ -6262,7 +6275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>316</v>
       </c>
@@ -6303,7 +6316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>319</v>
       </c>
@@ -6338,7 +6351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>321</v>
       </c>
@@ -6379,7 +6392,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>324</v>
       </c>
@@ -6417,7 +6430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>327</v>
       </c>
@@ -6452,7 +6465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>330</v>
       </c>
@@ -6490,7 +6503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>331</v>
       </c>
@@ -6528,7 +6541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>335</v>
       </c>
@@ -6566,7 +6579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>337</v>
       </c>
@@ -6604,7 +6617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>339</v>
       </c>
@@ -6642,7 +6655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>340</v>
       </c>
@@ -6680,7 +6693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>343</v>
       </c>
@@ -6718,7 +6731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>344</v>
       </c>
@@ -6756,7 +6769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>346</v>
       </c>
@@ -6797,7 +6810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>348</v>
       </c>
@@ -6838,7 +6851,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>349</v>
       </c>
@@ -6873,7 +6886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>350</v>
       </c>
@@ -6914,7 +6927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>351</v>
       </c>
@@ -6949,7 +6962,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>358</v>
       </c>
@@ -6987,7 +7000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>359</v>
       </c>
@@ -7025,7 +7038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>360</v>
       </c>
@@ -7060,7 +7073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>363</v>
       </c>
@@ -7098,7 +7111,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>366</v>
       </c>
@@ -7136,7 +7149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>367</v>
       </c>
@@ -7177,7 +7190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>369</v>
       </c>
@@ -7215,7 +7228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>370</v>
       </c>
@@ -7250,7 +7263,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>371</v>
       </c>
@@ -7285,7 +7298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>373</v>
       </c>
@@ -7323,7 +7336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>376</v>
       </c>
@@ -7361,7 +7374,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>377</v>
       </c>
@@ -7399,7 +7412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>382</v>
       </c>
@@ -7437,7 +7450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>384</v>
       </c>
@@ -7475,7 +7488,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>385</v>
       </c>
@@ -7513,7 +7526,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>390</v>
       </c>
@@ -7548,7 +7561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>392</v>
       </c>
@@ -7583,7 +7596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>394</v>
       </c>
@@ -7615,7 +7628,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>395</v>
       </c>
@@ -7653,7 +7666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>396</v>
       </c>
@@ -7691,7 +7704,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>400</v>
       </c>
@@ -7726,7 +7739,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>404</v>
       </c>
@@ -7761,7 +7774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>411</v>
       </c>
@@ -7799,7 +7812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>416</v>
       </c>
@@ -7834,7 +7847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>417</v>
       </c>
@@ -7869,7 +7882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>423</v>
       </c>
@@ -7904,7 +7917,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>428</v>
       </c>
@@ -7942,7 +7955,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>431</v>
       </c>
@@ -7980,7 +7993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>434</v>
       </c>
@@ -8018,7 +8031,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>442</v>
       </c>
@@ -8056,7 +8069,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>443</v>
       </c>
@@ -8094,7 +8107,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>444</v>
       </c>
@@ -8132,7 +8145,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>446</v>
       </c>
@@ -8170,7 +8183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>456</v>
       </c>
@@ -8208,7 +8221,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>463</v>
       </c>
@@ -8246,7 +8259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>465</v>
       </c>
@@ -8287,7 +8300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>493</v>
       </c>
@@ -8319,7 +8332,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>497</v>
       </c>
@@ -8351,7 +8364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>501</v>
       </c>
@@ -8383,7 +8396,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>517</v>
       </c>
@@ -8418,7 +8431,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>519</v>
       </c>
@@ -8450,7 +8463,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>534</v>
       </c>
@@ -8482,7 +8495,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>535</v>
       </c>
@@ -8514,7 +8527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>537</v>
       </c>
@@ -8546,7 +8559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>547</v>
       </c>
@@ -8578,7 +8591,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>548</v>
       </c>
@@ -8610,7 +8623,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>555</v>
       </c>
@@ -8645,7 +8658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>563</v>
       </c>
@@ -8677,7 +8690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>564</v>
       </c>
@@ -8709,7 +8722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>582</v>
       </c>
@@ -8747,7 +8760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>584</v>
       </c>
@@ -8785,7 +8798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>587</v>
       </c>
@@ -8817,7 +8830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>589</v>
       </c>
@@ -8849,7 +8862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>590</v>
       </c>
@@ -8884,7 +8897,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>591</v>
       </c>
@@ -8922,7 +8935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>611</v>
       </c>
@@ -8960,7 +8973,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>613</v>
       </c>
@@ -9001,7 +9014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>615</v>
       </c>
@@ -9039,7 +9052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>619</v>
       </c>
@@ -9077,7 +9090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>627</v>
       </c>
@@ -9115,7 +9128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>629</v>
       </c>
@@ -9153,7 +9166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>636</v>
       </c>
@@ -9194,7 +9207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>640</v>
       </c>
@@ -9235,7 +9248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>645</v>
       </c>
@@ -9273,7 +9286,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>647</v>
       </c>
@@ -9311,7 +9324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>650</v>
       </c>
@@ -9349,7 +9362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>651</v>
       </c>
@@ -9390,7 +9403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>656</v>
       </c>
@@ -9428,7 +9441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>658</v>
       </c>
@@ -9469,7 +9482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>659</v>
       </c>
@@ -9510,7 +9523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>660</v>
       </c>
@@ -9548,7 +9561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>661</v>
       </c>
@@ -9589,7 +9602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>662</v>
       </c>
@@ -9627,7 +9640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>663</v>
       </c>
@@ -9662,7 +9675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>669</v>
       </c>
@@ -9700,7 +9713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>670</v>
       </c>
@@ -9738,7 +9751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>672</v>
       </c>
@@ -9773,7 +9786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>674</v>
       </c>
@@ -9811,7 +9824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>677</v>
       </c>
@@ -9849,7 +9862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>682</v>
       </c>
@@ -9887,7 +9900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>684</v>
       </c>
@@ -9925,7 +9938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>686</v>
       </c>
@@ -9963,7 +9976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>688</v>
       </c>
@@ -10004,7 +10017,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>690</v>
       </c>
@@ -10042,7 +10055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>693</v>
       </c>
@@ -10080,7 +10093,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>697</v>
       </c>
@@ -10115,7 +10128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>698</v>
       </c>
@@ -10153,7 +10166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>699</v>
       </c>
@@ -10191,7 +10204,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>702</v>
       </c>
@@ -10229,7 +10242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>705</v>
       </c>
@@ -10267,7 +10280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>706</v>
       </c>
@@ -10305,7 +10318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>707</v>
       </c>
@@ -10343,7 +10356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>708</v>
       </c>
@@ -10381,7 +10394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>710</v>
       </c>
@@ -10419,7 +10432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>717</v>
       </c>
@@ -10457,7 +10470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>720</v>
       </c>
@@ -10495,7 +10508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>721</v>
       </c>
@@ -10533,7 +10546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>722</v>
       </c>
@@ -10571,7 +10584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>724</v>
       </c>
@@ -10609,7 +10622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>726</v>
       </c>
@@ -10647,7 +10660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>728</v>
       </c>
@@ -10685,7 +10698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>730</v>
       </c>
@@ -10723,7 +10736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>735</v>
       </c>
@@ -10761,7 +10774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>741</v>
       </c>
@@ -10799,7 +10812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>742</v>
       </c>
@@ -10837,7 +10850,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>746</v>
       </c>
@@ -10875,7 +10888,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>764</v>
       </c>
@@ -10913,7 +10926,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>765</v>
       </c>
@@ -10951,7 +10964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>773</v>
       </c>
@@ -10989,7 +11002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>782</v>
       </c>
@@ -11030,7 +11043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>785</v>
       </c>
@@ -11071,7 +11084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>789</v>
       </c>
@@ -11109,7 +11122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>793</v>
       </c>
@@ -11147,7 +11160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>797</v>
       </c>
@@ -11185,7 +11198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>800</v>
       </c>
@@ -11220,7 +11233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>803</v>
       </c>
@@ -11258,7 +11271,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>807</v>
       </c>
@@ -11296,7 +11309,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>810</v>
       </c>
@@ -11334,7 +11347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>813</v>
       </c>
@@ -11372,7 +11385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>814</v>
       </c>
@@ -11410,7 +11423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>818</v>
       </c>
@@ -11448,7 +11461,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>819</v>
       </c>
@@ -11486,7 +11499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>825</v>
       </c>
@@ -11524,7 +11537,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>829</v>
       </c>
@@ -11562,7 +11575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>838</v>
       </c>
@@ -11600,7 +11613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>842</v>
       </c>
@@ -11638,7 +11651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>845</v>
       </c>
@@ -11676,7 +11689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>849</v>
       </c>
@@ -11714,7 +11727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>853</v>
       </c>
@@ -11755,7 +11768,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>861</v>
       </c>
@@ -11796,7 +11809,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>864</v>
       </c>
@@ -11834,7 +11847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>871</v>
       </c>
@@ -11872,7 +11885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>887</v>
       </c>
@@ -11910,7 +11923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>898</v>
       </c>
@@ -11948,7 +11961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>901</v>
       </c>
@@ -11986,7 +11999,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>914</v>
       </c>
@@ -12021,7 +12034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>933</v>
       </c>
@@ -12059,7 +12072,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>935</v>
       </c>
@@ -12097,7 +12110,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>938</v>
       </c>
@@ -12135,7 +12148,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>943</v>
       </c>
@@ -12173,7 +12186,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>948</v>
       </c>
@@ -12211,7 +12224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>961</v>
       </c>
@@ -12249,7 +12262,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>980</v>
       </c>
@@ -12287,7 +12300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>983</v>
       </c>
@@ -12325,7 +12338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>984</v>
       </c>
@@ -12363,7 +12376,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>995</v>
       </c>
@@ -12401,7 +12414,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>1001</v>
       </c>
@@ -12439,7 +12452,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>1006</v>
       </c>
@@ -12474,7 +12487,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>1019</v>
       </c>
@@ -12512,7 +12525,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>1025</v>
       </c>
@@ -12550,7 +12563,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>1037</v>
       </c>
@@ -12588,7 +12601,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>1094</v>
       </c>
@@ -12626,7 +12639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>1101</v>
       </c>
@@ -12664,7 +12677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>1103</v>
       </c>
@@ -12702,7 +12715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>1104</v>
       </c>
@@ -12740,7 +12753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>1116</v>
       </c>
@@ -12778,7 +12791,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>1119</v>
       </c>
@@ -12816,7 +12829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1123</v>
       </c>
@@ -12854,7 +12867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1131</v>
       </c>
@@ -12892,7 +12905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1137</v>
       </c>
@@ -12930,7 +12943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1145</v>
       </c>
@@ -12968,7 +12981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1149</v>
       </c>
@@ -13006,7 +13019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1153</v>
       </c>
@@ -13044,7 +13057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1159</v>
       </c>
@@ -13082,7 +13095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1162</v>
       </c>
@@ -13120,7 +13133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1171</v>
       </c>
@@ -13158,7 +13171,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1195</v>
       </c>
@@ -13196,7 +13209,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1208</v>
       </c>
@@ -13234,7 +13247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1210</v>
       </c>
@@ -13272,7 +13285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1214</v>
       </c>
@@ -13310,7 +13323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1215</v>
       </c>
@@ -13348,7 +13361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1231</v>
       </c>
@@ -13386,7 +13399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1238</v>
       </c>
@@ -13424,7 +13437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1249</v>
       </c>
@@ -13462,7 +13475,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1250</v>
       </c>
@@ -13500,7 +13513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1261</v>
       </c>
@@ -13538,7 +13551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1262</v>
       </c>
@@ -13576,7 +13589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1274</v>
       </c>
@@ -13614,7 +13627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1282</v>
       </c>
@@ -13652,7 +13665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1290</v>
       </c>
@@ -13690,7 +13703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1300</v>
       </c>
@@ -13728,7 +13741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1313</v>
       </c>
@@ -13769,7 +13782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1317</v>
       </c>
@@ -13810,7 +13823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1321</v>
       </c>
@@ -13848,7 +13861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1330</v>
       </c>
@@ -13886,7 +13899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1355</v>
       </c>
@@ -13924,7 +13937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1360</v>
       </c>
@@ -13965,7 +13978,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1374</v>
       </c>
@@ -14003,7 +14016,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1389</v>
       </c>
@@ -14044,7 +14057,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1394</v>
       </c>
@@ -14082,7 +14095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1398</v>
       </c>
@@ -14120,7 +14133,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1411</v>
       </c>
@@ -14161,7 +14174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1424</v>
       </c>
@@ -14202,7 +14215,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1430</v>
       </c>
@@ -14240,7 +14253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1434</v>
       </c>
@@ -14278,7 +14291,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1444</v>
       </c>
@@ -14316,7 +14329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1450</v>
       </c>
@@ -14351,7 +14364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1451</v>
       </c>
@@ -14389,7 +14402,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1453</v>
       </c>
@@ -14427,7 +14440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1457</v>
       </c>
@@ -14465,7 +14478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1463</v>
       </c>
@@ -14503,7 +14516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>1466</v>
       </c>
@@ -14541,7 +14554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>1469</v>
       </c>
@@ -14579,7 +14592,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>1474</v>
       </c>
@@ -14617,7 +14630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>1500</v>
       </c>
@@ -14655,7 +14668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>1509</v>
       </c>
@@ -14696,7 +14709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>1520</v>
       </c>
@@ -14734,7 +14747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>1529</v>
       </c>
@@ -14772,7 +14785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>1536</v>
       </c>
@@ -14810,7 +14823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>1543</v>
       </c>
@@ -14848,7 +14861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>1553</v>
       </c>
@@ -14886,7 +14899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>1557</v>
       </c>
@@ -14924,7 +14937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>1573</v>
       </c>
@@ -14962,7 +14975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>1592</v>
       </c>
@@ -15000,7 +15013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>1601</v>
       </c>
@@ -15041,7 +15054,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>1604</v>
       </c>
@@ -15079,7 +15092,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>1612</v>
       </c>
@@ -15117,7 +15130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>1613</v>
       </c>
@@ -15155,7 +15168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>1614</v>
       </c>
@@ -15193,7 +15206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>1617</v>
       </c>
@@ -15231,7 +15244,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>1622</v>
       </c>
@@ -15269,7 +15282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>1625</v>
       </c>
@@ -15307,7 +15320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>1627</v>
       </c>
@@ -15345,7 +15358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>1635</v>
       </c>
@@ -15386,7 +15399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>1639</v>
       </c>
@@ -15424,7 +15437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>1644</v>
       </c>
@@ -15465,7 +15478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>1656</v>
       </c>
@@ -15503,7 +15516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>1664</v>
       </c>
@@ -15538,7 +15551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>1669</v>
       </c>
@@ -15576,7 +15589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>1677</v>
       </c>
@@ -15614,7 +15627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>1678</v>
       </c>
@@ -15652,7 +15665,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>1681</v>
       </c>
@@ -15690,7 +15703,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>1689</v>
       </c>
@@ -15728,7 +15741,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>1692</v>
       </c>
@@ -15766,7 +15779,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>1696</v>
       </c>
@@ -15804,7 +15817,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>1701</v>
       </c>
@@ -15842,7 +15855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>1705</v>
       </c>
@@ -15880,7 +15893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>1711</v>
       </c>
@@ -15918,7 +15931,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>1715</v>
       </c>
@@ -15959,7 +15972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>1720</v>
       </c>
@@ -15997,7 +16010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>1725</v>
       </c>
@@ -16035,7 +16048,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>1733</v>
       </c>
@@ -16076,7 +16089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>1744</v>
       </c>
@@ -16114,7 +16127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>1753</v>
       </c>
@@ -16152,7 +16165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>1756</v>
       </c>
@@ -16190,7 +16203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>1769</v>
       </c>
@@ -16228,7 +16241,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>1775</v>
       </c>
@@ -16266,7 +16279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>1779</v>
       </c>
@@ -16307,7 +16320,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>1790</v>
       </c>
@@ -16348,7 +16361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>1800</v>
       </c>
@@ -16386,7 +16399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>1810</v>
       </c>
@@ -16424,7 +16437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>1812</v>
       </c>
@@ -16465,7 +16478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>1818</v>
       </c>
@@ -16503,7 +16516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>1826</v>
       </c>
@@ -16544,7 +16557,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>1831</v>
       </c>
@@ -16582,7 +16595,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>1838</v>
       </c>
@@ -16617,7 +16630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>1846</v>
       </c>
@@ -16655,7 +16668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>1850</v>
       </c>
@@ -16693,7 +16706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>1852</v>
       </c>
@@ -16731,7 +16744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>1868</v>
       </c>
@@ -16772,7 +16785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>1876</v>
       </c>
@@ -16810,7 +16823,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>1877</v>
       </c>
@@ -16848,7 +16861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>1878</v>
       </c>
@@ -16886,7 +16899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>1880</v>
       </c>
@@ -16924,7 +16937,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>1887</v>
       </c>
@@ -16962,7 +16975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>1890</v>
       </c>
@@ -16997,7 +17010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>1893</v>
       </c>
@@ -17038,7 +17051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>1894</v>
       </c>
@@ -17076,7 +17089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>1899</v>
       </c>
@@ -17117,7 +17130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>1915</v>
       </c>
@@ -17155,7 +17168,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>1928</v>
       </c>
@@ -17193,7 +17206,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>1933</v>
       </c>
@@ -17234,7 +17247,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>1960</v>
       </c>
@@ -17272,7 +17285,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>1966</v>
       </c>
@@ -17310,7 +17323,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>11000</v>
       </c>
@@ -17348,7 +17361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>11050</v>
       </c>
@@ -17386,7 +17399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>11100</v>
       </c>
@@ -17424,7 +17437,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>11150</v>
       </c>
@@ -17462,7 +17475,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>11200</v>
       </c>
@@ -17500,7 +17513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>11250</v>
       </c>
@@ -17538,7 +17551,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>11300</v>
       </c>
@@ -17576,7 +17589,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>11350</v>
       </c>
@@ -17611,7 +17624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>11400</v>
       </c>
@@ -17649,7 +17662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>11450</v>
       </c>
@@ -17687,7 +17700,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>11500</v>
       </c>
@@ -17725,7 +17738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>11550</v>
       </c>

</xml_diff>

<commit_message>
10 more grid square descriptions
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4D4019B6-8E28-40E4-94AF-CDCA5B664157}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3495" uniqueCount="906">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3496" uniqueCount="907">
   <si>
     <t>species_order</t>
   </si>
@@ -2743,12 +2742,15 @@
   </si>
   <si>
     <t>https://c1.staticflickr.com/5/4827/44354642860_0a6414af1c_b_d.jpg</t>
+  </si>
+  <si>
+    <t>https://c2.staticflickr.com/2/1965/32369618868_8c2fa1ace7_b_d.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3094,30 +3096,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L89" sqref="L89"/>
+    <sheetView tabSelected="1" topLeftCell="A353" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B365" sqref="B365"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875"/>
-    <col min="2" max="2" width="37.5703125"/>
+    <col min="1" max="1" width="13.81640625"/>
+    <col min="2" max="2" width="37.54296875"/>
     <col min="3" max="3" width="32"/>
-    <col min="4" max="4" width="20.42578125"/>
-    <col min="5" max="5" width="31.7109375"/>
-    <col min="6" max="6" width="18.42578125"/>
-    <col min="7" max="8" width="13.5703125"/>
-    <col min="9" max="9" width="23.140625"/>
-    <col min="10" max="10" width="21.28515625"/>
-    <col min="11" max="11" width="8.85546875"/>
-    <col min="12" max="12" width="67.7109375"/>
-    <col min="13" max="1025" width="8.85546875"/>
+    <col min="4" max="4" width="20.453125"/>
+    <col min="5" max="5" width="31.7265625"/>
+    <col min="6" max="6" width="18.453125"/>
+    <col min="7" max="8" width="13.54296875"/>
+    <col min="9" max="9" width="23.1796875"/>
+    <col min="10" max="10" width="21.26953125"/>
+    <col min="11" max="11" width="8.81640625"/>
+    <col min="12" max="12" width="67.7265625"/>
+    <col min="13" max="1025" width="8.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3199,7 +3201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -3240,7 +3242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3281,7 +3283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -3319,7 +3321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>24</v>
       </c>
@@ -3398,7 +3400,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3480,7 +3482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>34</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>36</v>
       </c>
@@ -3562,7 +3564,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>37</v>
       </c>
@@ -3600,7 +3602,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41</v>
       </c>
@@ -3638,7 +3640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>42</v>
       </c>
@@ -3676,7 +3678,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43</v>
       </c>
@@ -3714,7 +3716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>44</v>
       </c>
@@ -3755,7 +3757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3796,7 +3798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3831,7 +3833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3872,7 +3874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>64</v>
       </c>
@@ -3910,7 +3912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>76</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>78</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>79</v>
       </c>
@@ -4027,7 +4029,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>81</v>
       </c>
@@ -4065,7 +4067,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
@@ -4106,7 +4108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>91</v>
       </c>
@@ -4147,7 +4149,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>96</v>
       </c>
@@ -4188,7 +4190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>100</v>
       </c>
@@ -4226,7 +4228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>115</v>
       </c>
@@ -4267,7 +4269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>120</v>
       </c>
@@ -4308,7 +4310,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>123</v>
       </c>
@@ -4346,7 +4348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4387,7 +4389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>128</v>
       </c>
@@ -4428,7 +4430,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>134</v>
       </c>
@@ -4469,7 +4471,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>145</v>
       </c>
@@ -4507,7 +4509,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>149</v>
       </c>
@@ -4542,7 +4544,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>151</v>
       </c>
@@ -4583,7 +4585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>158</v>
       </c>
@@ -4624,7 +4626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>161</v>
       </c>
@@ -4665,7 +4667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>167</v>
       </c>
@@ -4703,7 +4705,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>171</v>
       </c>
@@ -4744,7 +4746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>173</v>
       </c>
@@ -4785,7 +4787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>175</v>
       </c>
@@ -4826,7 +4828,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>178</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>184</v>
       </c>
@@ -4905,7 +4907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>186</v>
       </c>
@@ -4943,7 +4945,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>189</v>
       </c>
@@ -4984,7 +4986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>192</v>
       </c>
@@ -5025,7 +5027,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>195</v>
       </c>
@@ -5063,7 +5065,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>201</v>
       </c>
@@ -5104,7 +5106,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>206</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>213</v>
       </c>
@@ -5180,7 +5182,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>218</v>
       </c>
@@ -5221,7 +5223,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>223</v>
       </c>
@@ -5256,7 +5258,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>228</v>
       </c>
@@ -5294,7 +5296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>234</v>
       </c>
@@ -5332,7 +5334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>241</v>
       </c>
@@ -5373,7 +5375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>246</v>
       </c>
@@ -5408,7 +5410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>249</v>
       </c>
@@ -5449,7 +5451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>251</v>
       </c>
@@ -5490,7 +5492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>253</v>
       </c>
@@ -5531,7 +5533,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>259</v>
       </c>
@@ -5572,7 +5574,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>265</v>
       </c>
@@ -5610,7 +5612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>267</v>
       </c>
@@ -5645,7 +5647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>269</v>
       </c>
@@ -5683,7 +5685,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>273</v>
       </c>
@@ -5721,7 +5723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>274</v>
       </c>
@@ -5762,7 +5764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>275</v>
       </c>
@@ -5800,7 +5802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>278</v>
       </c>
@@ -5835,7 +5837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>279</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>280</v>
       </c>
@@ -5911,7 +5913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>284</v>
       </c>
@@ -5952,7 +5954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>285</v>
       </c>
@@ -5993,7 +5995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>286</v>
       </c>
@@ -6031,7 +6033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>288</v>
       </c>
@@ -6069,7 +6071,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>297</v>
       </c>
@@ -6107,7 +6109,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>298</v>
       </c>
@@ -6145,7 +6147,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>300</v>
       </c>
@@ -6183,7 +6185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>303</v>
       </c>
@@ -6221,7 +6223,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>310</v>
       </c>
@@ -6259,7 +6261,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>312</v>
       </c>
@@ -6294,7 +6296,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>313</v>
       </c>
@@ -6332,7 +6334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>316</v>
       </c>
@@ -6373,7 +6375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>319</v>
       </c>
@@ -6408,7 +6410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>321</v>
       </c>
@@ -6449,7 +6451,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>324</v>
       </c>
@@ -6490,7 +6492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>327</v>
       </c>
@@ -6525,7 +6527,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>330</v>
       </c>
@@ -6563,7 +6565,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>331</v>
       </c>
@@ -6601,7 +6603,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>335</v>
       </c>
@@ -6639,7 +6641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>337</v>
       </c>
@@ -6677,7 +6679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>339</v>
       </c>
@@ -6715,7 +6717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>340</v>
       </c>
@@ -6753,7 +6755,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>343</v>
       </c>
@@ -6791,7 +6793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>344</v>
       </c>
@@ -6829,7 +6831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>346</v>
       </c>
@@ -6870,7 +6872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>348</v>
       </c>
@@ -6911,7 +6913,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>349</v>
       </c>
@@ -6949,7 +6951,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>350</v>
       </c>
@@ -6990,7 +6992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>351</v>
       </c>
@@ -7025,7 +7027,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>358</v>
       </c>
@@ -7060,7 +7062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>359</v>
       </c>
@@ -7098,7 +7100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>360</v>
       </c>
@@ -7133,7 +7135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>363</v>
       </c>
@@ -7174,7 +7176,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>366</v>
       </c>
@@ -7212,7 +7214,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>367</v>
       </c>
@@ -7253,7 +7255,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>369</v>
       </c>
@@ -7291,7 +7293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>370</v>
       </c>
@@ -7326,7 +7328,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>371</v>
       </c>
@@ -7361,7 +7363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>373</v>
       </c>
@@ -7399,7 +7401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>376</v>
       </c>
@@ -7437,7 +7439,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>377</v>
       </c>
@@ -7475,7 +7477,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>382</v>
       </c>
@@ -7513,7 +7515,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>384</v>
       </c>
@@ -7551,7 +7553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>385</v>
       </c>
@@ -7592,7 +7594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>390</v>
       </c>
@@ -7627,7 +7629,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>392</v>
       </c>
@@ -7662,7 +7664,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>394</v>
       </c>
@@ -7694,7 +7696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>395</v>
       </c>
@@ -7732,7 +7734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>396</v>
       </c>
@@ -7770,7 +7772,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>400</v>
       </c>
@@ -7805,7 +7807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>404</v>
       </c>
@@ -7840,7 +7842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>411</v>
       </c>
@@ -7878,7 +7880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>416</v>
       </c>
@@ -7913,7 +7915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>417</v>
       </c>
@@ -7948,7 +7950,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>423</v>
       </c>
@@ -7983,7 +7985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>428</v>
       </c>
@@ -8021,7 +8023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>431</v>
       </c>
@@ -8059,7 +8061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>434</v>
       </c>
@@ -8100,7 +8102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>442</v>
       </c>
@@ -8138,7 +8140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>443</v>
       </c>
@@ -8176,7 +8178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>444</v>
       </c>
@@ -8214,7 +8216,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>446</v>
       </c>
@@ -8252,7 +8254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>456</v>
       </c>
@@ -8290,7 +8292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>463</v>
       </c>
@@ -8328,7 +8330,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>465</v>
       </c>
@@ -8369,7 +8371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>493</v>
       </c>
@@ -8401,7 +8403,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>497</v>
       </c>
@@ -8433,7 +8435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>501</v>
       </c>
@@ -8465,7 +8467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>517</v>
       </c>
@@ -8500,7 +8502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>519</v>
       </c>
@@ -8532,7 +8534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>534</v>
       </c>
@@ -8564,7 +8566,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>535</v>
       </c>
@@ -8596,7 +8598,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>537</v>
       </c>
@@ -8628,7 +8630,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>547</v>
       </c>
@@ -8660,7 +8662,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>548</v>
       </c>
@@ -8692,7 +8694,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>555</v>
       </c>
@@ -8727,7 +8729,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>563</v>
       </c>
@@ -8759,7 +8761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>564</v>
       </c>
@@ -8791,7 +8793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>582</v>
       </c>
@@ -8829,7 +8831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>584</v>
       </c>
@@ -8867,7 +8869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>587</v>
       </c>
@@ -8899,7 +8901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>589</v>
       </c>
@@ -8931,7 +8933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>590</v>
       </c>
@@ -8966,7 +8968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>591</v>
       </c>
@@ -9004,7 +9006,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>611</v>
       </c>
@@ -9042,7 +9044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>613</v>
       </c>
@@ -9083,7 +9085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>615</v>
       </c>
@@ -9121,7 +9123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>619</v>
       </c>
@@ -9159,7 +9161,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>627</v>
       </c>
@@ -9197,7 +9199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>629</v>
       </c>
@@ -9235,7 +9237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>636</v>
       </c>
@@ -9276,7 +9278,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>640</v>
       </c>
@@ -9317,7 +9319,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>645</v>
       </c>
@@ -9355,7 +9357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>647</v>
       </c>
@@ -9393,7 +9395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>650</v>
       </c>
@@ -9431,7 +9433,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>651</v>
       </c>
@@ -9472,7 +9474,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>656</v>
       </c>
@@ -9510,7 +9512,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>658</v>
       </c>
@@ -9551,7 +9553,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>659</v>
       </c>
@@ -9592,7 +9594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>660</v>
       </c>
@@ -9630,7 +9632,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>661</v>
       </c>
@@ -9671,7 +9673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>662</v>
       </c>
@@ -9709,7 +9711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>663</v>
       </c>
@@ -9744,7 +9746,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>669</v>
       </c>
@@ -9782,7 +9784,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>670</v>
       </c>
@@ -9820,7 +9822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>672</v>
       </c>
@@ -9855,7 +9857,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>674</v>
       </c>
@@ -9893,7 +9895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>677</v>
       </c>
@@ -9931,7 +9933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>682</v>
       </c>
@@ -9969,7 +9971,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>684</v>
       </c>
@@ -10007,7 +10009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>686</v>
       </c>
@@ -10045,7 +10047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>688</v>
       </c>
@@ -10086,7 +10088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>690</v>
       </c>
@@ -10124,7 +10126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>693</v>
       </c>
@@ -10162,7 +10164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>697</v>
       </c>
@@ -10197,7 +10199,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>698</v>
       </c>
@@ -10235,7 +10237,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>699</v>
       </c>
@@ -10273,7 +10275,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>702</v>
       </c>
@@ -10311,7 +10313,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>705</v>
       </c>
@@ -10349,7 +10351,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>706</v>
       </c>
@@ -10387,7 +10389,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>707</v>
       </c>
@@ -10425,7 +10427,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>708</v>
       </c>
@@ -10463,7 +10465,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>710</v>
       </c>
@@ -10501,7 +10503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>717</v>
       </c>
@@ -10539,7 +10541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>720</v>
       </c>
@@ -10577,7 +10579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>721</v>
       </c>
@@ -10615,7 +10617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>722</v>
       </c>
@@ -10653,7 +10655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>724</v>
       </c>
@@ -10691,7 +10693,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>726</v>
       </c>
@@ -10729,7 +10731,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>728</v>
       </c>
@@ -10767,7 +10769,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>730</v>
       </c>
@@ -10805,7 +10807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>735</v>
       </c>
@@ -10843,7 +10845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>741</v>
       </c>
@@ -10881,7 +10883,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>742</v>
       </c>
@@ -10919,7 +10921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>746</v>
       </c>
@@ -10957,7 +10959,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>764</v>
       </c>
@@ -10995,7 +10997,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>765</v>
       </c>
@@ -11033,7 +11035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>773</v>
       </c>
@@ -11071,7 +11073,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>782</v>
       </c>
@@ -11112,7 +11114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>785</v>
       </c>
@@ -11153,7 +11155,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>789</v>
       </c>
@@ -11191,7 +11193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>793</v>
       </c>
@@ -11229,7 +11231,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>797</v>
       </c>
@@ -11267,7 +11269,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>800</v>
       </c>
@@ -11302,7 +11304,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>803</v>
       </c>
@@ -11340,7 +11342,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>807</v>
       </c>
@@ -11378,7 +11380,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>810</v>
       </c>
@@ -11416,7 +11418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>813</v>
       </c>
@@ -11454,7 +11456,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>814</v>
       </c>
@@ -11492,7 +11494,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>818</v>
       </c>
@@ -11530,7 +11532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>819</v>
       </c>
@@ -11568,7 +11570,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>825</v>
       </c>
@@ -11606,7 +11608,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>829</v>
       </c>
@@ -11644,7 +11646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>838</v>
       </c>
@@ -11682,7 +11684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>842</v>
       </c>
@@ -11720,7 +11722,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>845</v>
       </c>
@@ -11758,7 +11760,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>849</v>
       </c>
@@ -11796,7 +11798,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>853</v>
       </c>
@@ -11837,7 +11839,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>861</v>
       </c>
@@ -11878,7 +11880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>864</v>
       </c>
@@ -11916,7 +11918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>871</v>
       </c>
@@ -11954,7 +11956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>887</v>
       </c>
@@ -11992,7 +11994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>898</v>
       </c>
@@ -12030,7 +12032,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>901</v>
       </c>
@@ -12068,7 +12070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>914</v>
       </c>
@@ -12103,7 +12105,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>933</v>
       </c>
@@ -12141,7 +12143,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>935</v>
       </c>
@@ -12179,7 +12181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>938</v>
       </c>
@@ -12217,7 +12219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>943</v>
       </c>
@@ -12255,7 +12257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>948</v>
       </c>
@@ -12293,7 +12295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>961</v>
       </c>
@@ -12331,7 +12333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>980</v>
       </c>
@@ -12369,7 +12371,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>983</v>
       </c>
@@ -12407,7 +12409,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>984</v>
       </c>
@@ -12445,7 +12447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>995</v>
       </c>
@@ -12483,7 +12485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1001</v>
       </c>
@@ -12521,7 +12523,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1006</v>
       </c>
@@ -12556,7 +12558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1019</v>
       </c>
@@ -12594,7 +12596,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1025</v>
       </c>
@@ -12632,7 +12634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1037</v>
       </c>
@@ -12670,7 +12672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1094</v>
       </c>
@@ -12708,7 +12710,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1101</v>
       </c>
@@ -12746,7 +12748,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1103</v>
       </c>
@@ -12784,7 +12786,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>1104</v>
       </c>
@@ -12822,7 +12824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1116</v>
       </c>
@@ -12860,7 +12862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1119</v>
       </c>
@@ -12898,7 +12900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1123</v>
       </c>
@@ -12936,7 +12938,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>1131</v>
       </c>
@@ -12974,7 +12976,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>1137</v>
       </c>
@@ -13012,7 +13014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>1145</v>
       </c>
@@ -13050,7 +13052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>1149</v>
       </c>
@@ -13088,7 +13090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1153</v>
       </c>
@@ -13126,7 +13128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1159</v>
       </c>
@@ -13164,7 +13166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>1162</v>
       </c>
@@ -13202,7 +13204,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1171</v>
       </c>
@@ -13240,7 +13242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>1195</v>
       </c>
@@ -13278,7 +13280,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1208</v>
       </c>
@@ -13316,7 +13318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>1210</v>
       </c>
@@ -13354,7 +13356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1214</v>
       </c>
@@ -13392,7 +13394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1215</v>
       </c>
@@ -13430,7 +13432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1231</v>
       </c>
@@ -13468,7 +13470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1238</v>
       </c>
@@ -13506,7 +13508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1249</v>
       </c>
@@ -13544,7 +13546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>1250</v>
       </c>
@@ -13582,7 +13584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>1261</v>
       </c>
@@ -13620,7 +13622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>1262</v>
       </c>
@@ -13658,7 +13660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1274</v>
       </c>
@@ -13696,7 +13698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>1282</v>
       </c>
@@ -13734,7 +13736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>1290</v>
       </c>
@@ -13772,7 +13774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>1300</v>
       </c>
@@ -13810,7 +13812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>1313</v>
       </c>
@@ -13851,7 +13853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1317</v>
       </c>
@@ -13889,7 +13891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1321</v>
       </c>
@@ -13927,7 +13929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1330</v>
       </c>
@@ -13965,7 +13967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1355</v>
       </c>
@@ -14003,7 +14005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1360</v>
       </c>
@@ -14044,7 +14046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1374</v>
       </c>
@@ -14082,7 +14084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1389</v>
       </c>
@@ -14123,7 +14125,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1394</v>
       </c>
@@ -14161,7 +14163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1398</v>
       </c>
@@ -14199,7 +14201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1411</v>
       </c>
@@ -14240,7 +14242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1424</v>
       </c>
@@ -14281,7 +14283,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1430</v>
       </c>
@@ -14319,7 +14321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1434</v>
       </c>
@@ -14357,7 +14359,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1444</v>
       </c>
@@ -14395,7 +14397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>1450</v>
       </c>
@@ -14430,7 +14432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>1451</v>
       </c>
@@ -14468,7 +14470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>1453</v>
       </c>
@@ -14506,7 +14508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>1457</v>
       </c>
@@ -14544,7 +14546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>1463</v>
       </c>
@@ -14582,7 +14584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>1466</v>
       </c>
@@ -14620,7 +14622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>1469</v>
       </c>
@@ -14658,7 +14660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>1474</v>
       </c>
@@ -14696,7 +14698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>1500</v>
       </c>
@@ -14734,7 +14736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>1509</v>
       </c>
@@ -14775,7 +14777,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1520</v>
       </c>
@@ -14813,7 +14815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1529</v>
       </c>
@@ -14851,7 +14853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>1536</v>
       </c>
@@ -14889,7 +14891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>1543</v>
       </c>
@@ -14927,7 +14929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>1553</v>
       </c>
@@ -14965,7 +14967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>1557</v>
       </c>
@@ -15003,7 +15005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>1573</v>
       </c>
@@ -15041,7 +15043,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>1592</v>
       </c>
@@ -15079,7 +15081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>1601</v>
       </c>
@@ -15120,7 +15122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>1604</v>
       </c>
@@ -15158,7 +15160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>1612</v>
       </c>
@@ -15196,7 +15198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>1613</v>
       </c>
@@ -15234,7 +15236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>1614</v>
       </c>
@@ -15272,7 +15274,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>1617</v>
       </c>
@@ -15310,7 +15312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>1622</v>
       </c>
@@ -15348,7 +15350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>1625</v>
       </c>
@@ -15386,7 +15388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>1627</v>
       </c>
@@ -15424,7 +15426,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1635</v>
       </c>
@@ -15465,7 +15467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1639</v>
       </c>
@@ -15503,7 +15505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>1644</v>
       </c>
@@ -15544,7 +15546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>1656</v>
       </c>
@@ -15582,7 +15584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>1664</v>
       </c>
@@ -15617,7 +15619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>1669</v>
       </c>
@@ -15655,7 +15657,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>1677</v>
       </c>
@@ -15693,7 +15695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>1678</v>
       </c>
@@ -15731,7 +15733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1681</v>
       </c>
@@ -15769,7 +15771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1689</v>
       </c>
@@ -15807,7 +15809,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>1692</v>
       </c>
@@ -15845,7 +15847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>1696</v>
       </c>
@@ -15883,7 +15885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>1701</v>
       </c>
@@ -15921,7 +15923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1705</v>
       </c>
@@ -15959,7 +15961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>1711</v>
       </c>
@@ -15997,7 +15999,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>1715</v>
       </c>
@@ -16038,7 +16040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>1720</v>
       </c>
@@ -16076,7 +16078,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>1725</v>
       </c>
@@ -16114,7 +16116,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>1733</v>
       </c>
@@ -16155,7 +16157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>1744</v>
       </c>
@@ -16193,7 +16195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>1753</v>
       </c>
@@ -16231,7 +16233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>1756</v>
       </c>
@@ -16269,7 +16271,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>1769</v>
       </c>
@@ -16307,7 +16309,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>1775</v>
       </c>
@@ -16345,7 +16347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>1779</v>
       </c>
@@ -16386,7 +16388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>1790</v>
       </c>
@@ -16427,7 +16429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1800</v>
       </c>
@@ -16465,7 +16467,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>1810</v>
       </c>
@@ -16503,7 +16505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>1812</v>
       </c>
@@ -16544,7 +16546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>1818</v>
       </c>
@@ -16582,7 +16584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>1826</v>
       </c>
@@ -16623,7 +16625,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>1831</v>
       </c>
@@ -16661,7 +16663,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>1838</v>
       </c>
@@ -16696,7 +16698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>1846</v>
       </c>
@@ -16734,7 +16736,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>1850</v>
       </c>
@@ -16772,7 +16774,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>1852</v>
       </c>
@@ -16810,7 +16812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>1868</v>
       </c>
@@ -16851,7 +16853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>1876</v>
       </c>
@@ -16889,7 +16891,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>1877</v>
       </c>
@@ -16927,7 +16929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>1878</v>
       </c>
@@ -16965,7 +16967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>1880</v>
       </c>
@@ -17003,7 +17005,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>1887</v>
       </c>
@@ -17037,11 +17039,14 @@
       <c r="K365" t="s">
         <v>19</v>
       </c>
+      <c r="L365" t="s">
+        <v>906</v>
+      </c>
       <c r="M365" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>1890</v>
       </c>
@@ -17076,7 +17081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>1893</v>
       </c>
@@ -17117,7 +17122,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>1894</v>
       </c>
@@ -17155,7 +17160,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>1899</v>
       </c>
@@ -17196,7 +17201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>1915</v>
       </c>
@@ -17234,7 +17239,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>1928</v>
       </c>
@@ -17272,7 +17277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>1933</v>
       </c>
@@ -17313,7 +17318,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>1960</v>
       </c>
@@ -17351,7 +17356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>1966</v>
       </c>
@@ -17389,7 +17394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>11000</v>
       </c>
@@ -17427,7 +17432,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>11050</v>
       </c>
@@ -17465,7 +17470,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>11100</v>
       </c>
@@ -17503,7 +17508,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>11150</v>
       </c>
@@ -17541,7 +17546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>11200</v>
       </c>
@@ -17579,7 +17584,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>11250</v>
       </c>
@@ -17617,7 +17622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>11300</v>
       </c>
@@ -17655,7 +17660,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>11350</v>
       </c>
@@ -17690,7 +17695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>11400</v>
       </c>
@@ -17728,7 +17733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>11450</v>
       </c>
@@ -17766,7 +17771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="385" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>11500</v>
       </c>
@@ -17804,7 +17809,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="386" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>11550</v>
       </c>

</xml_diff>

<commit_message>
removed "(hybrid)" from Mallard x PBD to hopefully fix surveyor sheet problem
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqrfulle_local\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D789EC9-FED6-4493-A461-BD28367F6752}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
@@ -2776,13 +2772,13 @@
     <t>Anas platyrhynchos x superciliosa</t>
   </si>
   <si>
-    <t>Mallard x Pacific Black Duck (hybrid)</t>
+    <t>Mallard x Pacific Black Duck</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3128,30 +3124,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView tabSelected="1" topLeftCell="A359" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C383" sqref="C383"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="32"/>
-    <col min="4" max="4" width="17.54296875" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" customWidth="1"/>
-    <col min="7" max="8" width="13.54296875"/>
-    <col min="9" max="9" width="7.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125"/>
+    <col min="9" max="9" width="7.28515625" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625"/>
-    <col min="12" max="12" width="67.7265625"/>
-    <col min="13" max="1025" width="8.81640625"/>
+    <col min="11" max="11" width="8.85546875"/>
+    <col min="12" max="12" width="67.7109375"/>
+    <col min="13" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3195,7 +3191,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -3239,7 +3235,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12</v>
       </c>
@@ -3283,7 +3279,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>13</v>
       </c>
@@ -3327,7 +3323,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
@@ -3368,7 +3364,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -3412,7 +3408,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>24</v>
       </c>
@@ -3453,7 +3449,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>28</v>
       </c>
@@ -3497,7 +3493,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3541,7 +3537,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>34</v>
       </c>
@@ -3585,7 +3581,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>36</v>
       </c>
@@ -3629,7 +3625,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>37</v>
       </c>
@@ -3670,7 +3666,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>41</v>
       </c>
@@ -3711,7 +3707,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>42</v>
       </c>
@@ -3752,7 +3748,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>43</v>
       </c>
@@ -3793,7 +3789,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>44</v>
       </c>
@@ -3837,7 +3833,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>47</v>
       </c>
@@ -3881,7 +3877,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>60</v>
       </c>
@@ -3919,7 +3915,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>61</v>
       </c>
@@ -3963,7 +3959,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>64</v>
       </c>
@@ -4004,7 +4000,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>76</v>
       </c>
@@ -4048,7 +4044,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>78</v>
       </c>
@@ -4089,7 +4085,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>79</v>
       </c>
@@ -4130,7 +4126,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>81</v>
       </c>
@@ -4171,7 +4167,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>85</v>
       </c>
@@ -4215,7 +4211,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>91</v>
       </c>
@@ -4259,7 +4255,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>96</v>
       </c>
@@ -4303,7 +4299,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>100</v>
       </c>
@@ -4344,7 +4340,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>115</v>
       </c>
@@ -4388,7 +4384,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>120</v>
       </c>
@@ -4432,7 +4428,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>123</v>
       </c>
@@ -4473,7 +4469,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>124</v>
       </c>
@@ -4517,7 +4513,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>128</v>
       </c>
@@ -4561,7 +4557,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>134</v>
       </c>
@@ -4605,7 +4601,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>145</v>
       </c>
@@ -4646,7 +4642,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>149</v>
       </c>
@@ -4684,7 +4680,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>151</v>
       </c>
@@ -4728,7 +4724,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>158</v>
       </c>
@@ -4772,7 +4768,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>161</v>
       </c>
@@ -4816,7 +4812,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>167</v>
       </c>
@@ -4857,7 +4853,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>171</v>
       </c>
@@ -4901,7 +4897,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>173</v>
       </c>
@@ -4945,7 +4941,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>175</v>
       </c>
@@ -4989,7 +4985,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>178</v>
       </c>
@@ -5030,7 +5026,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>184</v>
       </c>
@@ -5074,7 +5070,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>186</v>
       </c>
@@ -5115,7 +5111,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>189</v>
       </c>
@@ -5159,7 +5155,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>192</v>
       </c>
@@ -5203,7 +5199,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>195</v>
       </c>
@@ -5244,7 +5240,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>201</v>
       </c>
@@ -5288,7 +5284,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>206</v>
       </c>
@@ -5329,7 +5325,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>213</v>
       </c>
@@ -5370,7 +5366,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>218</v>
       </c>
@@ -5414,7 +5410,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>223</v>
       </c>
@@ -5452,7 +5448,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>228</v>
       </c>
@@ -5493,7 +5489,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>234</v>
       </c>
@@ -5534,7 +5530,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>241</v>
       </c>
@@ -5578,7 +5574,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>246</v>
       </c>
@@ -5616,7 +5612,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>249</v>
       </c>
@@ -5660,7 +5656,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>251</v>
       </c>
@@ -5704,7 +5700,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>253</v>
       </c>
@@ -5748,7 +5744,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>259</v>
       </c>
@@ -5792,7 +5788,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>265</v>
       </c>
@@ -5833,7 +5829,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>267</v>
       </c>
@@ -5871,7 +5867,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>269</v>
       </c>
@@ -5912,7 +5908,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>273</v>
       </c>
@@ -5953,7 +5949,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>274</v>
       </c>
@@ -5997,7 +5993,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>275</v>
       </c>
@@ -6038,7 +6034,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>278</v>
       </c>
@@ -6076,7 +6072,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>279</v>
       </c>
@@ -6117,7 +6113,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>280</v>
       </c>
@@ -6158,7 +6154,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>284</v>
       </c>
@@ -6202,7 +6198,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>285</v>
       </c>
@@ -6246,7 +6242,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>286</v>
       </c>
@@ -6287,7 +6283,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>288</v>
       </c>
@@ -6328,7 +6324,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>297</v>
       </c>
@@ -6369,7 +6365,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>298</v>
       </c>
@@ -6410,7 +6406,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>300</v>
       </c>
@@ -6451,7 +6447,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>303</v>
       </c>
@@ -6492,7 +6488,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>310</v>
       </c>
@@ -6533,7 +6529,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>312</v>
       </c>
@@ -6571,7 +6567,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>313</v>
       </c>
@@ -6612,7 +6608,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>316</v>
       </c>
@@ -6656,7 +6652,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>319</v>
       </c>
@@ -6694,7 +6690,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>321</v>
       </c>
@@ -6738,7 +6734,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>324</v>
       </c>
@@ -6782,7 +6778,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>327</v>
       </c>
@@ -6820,7 +6816,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>330</v>
       </c>
@@ -6861,7 +6857,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>331</v>
       </c>
@@ -6902,7 +6898,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>335</v>
       </c>
@@ -6943,7 +6939,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>337</v>
       </c>
@@ -6984,7 +6980,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>339</v>
       </c>
@@ -7025,7 +7021,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>340</v>
       </c>
@@ -7066,7 +7062,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>343</v>
       </c>
@@ -7107,7 +7103,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>344</v>
       </c>
@@ -7148,7 +7144,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>346</v>
       </c>
@@ -7192,7 +7188,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>348</v>
       </c>
@@ -7236,7 +7232,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>349</v>
       </c>
@@ -7277,7 +7273,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>350</v>
       </c>
@@ -7321,7 +7317,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>351</v>
       </c>
@@ -7359,7 +7355,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>358</v>
       </c>
@@ -7397,7 +7393,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>359</v>
       </c>
@@ -7438,7 +7434,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>360</v>
       </c>
@@ -7476,7 +7472,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>363</v>
       </c>
@@ -7520,7 +7516,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>366</v>
       </c>
@@ -7561,7 +7557,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>367</v>
       </c>
@@ -7605,7 +7601,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>369</v>
       </c>
@@ -7646,7 +7642,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>370</v>
       </c>
@@ -7684,7 +7680,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>371</v>
       </c>
@@ -7722,7 +7718,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>373</v>
       </c>
@@ -7763,7 +7759,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>376</v>
       </c>
@@ -7804,7 +7800,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>377</v>
       </c>
@@ -7845,7 +7841,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>382</v>
       </c>
@@ -7886,7 +7882,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>384</v>
       </c>
@@ -7927,7 +7923,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>385</v>
       </c>
@@ -7971,7 +7967,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>390</v>
       </c>
@@ -8009,7 +8005,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>392</v>
       </c>
@@ -8047,7 +8043,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>394</v>
       </c>
@@ -8082,7 +8078,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>395</v>
       </c>
@@ -8123,7 +8119,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>396</v>
       </c>
@@ -8164,7 +8160,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>400</v>
       </c>
@@ -8202,7 +8198,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>404</v>
       </c>
@@ -8240,7 +8236,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>411</v>
       </c>
@@ -8281,7 +8277,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>416</v>
       </c>
@@ -8319,7 +8315,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>417</v>
       </c>
@@ -8357,7 +8353,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>423</v>
       </c>
@@ -8395,7 +8391,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>428</v>
       </c>
@@ -8436,7 +8432,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>431</v>
       </c>
@@ -8477,7 +8473,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>434</v>
       </c>
@@ -8521,7 +8517,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>442</v>
       </c>
@@ -8562,7 +8558,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>443</v>
       </c>
@@ -8603,7 +8599,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>444</v>
       </c>
@@ -8644,7 +8640,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>446</v>
       </c>
@@ -8685,7 +8681,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>456</v>
       </c>
@@ -8726,7 +8722,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>463</v>
       </c>
@@ -8767,7 +8763,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>465</v>
       </c>
@@ -8811,7 +8807,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>493</v>
       </c>
@@ -8846,7 +8842,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>497</v>
       </c>
@@ -8881,7 +8877,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>501</v>
       </c>
@@ -8916,7 +8912,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>517</v>
       </c>
@@ -8954,7 +8950,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>519</v>
       </c>
@@ -8989,7 +8985,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>534</v>
       </c>
@@ -9024,7 +9020,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>537</v>
       </c>
@@ -9059,7 +9055,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>547</v>
       </c>
@@ -9094,7 +9090,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>548</v>
       </c>
@@ -9129,7 +9125,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>555</v>
       </c>
@@ -9167,7 +9163,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>563</v>
       </c>
@@ -9202,7 +9198,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>564</v>
       </c>
@@ -9237,7 +9233,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>582</v>
       </c>
@@ -9278,7 +9274,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>584</v>
       </c>
@@ -9319,7 +9315,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>587</v>
       </c>
@@ -9354,7 +9350,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>589</v>
       </c>
@@ -9389,7 +9385,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>590</v>
       </c>
@@ -9427,7 +9423,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>591</v>
       </c>
@@ -9468,7 +9464,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>611</v>
       </c>
@@ -9509,7 +9505,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>613</v>
       </c>
@@ -9553,7 +9549,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>615</v>
       </c>
@@ -9594,7 +9590,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>619</v>
       </c>
@@ -9635,7 +9631,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>627</v>
       </c>
@@ -9676,7 +9672,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>629</v>
       </c>
@@ -9717,7 +9713,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>636</v>
       </c>
@@ -9761,7 +9757,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>640</v>
       </c>
@@ -9805,7 +9801,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>645</v>
       </c>
@@ -9846,7 +9842,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>647</v>
       </c>
@@ -9887,7 +9883,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>650</v>
       </c>
@@ -9928,7 +9924,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>651</v>
       </c>
@@ -9972,7 +9968,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>656</v>
       </c>
@@ -10013,7 +10009,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>658</v>
       </c>
@@ -10057,7 +10053,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>659</v>
       </c>
@@ -10101,7 +10097,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>660</v>
       </c>
@@ -10142,7 +10138,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>661</v>
       </c>
@@ -10186,7 +10182,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>662</v>
       </c>
@@ -10227,7 +10223,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>663</v>
       </c>
@@ -10265,7 +10261,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>669</v>
       </c>
@@ -10306,7 +10302,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>670</v>
       </c>
@@ -10347,7 +10343,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>672</v>
       </c>
@@ -10385,7 +10381,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>674</v>
       </c>
@@ -10426,7 +10422,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>677</v>
       </c>
@@ -10467,7 +10463,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>682</v>
       </c>
@@ -10508,7 +10504,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>684</v>
       </c>
@@ -10549,7 +10545,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>686</v>
       </c>
@@ -10590,7 +10586,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>688</v>
       </c>
@@ -10634,7 +10630,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>690</v>
       </c>
@@ -10675,7 +10671,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>693</v>
       </c>
@@ -10716,7 +10712,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>697</v>
       </c>
@@ -10754,7 +10750,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>698</v>
       </c>
@@ -10795,7 +10791,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>699</v>
       </c>
@@ -10836,7 +10832,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>702</v>
       </c>
@@ -10877,7 +10873,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>705</v>
       </c>
@@ -10918,7 +10914,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>706</v>
       </c>
@@ -10959,7 +10955,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>707</v>
       </c>
@@ -11000,7 +10996,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>708</v>
       </c>
@@ -11041,7 +11037,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>710</v>
       </c>
@@ -11082,7 +11078,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>717</v>
       </c>
@@ -11123,7 +11119,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>720</v>
       </c>
@@ -11164,7 +11160,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>721</v>
       </c>
@@ -11205,7 +11201,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>722</v>
       </c>
@@ -11246,7 +11242,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>724</v>
       </c>
@@ -11287,7 +11283,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>726</v>
       </c>
@@ -11328,7 +11324,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>728</v>
       </c>
@@ -11369,7 +11365,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>730</v>
       </c>
@@ -11410,7 +11406,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>735</v>
       </c>
@@ -11451,7 +11447,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>741</v>
       </c>
@@ -11492,7 +11488,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>742</v>
       </c>
@@ -11533,7 +11529,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>746</v>
       </c>
@@ -11574,7 +11570,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>764</v>
       </c>
@@ -11615,7 +11611,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>765</v>
       </c>
@@ -11656,7 +11652,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>773</v>
       </c>
@@ -11697,7 +11693,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>782</v>
       </c>
@@ -11741,7 +11737,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>785</v>
       </c>
@@ -11785,7 +11781,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>789</v>
       </c>
@@ -11826,7 +11822,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>793</v>
       </c>
@@ -11867,7 +11863,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>797</v>
       </c>
@@ -11908,7 +11904,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>800</v>
       </c>
@@ -11946,7 +11942,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>803</v>
       </c>
@@ -11987,7 +11983,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>807</v>
       </c>
@@ -12028,7 +12024,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>810</v>
       </c>
@@ -12069,7 +12065,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>813</v>
       </c>
@@ -12110,7 +12106,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>814</v>
       </c>
@@ -12151,7 +12147,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>818</v>
       </c>
@@ -12192,7 +12188,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>819</v>
       </c>
@@ -12233,7 +12229,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>825</v>
       </c>
@@ -12274,7 +12270,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>829</v>
       </c>
@@ -12315,7 +12311,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>838</v>
       </c>
@@ -12356,7 +12352,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>842</v>
       </c>
@@ -12397,7 +12393,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>845</v>
       </c>
@@ -12438,7 +12434,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>849</v>
       </c>
@@ -12479,7 +12475,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>853</v>
       </c>
@@ -12523,7 +12519,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>861</v>
       </c>
@@ -12567,7 +12563,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>864</v>
       </c>
@@ -12608,7 +12604,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>871</v>
       </c>
@@ -12649,7 +12645,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>887</v>
       </c>
@@ -12690,7 +12686,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>898</v>
       </c>
@@ -12731,7 +12727,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>901</v>
       </c>
@@ -12772,7 +12768,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>914</v>
       </c>
@@ -12810,7 +12806,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>933</v>
       </c>
@@ -12851,7 +12847,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>935</v>
       </c>
@@ -12892,7 +12888,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>938</v>
       </c>
@@ -12933,7 +12929,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>943</v>
       </c>
@@ -12974,7 +12970,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>948</v>
       </c>
@@ -13015,7 +13011,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>961</v>
       </c>
@@ -13056,7 +13052,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>980</v>
       </c>
@@ -13097,7 +13093,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>983</v>
       </c>
@@ -13138,7 +13134,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>984</v>
       </c>
@@ -13179,7 +13175,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>995</v>
       </c>
@@ -13220,7 +13216,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>1001</v>
       </c>
@@ -13261,7 +13257,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>1006</v>
       </c>
@@ -13299,7 +13295,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>1019</v>
       </c>
@@ -13340,7 +13336,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>1025</v>
       </c>
@@ -13381,7 +13377,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>1037</v>
       </c>
@@ -13422,7 +13418,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>1094</v>
       </c>
@@ -13463,7 +13459,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>1101</v>
       </c>
@@ -13504,7 +13500,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>1103</v>
       </c>
@@ -13545,7 +13541,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>1104</v>
       </c>
@@ -13586,7 +13582,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>1116</v>
       </c>
@@ -13627,7 +13623,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>1119</v>
       </c>
@@ -13668,7 +13664,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>1123</v>
       </c>
@@ -13709,7 +13705,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>1131</v>
       </c>
@@ -13750,7 +13746,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>1137</v>
       </c>
@@ -13791,7 +13787,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>1145</v>
       </c>
@@ -13832,7 +13828,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>1149</v>
       </c>
@@ -13873,7 +13869,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>1153</v>
       </c>
@@ -13914,7 +13910,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>1159</v>
       </c>
@@ -13955,7 +13951,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>1162</v>
       </c>
@@ -13996,7 +13992,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>1171</v>
       </c>
@@ -14037,7 +14033,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>1195</v>
       </c>
@@ -14078,7 +14074,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>1208</v>
       </c>
@@ -14119,7 +14115,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>1210</v>
       </c>
@@ -14160,7 +14156,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>1214</v>
       </c>
@@ -14201,7 +14197,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>1215</v>
       </c>
@@ -14242,7 +14238,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>1231</v>
       </c>
@@ -14283,7 +14279,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>1238</v>
       </c>
@@ -14324,7 +14320,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>1249</v>
       </c>
@@ -14365,7 +14361,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>1250</v>
       </c>
@@ -14406,7 +14402,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>1261</v>
       </c>
@@ -14447,7 +14443,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>1262</v>
       </c>
@@ -14488,7 +14484,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>1274</v>
       </c>
@@ -14529,7 +14525,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>1282</v>
       </c>
@@ -14570,7 +14566,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>1290</v>
       </c>
@@ -14611,7 +14607,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>1300</v>
       </c>
@@ -14652,7 +14648,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>1313</v>
       </c>
@@ -14696,7 +14692,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>1317</v>
       </c>
@@ -14737,7 +14733,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>1321</v>
       </c>
@@ -14778,7 +14774,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>1330</v>
       </c>
@@ -14819,7 +14815,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>1355</v>
       </c>
@@ -14860,7 +14856,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>1360</v>
       </c>
@@ -14904,7 +14900,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>1374</v>
       </c>
@@ -14945,7 +14941,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>1389</v>
       </c>
@@ -14989,7 +14985,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>1394</v>
       </c>
@@ -15030,7 +15026,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>1398</v>
       </c>
@@ -15071,7 +15067,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>1411</v>
       </c>
@@ -15115,7 +15111,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>1424</v>
       </c>
@@ -15159,7 +15155,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>1430</v>
       </c>
@@ -15200,7 +15196,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>1434</v>
       </c>
@@ -15241,7 +15237,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>1444</v>
       </c>
@@ -15282,7 +15278,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>1450</v>
       </c>
@@ -15320,7 +15316,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>1451</v>
       </c>
@@ -15361,7 +15357,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>1453</v>
       </c>
@@ -15402,7 +15398,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>1457</v>
       </c>
@@ -15443,7 +15439,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>1463</v>
       </c>
@@ -15484,7 +15480,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>1466</v>
       </c>
@@ -15525,7 +15521,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>1469</v>
       </c>
@@ -15566,7 +15562,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>1474</v>
       </c>
@@ -15607,7 +15603,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>1500</v>
       </c>
@@ -15648,7 +15644,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>1509</v>
       </c>
@@ -15692,7 +15688,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>1520</v>
       </c>
@@ -15733,7 +15729,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>1529</v>
       </c>
@@ -15774,7 +15770,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>1536</v>
       </c>
@@ -15815,7 +15811,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>1543</v>
       </c>
@@ -15856,7 +15852,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>1553</v>
       </c>
@@ -15897,7 +15893,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>1557</v>
       </c>
@@ -15938,7 +15934,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>1573</v>
       </c>
@@ -15979,7 +15975,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>1592</v>
       </c>
@@ -16020,7 +16016,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>1601</v>
       </c>
@@ -16064,7 +16060,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>1604</v>
       </c>
@@ -16105,7 +16101,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>1612</v>
       </c>
@@ -16146,7 +16142,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>1613</v>
       </c>
@@ -16187,7 +16183,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>1614</v>
       </c>
@@ -16228,7 +16224,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>1617</v>
       </c>
@@ -16269,7 +16265,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>1622</v>
       </c>
@@ -16310,7 +16306,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>1625</v>
       </c>
@@ -16351,7 +16347,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>1627</v>
       </c>
@@ -16392,7 +16388,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>1635</v>
       </c>
@@ -16436,7 +16432,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>1639</v>
       </c>
@@ -16477,7 +16473,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>1644</v>
       </c>
@@ -16521,7 +16517,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>1656</v>
       </c>
@@ -16562,7 +16558,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>1664</v>
       </c>
@@ -16600,7 +16596,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>1669</v>
       </c>
@@ -16641,7 +16637,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>1677</v>
       </c>
@@ -16682,7 +16678,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>1678</v>
       </c>
@@ -16723,7 +16719,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>1681</v>
       </c>
@@ -16764,7 +16760,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>1689</v>
       </c>
@@ -16805,7 +16801,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>1692</v>
       </c>
@@ -16846,7 +16842,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>1696</v>
       </c>
@@ -16887,7 +16883,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>1701</v>
       </c>
@@ -16928,7 +16924,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>1705</v>
       </c>
@@ -16969,7 +16965,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>1711</v>
       </c>
@@ -17010,7 +17006,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>1715</v>
       </c>
@@ -17054,7 +17050,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>1720</v>
       </c>
@@ -17095,7 +17091,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>1725</v>
       </c>
@@ -17136,7 +17132,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>1733</v>
       </c>
@@ -17180,7 +17176,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>1744</v>
       </c>
@@ -17221,7 +17217,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>1753</v>
       </c>
@@ -17262,7 +17258,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>1756</v>
       </c>
@@ -17303,7 +17299,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>1769</v>
       </c>
@@ -17344,7 +17340,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>1775</v>
       </c>
@@ -17385,7 +17381,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>1779</v>
       </c>
@@ -17429,7 +17425,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>1790</v>
       </c>
@@ -17473,7 +17469,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>1800</v>
       </c>
@@ -17514,7 +17510,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>1810</v>
       </c>
@@ -17555,7 +17551,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>1812</v>
       </c>
@@ -17599,7 +17595,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>1818</v>
       </c>
@@ -17640,7 +17636,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>1826</v>
       </c>
@@ -17684,7 +17680,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>1831</v>
       </c>
@@ -17725,7 +17721,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>1838</v>
       </c>
@@ -17763,7 +17759,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>1846</v>
       </c>
@@ -17804,7 +17800,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>1850</v>
       </c>
@@ -17845,7 +17841,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>1852</v>
       </c>
@@ -17886,7 +17882,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>1868</v>
       </c>
@@ -17930,7 +17926,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>1876</v>
       </c>
@@ -17971,7 +17967,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>1877</v>
       </c>
@@ -18012,7 +18008,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>1878</v>
       </c>
@@ -18053,7 +18049,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>1880</v>
       </c>
@@ -18094,7 +18090,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>1887</v>
       </c>
@@ -18138,7 +18134,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>1890</v>
       </c>
@@ -18176,7 +18172,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>1893</v>
       </c>
@@ -18220,7 +18216,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>1894</v>
       </c>
@@ -18261,7 +18257,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>1899</v>
       </c>
@@ -18305,7 +18301,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>1915</v>
       </c>
@@ -18346,7 +18342,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>1928</v>
       </c>
@@ -18387,7 +18383,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>1933</v>
       </c>
@@ -18431,7 +18427,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>1960</v>
       </c>
@@ -18472,7 +18468,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>1966</v>
       </c>
@@ -18513,7 +18509,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>11000</v>
       </c>
@@ -18554,7 +18550,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>11050</v>
       </c>
@@ -18595,7 +18591,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>11100</v>
       </c>
@@ -18636,7 +18632,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>11150</v>
       </c>
@@ -18677,7 +18673,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>11180</v>
       </c>
@@ -18718,7 +18714,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>11200</v>
       </c>
@@ -18759,7 +18755,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>11248</v>
       </c>
@@ -18800,7 +18796,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>11250</v>
       </c>
@@ -18841,7 +18837,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>11252</v>
       </c>
@@ -18882,7 +18878,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>11300</v>
       </c>
@@ -18923,7 +18919,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>11350</v>
       </c>
@@ -18961,7 +18957,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>11400</v>
       </c>
@@ -19002,7 +18998,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>11450</v>
       </c>
@@ -19043,7 +19039,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>11500</v>
       </c>
@@ -19084,7 +19080,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>11550</v>
       </c>

</xml_diff>

<commit_message>
add flesh-footed shearwater photo
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337AABB2-1BEE-4D7B-8047-5BDEEB992A14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40515687-5FC2-4FC2-8DDE-D8FADE4260F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="932">
   <si>
     <t>species_order</t>
   </si>
@@ -2823,6 +2823,9 @@
   </si>
   <si>
     <t>Tahiti Petrel</t>
+  </si>
+  <si>
+    <t>https://farm8.staticflickr.com/7870/47401626722_bf183f6cc7_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -3178,7 +3181,7 @@
   <dimension ref="A1:N395"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A133" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9609,6 +9612,9 @@
       <c r="K156" t="s">
         <v>306</v>
       </c>
+      <c r="L156" t="s">
+        <v>931</v>
+      </c>
       <c r="M156" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
remove FFSW image link
https://farm8.staticflickr.com/7870/47401626722_bf183f6cc7_b_d.jpg
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40515687-5FC2-4FC2-8DDE-D8FADE4260F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37517813-0F90-440D-962E-E3F533791B59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3972" uniqueCount="931">
   <si>
     <t>species_order</t>
   </si>
@@ -2823,9 +2823,6 @@
   </si>
   <si>
     <t>Tahiti Petrel</t>
-  </si>
-  <si>
-    <t>https://farm8.staticflickr.com/7870/47401626722_bf183f6cc7_b_d.jpg</t>
   </si>
 </sst>
 </file>
@@ -3180,8 +3177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N395"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A158" sqref="A158"/>
+    <sheetView tabSelected="1" topLeftCell="C148" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L156" sqref="L156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9612,9 +9609,6 @@
       <c r="K156" t="s">
         <v>306</v>
       </c>
-      <c r="L156" t="s">
-        <v>931</v>
-      </c>
       <c r="M156" s="2" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
change d/e/g/h to numerical values
try #127
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467A178C-7BAE-4921-9147-AD3E89035708}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4F41CA-9E94-4F19-9EBD-1C23CE012A36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="951">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3971" uniqueCount="934">
   <si>
     <t>species_order</t>
   </si>
@@ -2807,36 +2807,6 @@
     <t>Tahiti Petrel</t>
   </si>
   <si>
-    <t>E11632</t>
-  </si>
-  <si>
-    <t>E11835</t>
-  </si>
-  <si>
-    <t>G11513</t>
-  </si>
-  <si>
-    <t>G00248</t>
-  </si>
-  <si>
-    <t>E00393</t>
-  </si>
-  <si>
-    <t>G01128</t>
-  </si>
-  <si>
-    <t>E00464</t>
-  </si>
-  <si>
-    <t>G00467</t>
-  </si>
-  <si>
-    <t>H00475</t>
-  </si>
-  <si>
-    <t>G00385</t>
-  </si>
-  <si>
     <t>Cockatiel (Domestic type)</t>
   </si>
   <si>
@@ -2852,31 +2822,10 @@
     <t>Muscovy Duck (Domestic type)</t>
   </si>
   <si>
-    <t>E11911</t>
-  </si>
-  <si>
-    <t>G01340</t>
-  </si>
-  <si>
     <t>Red Junglefowl (Domestic type)</t>
   </si>
   <si>
-    <t>E01424</t>
-  </si>
-  <si>
-    <t>E11639</t>
-  </si>
-  <si>
-    <t>G00852</t>
-  </si>
-  <si>
     <t>Helmeted Guineafowl (Domestic type)</t>
-  </si>
-  <si>
-    <t>D34120</t>
-  </si>
-  <si>
-    <t>D30075</t>
   </si>
   <si>
     <t>European Greenfinch</t>
@@ -3241,7 +3190,7 @@
   <dimension ref="A1:O395"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A365" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C378" sqref="C378"/>
+      <selection activeCell="B384" sqref="B384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3305,7 +3254,7 @@
         <v>873</v>
       </c>
       <c r="O1" t="s">
-        <v>950</v>
+        <v>933</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -19964,14 +19913,14 @@
       </c>
     </row>
     <row r="379" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A379" s="3" t="s">
-        <v>948</v>
+      <c r="A379" s="3">
+        <v>4030075</v>
       </c>
       <c r="B379" t="s">
         <v>808</v>
       </c>
       <c r="C379" t="s">
-        <v>949</v>
+        <v>932</v>
       </c>
       <c r="D379" t="s">
         <v>15</v>
@@ -20002,8 +19951,8 @@
       </c>
     </row>
     <row r="380" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A380" s="3" t="s">
-        <v>947</v>
+      <c r="A380" s="3">
+        <v>4034120</v>
       </c>
       <c r="B380" t="s">
         <v>794</v>
@@ -20046,8 +19995,8 @@
       </c>
     </row>
     <row r="381" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A381" s="3" t="s">
-        <v>929</v>
+      <c r="A381" s="3">
+        <v>5000393</v>
       </c>
       <c r="B381" t="s">
         <v>880</v>
@@ -20090,8 +20039,8 @@
       </c>
     </row>
     <row r="382" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A382" s="3" t="s">
-        <v>931</v>
+      <c r="A382" s="3">
+        <v>5000464</v>
       </c>
       <c r="B382" t="s">
         <v>881</v>
@@ -20134,8 +20083,8 @@
       </c>
     </row>
     <row r="383" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A383" s="3" t="s">
-        <v>943</v>
+      <c r="A383" s="3">
+        <v>5001424</v>
       </c>
       <c r="B383" t="s">
         <v>861</v>
@@ -20178,8 +20127,8 @@
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A384" s="3" t="s">
-        <v>925</v>
+      <c r="A384" s="3">
+        <v>5011632</v>
       </c>
       <c r="B384" t="s">
         <v>848</v>
@@ -20222,8 +20171,8 @@
       </c>
     </row>
     <row r="385" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A385" s="3" t="s">
-        <v>944</v>
+      <c r="A385" s="3">
+        <v>5011639</v>
       </c>
       <c r="B385" t="s">
         <v>863</v>
@@ -20266,8 +20215,8 @@
       </c>
     </row>
     <row r="386" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A386" s="3" t="s">
-        <v>926</v>
+      <c r="A386" s="3">
+        <v>5011835</v>
       </c>
       <c r="B386" t="s">
         <v>850</v>
@@ -20310,8 +20259,8 @@
       </c>
     </row>
     <row r="387" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A387" s="3" t="s">
-        <v>940</v>
+      <c r="A387" s="3">
+        <v>5011911</v>
       </c>
       <c r="B387" t="s">
         <v>858</v>
@@ -20351,14 +20300,14 @@
       </c>
     </row>
     <row r="388" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A388" s="3" t="s">
-        <v>928</v>
+      <c r="A388" s="3">
+        <v>7000248</v>
       </c>
       <c r="B388" t="s">
         <v>853</v>
       </c>
       <c r="C388" t="s">
-        <v>936</v>
+        <v>926</v>
       </c>
       <c r="D388" t="s">
         <v>15</v>
@@ -20395,14 +20344,14 @@
       </c>
     </row>
     <row r="389" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A389" s="3" t="s">
-        <v>934</v>
+      <c r="A389" s="3">
+        <v>7000385</v>
       </c>
       <c r="B389" t="s">
         <v>857</v>
       </c>
       <c r="C389" t="s">
-        <v>939</v>
+        <v>929</v>
       </c>
       <c r="D389" t="s">
         <v>15</v>
@@ -20439,14 +20388,14 @@
       </c>
     </row>
     <row r="390" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A390" s="3" t="s">
-        <v>932</v>
+      <c r="A390" s="3">
+        <v>7000467</v>
       </c>
       <c r="B390" t="s">
         <v>855</v>
       </c>
       <c r="C390" t="s">
-        <v>938</v>
+        <v>928</v>
       </c>
       <c r="D390" t="s">
         <v>15</v>
@@ -20483,14 +20432,14 @@
       </c>
     </row>
     <row r="391" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A391" s="3" t="s">
-        <v>945</v>
+      <c r="A391" s="3">
+        <v>7000852</v>
       </c>
       <c r="B391" t="s">
         <v>865</v>
       </c>
       <c r="C391" t="s">
-        <v>946</v>
+        <v>931</v>
       </c>
       <c r="D391" t="s">
         <v>15</v>
@@ -20527,14 +20476,14 @@
       </c>
     </row>
     <row r="392" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A392" s="3" t="s">
-        <v>930</v>
+      <c r="A392" s="3">
+        <v>7001128</v>
       </c>
       <c r="B392" t="s">
         <v>854</v>
       </c>
       <c r="C392" t="s">
-        <v>937</v>
+        <v>927</v>
       </c>
       <c r="D392" t="s">
         <v>15</v>
@@ -20571,14 +20520,14 @@
       </c>
     </row>
     <row r="393" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A393" s="3" t="s">
-        <v>941</v>
+      <c r="A393" s="3">
+        <v>7001340</v>
       </c>
       <c r="B393" t="s">
         <v>860</v>
       </c>
       <c r="C393" t="s">
-        <v>942</v>
+        <v>930</v>
       </c>
       <c r="D393" t="s">
         <v>15</v>
@@ -20615,14 +20564,14 @@
       </c>
     </row>
     <row r="394" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A394" s="3" t="s">
-        <v>927</v>
+      <c r="A394" s="3">
+        <v>7011513</v>
       </c>
       <c r="B394" t="s">
         <v>852</v>
       </c>
       <c r="C394" t="s">
-        <v>935</v>
+        <v>925</v>
       </c>
       <c r="D394" t="s">
         <v>15</v>
@@ -20659,8 +20608,8 @@
       </c>
     </row>
     <row r="395" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A395" s="3" t="s">
-        <v>933</v>
+      <c r="A395" s="3">
+        <v>8000475</v>
       </c>
       <c r="B395" t="s">
         <v>882</v>

</xml_diff>

<commit_message>
remove graphs for 2 species
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC32154-684B-4A15-8D4E-0F1753106374}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F7FCE-E314-470E-85BB-4AA968AB199B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4215" uniqueCount="984">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4213" uniqueCount="984">
   <si>
     <t>species_order</t>
   </si>
@@ -3343,7 +3343,7 @@
   <dimension ref="A1:O418"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A389" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C412" sqref="C411:C412"/>
+      <selection activeCell="G401" sqref="G401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -21004,9 +21004,6 @@
       <c r="F400" t="s">
         <v>17</v>
       </c>
-      <c r="G400" t="s">
-        <v>18</v>
-      </c>
       <c r="H400" t="s">
         <v>18</v>
       </c>
@@ -21091,9 +21088,6 @@
       </c>
       <c r="F402" t="s">
         <v>17</v>
-      </c>
-      <c r="G402" t="s">
-        <v>18</v>
       </c>
       <c r="H402" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
change marine only species graphs
#150
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05AEB87-7AE4-448B-B536-3703FA3D8C46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1008336-7E12-4592-9128-34BA756EE863}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atlas_list" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4179" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="979">
   <si>
     <t>species_order</t>
   </si>
@@ -2967,6 +2967,9 @@
   </si>
   <si>
     <t>https://live.staticflickr.com/7870/47401626722_bf183f6cc7_b_d.jpg</t>
+  </si>
+  <si>
+    <t>3_4_5_6</t>
   </si>
 </sst>
 </file>
@@ -3324,8 +3327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L158" sqref="L158"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G176" sqref="G176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8612,7 +8615,7 @@
         <v>17</v>
       </c>
       <c r="G118" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H118" t="s">
         <v>18</v>
@@ -8656,7 +8659,7 @@
         <v>17</v>
       </c>
       <c r="G119" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H119" t="s">
         <v>18</v>
@@ -8699,6 +8702,9 @@
       <c r="F120" t="s">
         <v>17</v>
       </c>
+      <c r="G120" t="s">
+        <v>978</v>
+      </c>
       <c r="H120" t="s">
         <v>18</v>
       </c>
@@ -8907,6 +8913,9 @@
       <c r="F125" t="s">
         <v>17</v>
       </c>
+      <c r="G125" t="s">
+        <v>978</v>
+      </c>
       <c r="H125" t="s">
         <v>18</v>
       </c>
@@ -8948,6 +8957,9 @@
       <c r="F126" t="s">
         <v>17</v>
       </c>
+      <c r="G126" t="s">
+        <v>978</v>
+      </c>
       <c r="H126" t="s">
         <v>18</v>
       </c>
@@ -8989,6 +9001,9 @@
       <c r="F127" t="s">
         <v>17</v>
       </c>
+      <c r="G127" t="s">
+        <v>978</v>
+      </c>
       <c r="H127" t="s">
         <v>18</v>
       </c>
@@ -9077,6 +9092,9 @@
       <c r="F129" t="s">
         <v>17</v>
       </c>
+      <c r="G129" t="s">
+        <v>18</v>
+      </c>
       <c r="H129" t="s">
         <v>18</v>
       </c>
@@ -9476,6 +9494,9 @@
       <c r="F138" t="s">
         <v>17</v>
       </c>
+      <c r="G138" t="s">
+        <v>978</v>
+      </c>
       <c r="H138" t="s">
         <v>18</v>
       </c>
@@ -9517,6 +9538,9 @@
       <c r="F139" t="s">
         <v>17</v>
       </c>
+      <c r="G139" t="s">
+        <v>978</v>
+      </c>
       <c r="H139" t="s">
         <v>18</v>
       </c>
@@ -9558,6 +9582,9 @@
       <c r="F140" t="s">
         <v>17</v>
       </c>
+      <c r="G140" t="s">
+        <v>978</v>
+      </c>
       <c r="H140" t="s">
         <v>18</v>
       </c>
@@ -9599,6 +9626,9 @@
       <c r="F141" t="s">
         <v>146</v>
       </c>
+      <c r="G141" t="s">
+        <v>978</v>
+      </c>
       <c r="H141" t="s">
         <v>18</v>
       </c>
@@ -9640,6 +9670,9 @@
       <c r="F142" t="s">
         <v>146</v>
       </c>
+      <c r="G142" t="s">
+        <v>978</v>
+      </c>
       <c r="H142" t="s">
         <v>18</v>
       </c>
@@ -9681,6 +9714,9 @@
       <c r="F143" t="s">
         <v>146</v>
       </c>
+      <c r="G143" t="s">
+        <v>978</v>
+      </c>
       <c r="H143" t="s">
         <v>18</v>
       </c>
@@ -9722,6 +9758,9 @@
       <c r="F144" t="s">
         <v>17</v>
       </c>
+      <c r="G144" t="s">
+        <v>978</v>
+      </c>
       <c r="H144" t="s">
         <v>18</v>
       </c>
@@ -9764,7 +9803,7 @@
         <v>17</v>
       </c>
       <c r="G145" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H145" t="s">
         <v>18</v>
@@ -9807,6 +9846,9 @@
       <c r="F146" t="s">
         <v>17</v>
       </c>
+      <c r="G146" t="s">
+        <v>978</v>
+      </c>
       <c r="H146" t="s">
         <v>18</v>
       </c>
@@ -9848,6 +9890,9 @@
       <c r="F147" t="s">
         <v>17</v>
       </c>
+      <c r="G147" t="s">
+        <v>978</v>
+      </c>
       <c r="H147" t="s">
         <v>18</v>
       </c>
@@ -9889,6 +9934,9 @@
       <c r="F148" t="s">
         <v>17</v>
       </c>
+      <c r="G148" t="s">
+        <v>978</v>
+      </c>
       <c r="H148" t="s">
         <v>18</v>
       </c>
@@ -9930,6 +9978,9 @@
       <c r="F149" t="s">
         <v>215</v>
       </c>
+      <c r="G149" t="s">
+        <v>978</v>
+      </c>
       <c r="H149" t="s">
         <v>18</v>
       </c>
@@ -9971,6 +10022,9 @@
       <c r="F150" t="s">
         <v>17</v>
       </c>
+      <c r="G150" t="s">
+        <v>978</v>
+      </c>
       <c r="H150" t="s">
         <v>18</v>
       </c>
@@ -10012,6 +10066,9 @@
       <c r="F151" t="s">
         <v>17</v>
       </c>
+      <c r="G151" t="s">
+        <v>978</v>
+      </c>
       <c r="H151" t="s">
         <v>18</v>
       </c>
@@ -10054,7 +10111,7 @@
         <v>17</v>
       </c>
       <c r="G152" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H152" t="s">
         <v>18</v>
@@ -10097,6 +10154,9 @@
       <c r="F153" t="s">
         <v>17</v>
       </c>
+      <c r="G153" t="s">
+        <v>978</v>
+      </c>
       <c r="H153" t="s">
         <v>18</v>
       </c>
@@ -10138,6 +10198,9 @@
       <c r="F154" t="s">
         <v>17</v>
       </c>
+      <c r="G154" t="s">
+        <v>978</v>
+      </c>
       <c r="H154" t="s">
         <v>18</v>
       </c>
@@ -10179,6 +10242,9 @@
       <c r="F155" t="s">
         <v>17</v>
       </c>
+      <c r="G155" t="s">
+        <v>978</v>
+      </c>
       <c r="H155" t="s">
         <v>18</v>
       </c>
@@ -10220,6 +10286,9 @@
       <c r="F156" t="s">
         <v>17</v>
       </c>
+      <c r="G156" t="s">
+        <v>978</v>
+      </c>
       <c r="H156" t="s">
         <v>18</v>
       </c>
@@ -10261,6 +10330,9 @@
       <c r="F157" t="s">
         <v>17</v>
       </c>
+      <c r="G157" t="s">
+        <v>978</v>
+      </c>
       <c r="H157" t="s">
         <v>18</v>
       </c>
@@ -10302,6 +10374,9 @@
       <c r="F158" t="s">
         <v>17</v>
       </c>
+      <c r="G158" t="s">
+        <v>978</v>
+      </c>
       <c r="H158" t="s">
         <v>18</v>
       </c>
@@ -10344,7 +10419,7 @@
         <v>17</v>
       </c>
       <c r="G159" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H159" t="s">
         <v>18</v>
@@ -10388,7 +10463,7 @@
         <v>17</v>
       </c>
       <c r="G160" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H160" t="s">
         <v>18</v>
@@ -10431,6 +10506,9 @@
       <c r="F161" t="s">
         <v>17</v>
       </c>
+      <c r="G161" t="s">
+        <v>978</v>
+      </c>
       <c r="H161" t="s">
         <v>18</v>
       </c>
@@ -10472,6 +10550,9 @@
       <c r="F162" t="s">
         <v>17</v>
       </c>
+      <c r="G162" t="s">
+        <v>978</v>
+      </c>
       <c r="H162" t="s">
         <v>18</v>
       </c>
@@ -10513,6 +10594,9 @@
       <c r="F163" t="s">
         <v>17</v>
       </c>
+      <c r="G163" t="s">
+        <v>978</v>
+      </c>
       <c r="H163" t="s">
         <v>18</v>
       </c>
@@ -10554,6 +10638,9 @@
       <c r="F164" t="s">
         <v>17</v>
       </c>
+      <c r="G164" t="s">
+        <v>978</v>
+      </c>
       <c r="H164" t="s">
         <v>18</v>
       </c>
@@ -10596,7 +10683,7 @@
         <v>146</v>
       </c>
       <c r="G165" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H165" t="s">
         <v>18</v>
@@ -10643,7 +10730,7 @@
         <v>17</v>
       </c>
       <c r="G166" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H166" t="s">
         <v>18</v>
@@ -10687,7 +10774,7 @@
         <v>17</v>
       </c>
       <c r="G167" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H167" t="s">
         <v>18</v>
@@ -10734,7 +10821,7 @@
         <v>17</v>
       </c>
       <c r="G168" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H168" t="s">
         <v>18</v>
@@ -10778,7 +10865,7 @@
         <v>17</v>
       </c>
       <c r="G169" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H169" t="s">
         <v>18</v>
@@ -10865,6 +10952,9 @@
       <c r="F171" t="s">
         <v>17</v>
       </c>
+      <c r="G171" t="s">
+        <v>978</v>
+      </c>
       <c r="H171" t="s">
         <v>18</v>
       </c>
@@ -10907,7 +10997,7 @@
         <v>17</v>
       </c>
       <c r="G172" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H172" t="s">
         <v>18</v>
@@ -10950,6 +11040,9 @@
       <c r="F173" t="s">
         <v>17</v>
       </c>
+      <c r="G173" t="s">
+        <v>978</v>
+      </c>
       <c r="H173" t="s">
         <v>18</v>
       </c>
@@ -10992,7 +11085,7 @@
         <v>17</v>
       </c>
       <c r="G174" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H174" t="s">
         <v>18</v>
@@ -11036,7 +11129,7 @@
         <v>17</v>
       </c>
       <c r="G175" t="s">
-        <v>18</v>
+        <v>978</v>
       </c>
       <c r="H175" t="s">
         <v>18</v>
@@ -21640,7 +21733,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O411">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O411">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
bunch of aesthetic edits
change book cover - now fancy, vectorized
- update references, add source files for cover
minor edits to icons
add some links to species
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5BC74-97A9-4D9B-8C88-A119E61B874E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA9599-01AD-44EB-ADAE-CAF953E977D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="178" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5169" uniqueCount="1506">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5192" uniqueCount="1529">
   <si>
     <t>species_order</t>
   </si>
@@ -4552,6 +4552,75 @@
   </si>
   <si>
     <t>22698453/132647873</t>
+  </si>
+  <si>
+    <t>22679843/131907524</t>
+  </si>
+  <si>
+    <t>22680029/92839434</t>
+  </si>
+  <si>
+    <t>22680090/92842427</t>
+  </si>
+  <si>
+    <t>7176-Chenonetta-jubata</t>
+  </si>
+  <si>
+    <t>22680111/92844188</t>
+  </si>
+  <si>
+    <t>22680243/92852551</t>
+  </si>
+  <si>
+    <t>22680217/92849931</t>
+  </si>
+  <si>
+    <t>22680271/92853108</t>
+  </si>
+  <si>
+    <t>22680277/92853345</t>
+  </si>
+  <si>
+    <t>22680336/92856515</t>
+  </si>
+  <si>
+    <t>22680387/112385790</t>
+  </si>
+  <si>
+    <t>22679830/92831295</t>
+  </si>
+  <si>
+    <t>22678551/131902671</t>
+  </si>
+  <si>
+    <t>22678965/92796647</t>
+  </si>
+  <si>
+    <t>22678979/92797212</t>
+  </si>
+  <si>
+    <t>22678952/92795607</t>
+  </si>
+  <si>
+    <t>22696553/93570492</t>
+  </si>
+  <si>
+    <t>22696589/93572515</t>
+  </si>
+  <si>
+    <t>22696602/154250080</t>
+  </si>
+  <si>
+    <t>22690066/155493121</t>
+  </si>
+  <si>
+    <t>22690215/93265605</t>
+  </si>
+  <si>
+    <t>60482887/95160992</t>
+  </si>
+  <si>
+    <t>22690571/93277985</t>
   </si>
 </sst>
 </file>
@@ -4911,10 +4980,10 @@
   <dimension ref="A1:AF421"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T150" sqref="T150"/>
+      <selection pane="bottomRight" activeCell="T28" sqref="T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5530,9 +5599,8 @@
         <f t="shared" si="1"/>
         <v>Cygnus%20atratus</v>
       </c>
-      <c r="T6" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T6" t="s">
+        <v>1506</v>
       </c>
       <c r="U6" t="str">
         <f t="shared" si="2"/>
@@ -5562,9 +5630,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Cygnus%20atratus</v>
       </c>
-      <c r="AC6" t="e">
+      <c r="AC6" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22679843/131907524</v>
       </c>
       <c r="AD6" t="str">
         <f t="shared" si="9"/>
@@ -5635,9 +5703,8 @@
         <f t="shared" si="1"/>
         <v>Radjah%20radjah</v>
       </c>
-      <c r="T7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T7" t="s">
+        <v>1507</v>
       </c>
       <c r="U7" t="str">
         <f t="shared" si="2"/>
@@ -5667,9 +5734,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Radjah%20radjah</v>
       </c>
-      <c r="AC7" t="e">
+      <c r="AC7" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680029/92839434</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="9"/>
@@ -5743,9 +5810,8 @@
         <f t="shared" si="1"/>
         <v>Nettapus%20coromandelianus</v>
       </c>
-      <c r="T8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T8" t="s">
+        <v>1508</v>
       </c>
       <c r="U8" t="str">
         <f t="shared" si="2"/>
@@ -5775,9 +5841,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Nettapus%20coromandelianus</v>
       </c>
-      <c r="AC8" t="e">
+      <c r="AC8" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680090/92842427</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="9"/>
@@ -5842,15 +5908,14 @@
         <v>1000</v>
       </c>
       <c r="R9" t="s">
-        <v>1453</v>
+        <v>1509</v>
       </c>
       <c r="S9" t="str">
         <f t="shared" si="1"/>
         <v>Chenonetta%20jubata</v>
       </c>
-      <c r="T9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T9" t="s">
+        <v>1510</v>
       </c>
       <c r="U9" t="str">
         <f t="shared" si="2"/>
@@ -5873,16 +5938,16 @@
         <v>https://beta.birdsoftheworld.org/bow/species/manduc1</v>
       </c>
       <c r="AA9" t="str">
-        <f t="shared" si="6"/>
+        <f>"https://www.inaturalist.org/taxa/"&amp;R396</f>
         <v>https://www.inaturalist.org/taxa/7106-Aix-galericulata</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Chenonetta%20jubata</v>
       </c>
-      <c r="AC9" t="e">
+      <c r="AC9" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680111/92844188</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="9"/>
@@ -5956,9 +6021,8 @@
         <f t="shared" si="1"/>
         <v>Spatula%20rhynchotis</v>
       </c>
-      <c r="T10" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T10" t="s">
+        <v>1511</v>
       </c>
       <c r="U10" t="str">
         <f t="shared" si="2"/>
@@ -5988,9 +6052,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Spatula%20rhynchotis</v>
       </c>
-      <c r="AC10" t="e">
+      <c r="AC10" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680243/92852551</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="9"/>
@@ -6064,9 +6128,8 @@
         <f t="shared" si="1"/>
         <v>Anas%20superciliosa</v>
       </c>
-      <c r="T11" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T11" t="s">
+        <v>1512</v>
       </c>
       <c r="U11" t="str">
         <f t="shared" si="2"/>
@@ -6096,9 +6159,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Anas%20superciliosa</v>
       </c>
-      <c r="AC11" t="e">
+      <c r="AC11" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680217/92849931</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="9"/>
@@ -6172,9 +6235,8 @@
         <f t="shared" si="1"/>
         <v>Anas%20gracilis</v>
       </c>
-      <c r="T12" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T12" t="s">
+        <v>1513</v>
       </c>
       <c r="U12" t="str">
         <f t="shared" si="2"/>
@@ -6204,9 +6266,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Anas%20gracilis</v>
       </c>
-      <c r="AC12" t="e">
+      <c r="AC12" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680271/92853108</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="9"/>
@@ -6277,9 +6339,8 @@
         <f t="shared" si="1"/>
         <v>Anas%20castanea</v>
       </c>
-      <c r="T13" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T13" t="s">
+        <v>1514</v>
       </c>
       <c r="U13" t="str">
         <f t="shared" si="2"/>
@@ -6309,9 +6370,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Anas%20castanea</v>
       </c>
-      <c r="AC13" t="e">
+      <c r="AC13" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680277/92853345</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="9"/>
@@ -6382,9 +6443,8 @@
         <f t="shared" si="1"/>
         <v>Malacorhynchus%20membranaceus</v>
       </c>
-      <c r="T14" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T14" t="s">
+        <v>1515</v>
       </c>
       <c r="U14" t="str">
         <f t="shared" si="2"/>
@@ -6414,9 +6474,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Malacorhynchus%20membranaceus</v>
       </c>
-      <c r="AC14" t="e">
+      <c r="AC14" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680336/92856515</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="9"/>
@@ -6490,9 +6550,8 @@
         <f t="shared" si="1"/>
         <v>Aythya%20australis</v>
       </c>
-      <c r="T15" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T15" t="s">
+        <v>1516</v>
       </c>
       <c r="U15" t="str">
         <f t="shared" si="2"/>
@@ -6522,9 +6581,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Aythya%20australis</v>
       </c>
-      <c r="AC15" t="e">
+      <c r="AC15" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22680387/112385790</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="9"/>
@@ -6595,9 +6654,8 @@
         <f t="shared" si="1"/>
         <v>Biziura%20lobata</v>
       </c>
-      <c r="T16" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T16" t="s">
+        <v>1517</v>
       </c>
       <c r="U16" t="str">
         <f t="shared" si="2"/>
@@ -6627,9 +6685,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Biziura%20lobata</v>
       </c>
-      <c r="AC16" t="e">
+      <c r="AC16" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22679830/92831295</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="9"/>
@@ -6703,9 +6761,8 @@
         <f t="shared" si="1"/>
         <v>Alectura%20lathami</v>
       </c>
-      <c r="T17" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T17" t="s">
+        <v>1518</v>
       </c>
       <c r="U17" t="str">
         <f t="shared" si="2"/>
@@ -6735,9 +6792,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Alectura%20lathami</v>
       </c>
-      <c r="AC17" t="e">
+      <c r="AC17" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22678551/131902671</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" si="9"/>
@@ -6811,9 +6868,8 @@
         <f t="shared" si="1"/>
         <v>Synoicus%20ypsilophorus</v>
       </c>
-      <c r="T18" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T18" t="s">
+        <v>1519</v>
       </c>
       <c r="U18" t="str">
         <f t="shared" si="2"/>
@@ -6843,9 +6899,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Synoicus%20ypsilophorus</v>
       </c>
-      <c r="AC18" t="e">
+      <c r="AC18" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22678965/92796647</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="9"/>
@@ -6916,9 +6972,8 @@
         <f t="shared" si="1"/>
         <v>Synoicus%20chinensis</v>
       </c>
-      <c r="T19" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T19" t="s">
+        <v>1520</v>
       </c>
       <c r="U19" t="str">
         <f t="shared" si="2"/>
@@ -6948,9 +7003,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Synoicus%20chinensis</v>
       </c>
-      <c r="AC19" t="e">
+      <c r="AC19" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22678979/92797212</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="9"/>
@@ -7018,9 +7073,8 @@
         <f t="shared" si="1"/>
         <v>Coturnix%20pectoralis</v>
       </c>
-      <c r="T20" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T20" t="s">
+        <v>1521</v>
       </c>
       <c r="U20" t="str">
         <f t="shared" si="2"/>
@@ -7050,9 +7104,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Coturnix%20pectoralis</v>
       </c>
-      <c r="AC20" t="e">
+      <c r="AC20" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22678952/92795607</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="9"/>
@@ -7126,9 +7180,8 @@
         <f t="shared" si="1"/>
         <v>Tachybaptus%20novaehollandiae</v>
       </c>
-      <c r="T21" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T21" t="s">
+        <v>1522</v>
       </c>
       <c r="U21" t="str">
         <f t="shared" si="2"/>
@@ -7158,9 +7211,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Tachybaptus%20novaehollandiae</v>
       </c>
-      <c r="AC21" t="e">
+      <c r="AC21" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22696553/93570492</v>
       </c>
       <c r="AD21" t="str">
         <f t="shared" si="9"/>
@@ -7231,9 +7284,8 @@
         <f t="shared" si="1"/>
         <v>Poliocephalus%20poliocephalus</v>
       </c>
-      <c r="T22" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T22" t="s">
+        <v>1523</v>
       </c>
       <c r="U22" t="str">
         <f t="shared" si="2"/>
@@ -7263,9 +7315,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Poliocephalus%20poliocephalus</v>
       </c>
-      <c r="AC22" t="e">
+      <c r="AC22" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22696589/93572515</v>
       </c>
       <c r="AD22" t="str">
         <f t="shared" si="9"/>
@@ -7336,9 +7388,8 @@
         <f t="shared" si="1"/>
         <v>Podiceps%20cristatus</v>
       </c>
-      <c r="T23" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T23" t="s">
+        <v>1524</v>
       </c>
       <c r="U23" t="str">
         <f t="shared" si="2"/>
@@ -7368,9 +7419,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Podiceps%20cristatus</v>
       </c>
-      <c r="AC23" t="e">
+      <c r="AC23" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22696602/154250080</v>
       </c>
       <c r="AD23" t="str">
         <f t="shared" si="9"/>
@@ -7441,9 +7492,8 @@
         <f t="shared" si="1"/>
         <v>Columba%20livia</v>
       </c>
-      <c r="T24" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T24" t="s">
+        <v>1525</v>
       </c>
       <c r="U24" t="str">
         <f t="shared" si="2"/>
@@ -7473,9 +7523,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Columba%20livia</v>
       </c>
-      <c r="AC24" t="e">
+      <c r="AC24" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690066/155493121</v>
       </c>
       <c r="AD24" t="str">
         <f t="shared" si="9"/>
@@ -7549,9 +7599,8 @@
         <f t="shared" si="1"/>
         <v>Columba%20leucomela</v>
       </c>
-      <c r="T25" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T25" t="s">
+        <v>1526</v>
       </c>
       <c r="U25" t="str">
         <f t="shared" si="2"/>
@@ -7581,9 +7630,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Columba%20leucomela</v>
       </c>
-      <c r="AC25" t="e">
+      <c r="AC25" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690215/93265605</v>
       </c>
       <c r="AD25" t="str">
         <f t="shared" si="9"/>
@@ -7658,9 +7707,8 @@
         <f t="shared" si="1"/>
         <v>Streptopelia%20chinensis</v>
       </c>
-      <c r="T26" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T26" t="s">
+        <v>1527</v>
       </c>
       <c r="U26" t="str">
         <f t="shared" si="2"/>
@@ -7690,9 +7738,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Streptopelia%20chinensis</v>
       </c>
-      <c r="AC26" t="e">
+      <c r="AC26" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/60482887/95160992</v>
       </c>
       <c r="AD26" t="str">
         <f t="shared" si="9"/>
@@ -7767,9 +7815,8 @@
         <f t="shared" si="1"/>
         <v>Macropygia%20phasianella</v>
       </c>
-      <c r="T27" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T27" t="s">
+        <v>1528</v>
       </c>
       <c r="U27" t="str">
         <f t="shared" si="2"/>
@@ -7799,9 +7846,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Macropygia%20phasianella</v>
       </c>
-      <c r="AC27" t="e">
+      <c r="AC27" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690571/93277985</v>
       </c>
       <c r="AD27" t="str">
         <f t="shared" si="9"/>
@@ -46887,9 +46934,8 @@
       <c r="Q396" t="s">
         <v>1387</v>
       </c>
-      <c r="R396" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="R396" t="s">
+        <v>1453</v>
       </c>
       <c r="S396" t="str">
         <f t="shared" si="73"/>
@@ -46919,8 +46965,8 @@
         <v>https://beta.birdsoftheworld.org/bow/species/manduc</v>
       </c>
       <c r="AA396" t="e">
-        <f t="shared" si="78"/>
-        <v>#N/A</v>
+        <f>"https://www.inaturalist.org/taxa/"&amp;#REF!</f>
+        <v>#REF!</v>
       </c>
       <c r="AB396" t="str">
         <f t="shared" si="79"/>

</xml_diff>

<commit_message>
add curlew sandpiper draft
also fix typo in hardhead and add more species links
</commit_message>
<xml_diff>
--- a/data/species/atlas_list.xlsx
+++ b/data/species/atlas_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Documents\GitHub\brisbane-bird-atlas\data\species\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA9599-01AD-44EB-ADAE-CAF953E977D8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F86B55-7DE7-4035-B0B9-88AA21EB68B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="178" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5192" uniqueCount="1529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5213" uniqueCount="1550">
   <si>
     <t>species_order</t>
   </si>
@@ -4621,6 +4621,69 @@
   </si>
   <si>
     <t>22690571/93277985</t>
+  </si>
+  <si>
+    <t>22725548/94895730</t>
+  </si>
+  <si>
+    <t>22690667/93282812</t>
+  </si>
+  <si>
+    <t>22690676/93283379</t>
+  </si>
+  <si>
+    <t>22690727/93285451</t>
+  </si>
+  <si>
+    <t>22690705/93284384</t>
+  </si>
+  <si>
+    <t>22690719/93285055</t>
+  </si>
+  <si>
+    <t>22690724/93285257</t>
+  </si>
+  <si>
+    <t>22689580/93237832</t>
+  </si>
+  <si>
+    <t>22736125/95125102</t>
+  </si>
+  <si>
+    <t>22725660/112390311</t>
+  </si>
+  <si>
+    <t>22689555/93236849</t>
+  </si>
+  <si>
+    <t>22686677/155548867</t>
+  </si>
+  <si>
+    <t>22686534/93116529</t>
+  </si>
+  <si>
+    <t>22686845/155438660</t>
+  </si>
+  <si>
+    <t>22692521/93357101</t>
+  </si>
+  <si>
+    <t>22692425/93353232</t>
+  </si>
+  <si>
+    <t>22692893/93373735</t>
+  </si>
+  <si>
+    <t>22692680/93363806</t>
+  </si>
+  <si>
+    <t>22692880/93372762</t>
+  </si>
+  <si>
+    <t>22692913/154269531</t>
+  </si>
+  <si>
+    <t>22692792/155531172</t>
   </si>
 </sst>
 </file>
@@ -4980,10 +5043,10 @@
   <dimension ref="A1:AF421"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T28" sqref="T28"/>
+      <selection pane="bottomRight" activeCell="T64" sqref="T64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7923,9 +7986,8 @@
         <f t="shared" si="1"/>
         <v>Chalcophaps%20longirostris</v>
       </c>
-      <c r="T28" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T28" t="s">
+        <v>1529</v>
       </c>
       <c r="U28" t="str">
         <f t="shared" si="2"/>
@@ -7955,9 +8017,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Chalcophaps%20longirostris</v>
       </c>
-      <c r="AC28" t="e">
+      <c r="AC28" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22725548/94895730</v>
       </c>
       <c r="AD28" t="str">
         <f t="shared" si="9"/>
@@ -8032,9 +8094,8 @@
         <f t="shared" si="1"/>
         <v>Phaps%20chalcoptera</v>
       </c>
-      <c r="T29" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T29" t="s">
+        <v>1530</v>
       </c>
       <c r="U29" t="str">
         <f t="shared" si="2"/>
@@ -8064,9 +8125,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Phaps%20chalcoptera</v>
       </c>
-      <c r="AC29" t="e">
+      <c r="AC29" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690667/93282812</v>
       </c>
       <c r="AD29" t="str">
         <f t="shared" si="9"/>
@@ -8141,9 +8202,8 @@
         <f t="shared" si="1"/>
         <v>Ocyphaps%20lophotes</v>
       </c>
-      <c r="T30" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T30" t="s">
+        <v>1531</v>
       </c>
       <c r="U30" t="str">
         <f t="shared" si="2"/>
@@ -8173,9 +8233,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Ocyphaps%20lophotes</v>
       </c>
-      <c r="AC30" t="e">
+      <c r="AC30" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690676/93283379</v>
       </c>
       <c r="AD30" t="str">
         <f t="shared" si="9"/>
@@ -8247,9 +8307,8 @@
         <f t="shared" si="1"/>
         <v>Leucosarcia%20melanoleuca</v>
       </c>
-      <c r="T31" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T31" t="s">
+        <v>1532</v>
       </c>
       <c r="U31" t="str">
         <f t="shared" si="2"/>
@@ -8279,9 +8338,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Leucosarcia%20melanoleuca</v>
       </c>
-      <c r="AC31" t="e">
+      <c r="AC31" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690727/93285451</v>
       </c>
       <c r="AD31" t="str">
         <f t="shared" si="9"/>
@@ -8353,9 +8412,8 @@
         <f t="shared" si="1"/>
         <v>Geopelia%20cuneata</v>
       </c>
-      <c r="T32" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T32" t="s">
+        <v>1533</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="2"/>
@@ -8385,9 +8443,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Geopelia%20cuneata</v>
       </c>
-      <c r="AC32" t="e">
+      <c r="AC32" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690705/93284384</v>
       </c>
       <c r="AD32" t="str">
         <f t="shared" si="9"/>
@@ -8462,9 +8520,8 @@
         <f t="shared" si="1"/>
         <v>Geopelia%20placida</v>
       </c>
-      <c r="T33" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T33" t="s">
+        <v>1534</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="2"/>
@@ -8494,9 +8551,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Geopelia%20placida</v>
       </c>
-      <c r="AC33" t="e">
+      <c r="AC33" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690719/93285055</v>
       </c>
       <c r="AD33" t="str">
         <f t="shared" si="9"/>
@@ -8571,9 +8628,8 @@
         <f t="shared" si="1"/>
         <v>Geopelia%20humeralis</v>
       </c>
-      <c r="T34" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T34" t="s">
+        <v>1535</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="2"/>
@@ -8603,9 +8659,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Geopelia%20humeralis</v>
       </c>
-      <c r="AC34" t="e">
+      <c r="AC34" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22690724/93285257</v>
       </c>
       <c r="AD34" t="str">
         <f t="shared" si="9"/>
@@ -10276,9 +10332,8 @@
         <f t="shared" si="1"/>
         <v>Podargus%20strigoides</v>
       </c>
-      <c r="T50" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T50" t="s">
+        <v>1536</v>
       </c>
       <c r="U50" t="str">
         <f t="shared" si="2"/>
@@ -10308,9 +10363,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Podargus%20strigoides</v>
       </c>
-      <c r="AC50" t="e">
+      <c r="AC50" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22689580/93237832</v>
       </c>
       <c r="AD50" t="str">
         <f t="shared" si="9"/>
@@ -10382,9 +10437,8 @@
         <f t="shared" si="1"/>
         <v>Podargus%20ocellatus</v>
       </c>
-      <c r="T51" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T51" t="s">
+        <v>1537</v>
       </c>
       <c r="U51" t="str">
         <f t="shared" si="2"/>
@@ -10414,9 +10468,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Podargus%20ocellatus</v>
       </c>
-      <c r="AC51" t="e">
+      <c r="AC51" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22736125/95125102</v>
       </c>
       <c r="AD51" t="str">
         <f t="shared" si="9"/>
@@ -10488,9 +10542,8 @@
         <f t="shared" si="1"/>
         <v>Eurostopodus%20mystacalis</v>
       </c>
-      <c r="T52" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T52" t="s">
+        <v>1538</v>
       </c>
       <c r="U52" t="str">
         <f t="shared" si="2"/>
@@ -10520,9 +10573,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Eurostopodus%20mystacalis</v>
       </c>
-      <c r="AC52" t="e">
+      <c r="AC52" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22725660/112390311</v>
       </c>
       <c r="AD52" t="str">
         <f t="shared" si="9"/>
@@ -10594,9 +10647,8 @@
         <f t="shared" si="1"/>
         <v>Aegotheles%20cristatus</v>
       </c>
-      <c r="T53" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T53" t="s">
+        <v>1539</v>
       </c>
       <c r="U53" t="str">
         <f t="shared" si="2"/>
@@ -10626,9 +10678,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Aegotheles%20cristatus</v>
       </c>
-      <c r="AC53" t="e">
+      <c r="AC53" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22689555/93236849</v>
       </c>
       <c r="AD53" t="str">
         <f t="shared" si="9"/>
@@ -10703,9 +10755,8 @@
         <f t="shared" si="1"/>
         <v>Hirundapus%20caudacutus</v>
       </c>
-      <c r="T54" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T54" t="s">
+        <v>1540</v>
       </c>
       <c r="U54" t="str">
         <f t="shared" si="2"/>
@@ -10735,9 +10786,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Hirundapus%20caudacutus</v>
       </c>
-      <c r="AC54" t="e">
+      <c r="AC54" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22686677/155548867</v>
       </c>
       <c r="AD54" t="str">
         <f t="shared" si="9"/>
@@ -10806,9 +10857,8 @@
         <f t="shared" si="1"/>
         <v>Aerodramus%20terraereginae</v>
       </c>
-      <c r="T55" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T55" t="s">
+        <v>1541</v>
       </c>
       <c r="U55" t="str">
         <f t="shared" si="2"/>
@@ -10838,9 +10888,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Aerodramus%20terraereginae</v>
       </c>
-      <c r="AC55" t="e">
+      <c r="AC55" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22686534/93116529</v>
       </c>
       <c r="AD55" t="str">
         <f t="shared" si="9"/>
@@ -10912,9 +10962,8 @@
         <f t="shared" si="1"/>
         <v>Apus%20pacificus</v>
       </c>
-      <c r="T56" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T56" t="s">
+        <v>1542</v>
       </c>
       <c r="U56" t="str">
         <f t="shared" si="2"/>
@@ -10944,9 +10993,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Apus%20pacificus</v>
       </c>
-      <c r="AC56" t="e">
+      <c r="AC56" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22686845/155438660</v>
       </c>
       <c r="AD56" t="str">
         <f t="shared" si="9"/>
@@ -11018,9 +11067,8 @@
         <f t="shared" si="1"/>
         <v>Lewinia%20pectoralis</v>
       </c>
-      <c r="T57" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T57" t="s">
+        <v>1543</v>
       </c>
       <c r="U57" t="str">
         <f t="shared" si="2"/>
@@ -11050,9 +11098,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Lewinia%20pectoralis</v>
       </c>
-      <c r="AC57" t="e">
+      <c r="AC57" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692521/93357101</v>
       </c>
       <c r="AD57" t="str">
         <f t="shared" si="9"/>
@@ -11127,9 +11175,8 @@
         <f t="shared" si="1"/>
         <v>Gallirallus%20philippensis</v>
       </c>
-      <c r="T58" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T58" t="s">
+        <v>1544</v>
       </c>
       <c r="U58" t="str">
         <f t="shared" si="2"/>
@@ -11159,9 +11206,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Gallirallus%20philippensis</v>
       </c>
-      <c r="AC58" t="e">
+      <c r="AC58" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692425/93353232</v>
       </c>
       <c r="AD58" t="str">
         <f t="shared" si="9"/>
@@ -11230,9 +11277,8 @@
         <f t="shared" si="1"/>
         <v>Tribonyx%20ventralis</v>
       </c>
-      <c r="T59" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T59" t="s">
+        <v>1545</v>
       </c>
       <c r="U59" t="str">
         <f t="shared" si="2"/>
@@ -11262,9 +11308,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Tribonyx%20ventralis</v>
       </c>
-      <c r="AC59" t="e">
+      <c r="AC59" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692893/93373735</v>
       </c>
       <c r="AD59" t="str">
         <f t="shared" si="9"/>
@@ -11333,9 +11379,8 @@
         <f t="shared" si="1"/>
         <v>Porzana%20fluminea</v>
       </c>
-      <c r="T60" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T60" t="s">
+        <v>1546</v>
       </c>
       <c r="U60" t="str">
         <f t="shared" si="2"/>
@@ -11365,9 +11410,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Porzana%20fluminea</v>
       </c>
-      <c r="AC60" t="e">
+      <c r="AC60" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692680/93363806</v>
       </c>
       <c r="AD60" t="str">
         <f t="shared" si="9"/>
@@ -11439,9 +11484,8 @@
         <f t="shared" si="1"/>
         <v>Gallinula%20tenebrosa</v>
       </c>
-      <c r="T61" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T61" t="s">
+        <v>1547</v>
       </c>
       <c r="U61" t="str">
         <f t="shared" si="2"/>
@@ -11471,9 +11515,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Gallinula%20tenebrosa</v>
       </c>
-      <c r="AC61" t="e">
+      <c r="AC61" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692880/93372762</v>
       </c>
       <c r="AD61" t="str">
         <f t="shared" si="9"/>
@@ -11545,9 +11589,8 @@
         <f t="shared" si="1"/>
         <v>Fulica%20atra</v>
       </c>
-      <c r="T62" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T62" t="s">
+        <v>1548</v>
       </c>
       <c r="U62" t="str">
         <f t="shared" si="2"/>
@@ -11577,9 +11620,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Fulica%20atra</v>
       </c>
-      <c r="AC62" t="e">
+      <c r="AC62" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692913/154269531</v>
       </c>
       <c r="AD62" t="str">
         <f t="shared" si="9"/>
@@ -11654,9 +11697,8 @@
         <f t="shared" si="1"/>
         <v>Porphyrio%20melanotus</v>
       </c>
-      <c r="T63" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="T63" t="s">
+        <v>1549</v>
       </c>
       <c r="U63" t="str">
         <f t="shared" si="2"/>
@@ -11686,9 +11728,9 @@
         <f t="shared" si="7"/>
         <v>https://bie.ala.org.au/species/Porphyrio%20melanotus</v>
       </c>
-      <c r="AC63" t="e">
+      <c r="AC63" t="str">
         <f t="shared" si="8"/>
-        <v>#N/A</v>
+        <v>https://www.iucnredlist.org/species/22692792/155531172</v>
       </c>
       <c r="AD63" t="str">
         <f t="shared" si="9"/>

</xml_diff>